<commit_message>
Removed duplicate mapScripts, Fixed missing strings
Also added some more stuff to weapon spreadsheat
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BD1FD1-89FF-4728-B18E-41CF807106C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F46B88-B071-4F6E-9A4C-7C5A156B708D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -43,8 +43,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -581,6 +603,48 @@
   </si>
   <si>
     <t>Needs a nerf imo, should not out compete all AP pistol rounds and some rifle rounds -wethan2</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <t>Serbu</t>
+  </si>
+  <si>
+    <t>Remington 870</t>
+  </si>
+  <si>
+    <t>[8]</t>
+  </si>
+  <si>
+    <t>NL &amp; Slug ammo</t>
+  </si>
+  <si>
+    <t>Spas-12</t>
+  </si>
+  <si>
+    <t>KS-23</t>
+  </si>
+  <si>
+    <t>[3]</t>
+  </si>
+  <si>
+    <t>Origin 12</t>
+  </si>
+  <si>
+    <t>[8,20,30]</t>
+  </si>
+  <si>
+    <t>NL &amp; Slug ammo (8rnd only)</t>
+  </si>
+  <si>
+    <t>AA-12</t>
+  </si>
+  <si>
+    <t>USAS 12</t>
+  </si>
+  <si>
+    <t>Saiga 12</t>
   </si>
 </sst>
 </file>
@@ -1581,7 +1645,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4954,10 +5018,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E308052D-1B88-4699-843E-12AA607B59B8}">
-  <dimension ref="A1:AA30"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7125,13 +7189,82 @@
       <c r="A27" t="s">
         <v>149</v>
       </c>
-      <c r="X27" t="e">
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27">
+        <v>17500</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>125</v>
+      </c>
+      <c r="I27">
+        <v>50</v>
+      </c>
+      <c r="J27">
+        <v>35</v>
+      </c>
+      <c r="K27">
+        <v>55</v>
+      </c>
+      <c r="L27">
+        <v>55</v>
+      </c>
+      <c r="M27">
+        <v>60</v>
+      </c>
+      <c r="N27">
+        <v>40</v>
+      </c>
+      <c r="O27">
+        <v>22</v>
+      </c>
+      <c r="P27">
+        <v>32</v>
+      </c>
+      <c r="Q27">
+        <v>10</v>
+      </c>
+      <c r="R27">
+        <v>200</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>3</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>5</v>
+      </c>
+      <c r="W27" t="s">
+        <v>122</v>
+      </c>
+      <c r="X27">
         <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W27,Caliber!B11:'Caliber'!B21,0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y27" t="e">
+        <v>37</v>
+      </c>
+      <c r="Y27">
         <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W27,Caliber!B11:'Caliber'!B21,0),2)</f>
-        <v>#N/A</v>
+        <v>0.4</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
@@ -7161,6 +7294,206 @@
       </c>
       <c r="Y30" t="e">
         <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W30,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X31" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W31,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y31" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W31,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X32" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W32,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y32" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W32,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X33" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W33,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y33" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W33,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X34" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W34,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y34" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W34,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X35" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W35,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y35" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W35,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X36" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W36,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y36" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W36,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X37" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W37,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y37" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W37,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X38" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W38,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y38" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W38,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X39" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W39,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y39" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W39,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X40" t="e">
+        <f>INDEX(Caliber!B11:'Caliber'!C21,MATCH(W40,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y40" t="e">
+        <f>INDEX(Caliber!C11:'Caliber'!D21,MATCH(W40,Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X41" t="e" cm="1">
+        <f t="array" aca="1" ref="X41" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y41" t="e" cm="1">
+        <f t="array" aca="1" ref="Y41" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X42" t="e" cm="1">
+        <f t="array" aca="1" ref="X42" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y42" t="e" cm="1">
+        <f t="array" aca="1" ref="Y42" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X43" t="e" cm="1">
+        <f t="array" aca="1" ref="X43" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y43" t="e" cm="1">
+        <f t="array" aca="1" ref="Y43" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X44" t="e" cm="1">
+        <f t="array" aca="1" ref="X44" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y44" t="e" cm="1">
+        <f t="array" aca="1" ref="Y44" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X45" t="e" cm="1">
+        <f t="array" aca="1" ref="X45" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y45" t="e" cm="1">
+        <f t="array" aca="1" ref="Y45" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X46" t="e" cm="1">
+        <f t="array" aca="1" ref="X46" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y46" t="e" cm="1">
+        <f t="array" aca="1" ref="Y46" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X47" t="e" cm="1">
+        <f t="array" aca="1" ref="X47" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y47" t="e" cm="1">
+        <f t="array" aca="1" ref="Y47" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X48" t="e" cm="1">
+        <f t="array" aca="1" ref="X48" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y48" t="e" cm="1">
+        <f t="array" aca="1" ref="Y48" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X49" t="e" cm="1">
+        <f t="array" aca="1" ref="X49" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y49" t="e" cm="1">
+        <f t="array" aca="1" ref="Y49" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="50" spans="24:25" x14ac:dyDescent="0.25">
+      <c r="X50" t="e" cm="1">
+        <f t="array" aca="1" ref="X50" ca="1">INDEX(Caliber!B11:'Caliber'!C21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y50" t="e" cm="1">
+        <f t="array" aca="1" ref="Y50" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -7173,7 +7506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52ABDA0-E560-473A-9AD2-E06CBFB7AB92}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M10" sqref="M10"/>
     </sheetView>
@@ -8455,32 +8788,35 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CF758D-66BB-49AA-8233-CCB9E398E093}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
     <col min="16" max="16" width="10.140625" customWidth="1"/>
     <col min="17" max="17" width="10" customWidth="1"/>
     <col min="18" max="18" width="9.5703125" customWidth="1"/>
     <col min="19" max="19" width="11.85546875" customWidth="1"/>
-    <col min="20" max="20" width="10" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" customWidth="1"/>
+    <col min="22" max="22" width="10" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" customWidth="1"/>
     <col min="24" max="24" width="11.5703125" customWidth="1"/>
-    <col min="25" max="25" width="9.42578125" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
+    <col min="28" max="28" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -8554,21 +8890,811 @@
         <v>2</v>
       </c>
       <c r="Y1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>171</v>
       </c>
       <c r="B2">
         <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+      <c r="G2">
+        <v>115</v>
+      </c>
+      <c r="H2">
+        <v>90</v>
+      </c>
+      <c r="I2">
+        <v>65</v>
+      </c>
+      <c r="J2">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2">
+        <v>80</v>
+      </c>
+      <c r="M2">
+        <v>40</v>
+      </c>
+      <c r="N2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O2">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2">
+        <v>30</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>77</v>
+      </c>
+      <c r="W2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W2,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y2">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W2,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>10</v>
+      </c>
+      <c r="Z2">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W2,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3">
+        <v>30000</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>80</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>80</v>
+      </c>
+      <c r="I3">
+        <v>60</v>
+      </c>
+      <c r="J3">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3">
+        <v>75</v>
+      </c>
+      <c r="M3">
+        <v>45</v>
+      </c>
+      <c r="N3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3">
+        <v>12</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3">
+        <v>30</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W3,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y3">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W3,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>10</v>
+      </c>
+      <c r="Z3">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W3,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4">
+        <v>21000</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>115</v>
+      </c>
+      <c r="H4">
+        <v>85</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4">
+        <v>95</v>
+      </c>
+      <c r="M4">
+        <v>50</v>
+      </c>
+      <c r="N4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O4">
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <v>7</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4">
+        <v>30</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
+        <v>77</v>
+      </c>
+      <c r="W4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W4,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y4">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W4,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>10</v>
+      </c>
+      <c r="Z4">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W4,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5">
+        <v>28000</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>115</v>
+      </c>
+      <c r="H5">
+        <v>85</v>
+      </c>
+      <c r="I5">
+        <v>55</v>
+      </c>
+      <c r="J5">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5">
+        <v>110</v>
+      </c>
+      <c r="M5">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5">
+        <v>18</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R5">
+        <v>30</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5" t="s">
+        <v>77</v>
+      </c>
+      <c r="W5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W5,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y5">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W5,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>10</v>
+      </c>
+      <c r="Z5">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W5,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6">
+        <v>30000</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>35</v>
+      </c>
+      <c r="G6">
+        <v>115</v>
+      </c>
+      <c r="H6">
+        <v>95</v>
+      </c>
+      <c r="I6">
+        <v>55</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="M6">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6">
+        <v>20</v>
+      </c>
+      <c r="P6">
+        <v>10</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6">
+        <v>30</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6" t="s">
+        <v>77</v>
+      </c>
+      <c r="W6" t="s">
+        <v>38</v>
+      </c>
+      <c r="X6">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W6,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y6">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W6,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>20</v>
+      </c>
+      <c r="Z6">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W6,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7">
+        <v>51000</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>35</v>
+      </c>
+      <c r="G7">
+        <v>115</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7">
+        <v>40</v>
+      </c>
+      <c r="J7">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7">
+        <v>80</v>
+      </c>
+      <c r="M7">
+        <v>50</v>
+      </c>
+      <c r="N7" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7">
+        <v>15</v>
+      </c>
+      <c r="P7">
+        <v>7</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>77</v>
+      </c>
+      <c r="R7">
+        <v>30</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>77</v>
+      </c>
+      <c r="W7" t="s">
+        <v>34</v>
+      </c>
+      <c r="X7">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W7,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y7">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W7,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>10</v>
+      </c>
+      <c r="Z7">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W7,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8">
+        <v>40000</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <v>115</v>
+      </c>
+      <c r="H8">
+        <v>85</v>
+      </c>
+      <c r="I8">
+        <v>40</v>
+      </c>
+      <c r="J8">
+        <v>75</v>
+      </c>
+      <c r="K8">
+        <v>50</v>
+      </c>
+      <c r="L8">
+        <v>80</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+      <c r="N8">
+        <v>65</v>
+      </c>
+      <c r="O8">
+        <v>12</v>
+      </c>
+      <c r="P8">
+        <v>18</v>
+      </c>
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>30</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X8">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W8,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y8">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W8,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>10</v>
+      </c>
+      <c r="Z8">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W8,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9">
+        <v>32000</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>35</v>
+      </c>
+      <c r="G9">
+        <v>115</v>
+      </c>
+      <c r="H9">
+        <v>90</v>
+      </c>
+      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="J9">
+        <v>65</v>
+      </c>
+      <c r="K9">
+        <v>50</v>
+      </c>
+      <c r="L9">
+        <v>60</v>
+      </c>
+      <c r="M9">
+        <v>80</v>
+      </c>
+      <c r="N9">
+        <v>50</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+      <c r="P9">
+        <v>14</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9">
+        <v>30</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>3</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W9,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y9">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W9,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>10</v>
+      </c>
+      <c r="Z9">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W9,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10">
+        <v>43000</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>35</v>
+      </c>
+      <c r="G10">
+        <v>115</v>
+      </c>
+      <c r="H10">
+        <v>85</v>
+      </c>
+      <c r="I10">
+        <v>25</v>
+      </c>
+      <c r="J10">
+        <v>65</v>
+      </c>
+      <c r="K10">
+        <v>45</v>
+      </c>
+      <c r="L10">
+        <v>70</v>
+      </c>
+      <c r="M10">
+        <v>90</v>
+      </c>
+      <c r="N10">
+        <v>35</v>
+      </c>
+      <c r="O10">
+        <v>9</v>
+      </c>
+      <c r="P10">
+        <v>13</v>
+      </c>
+      <c r="Q10">
+        <v>6</v>
+      </c>
+      <c r="R10">
+        <v>30</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>3</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>5</v>
+      </c>
+      <c r="W10" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10">
+        <f>INDEX(Caliber!B23:'Caliber'!C28,MATCH(W10,Caliber!B23:'Caliber'!B28,0),2)</f>
+        <v>25</v>
+      </c>
+      <c r="Y10">
+        <f>INDEX(Caliber!B23:'Caliber'!D28,MATCH(W10,Caliber!B23:'Caliber'!B28,0),3)</f>
+        <v>10</v>
+      </c>
+      <c r="Z10">
+        <f>INDEX(Caliber!B23:'Caliber'!F28,MATCH(W10,Caliber!B23:'Caliber'!B28,0),5)</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Skorpion Evo, C4, Medkit
Also increased reserved space for assets, and forced instant nades to be off
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E90313E-E85F-4DE7-854C-F1A872336B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B113A2-9D4F-48F3-888E-540CB10D1B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="455">
   <si>
     <t>Name</t>
   </si>
@@ -1543,6 +1543,12 @@
   </si>
   <si>
     <t>G36C</t>
+  </si>
+  <si>
+    <t>Skorpion Evo</t>
+  </si>
+  <si>
+    <t>[30,40]</t>
   </si>
 </sst>
 </file>
@@ -2022,24 +2028,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2066,6 +2054,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7475,10 +7481,10 @@
       <c r="D26" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E26" s="63"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="66"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="75"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="61"/>
@@ -7487,10 +7493,10 @@
       <c r="D27" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="67"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="76"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="61"/>
@@ -7499,10 +7505,10 @@
       <c r="D28" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="68"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="77"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="61"/>
@@ -7515,11 +7521,11 @@
       <c r="D29" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E29" s="69" t="s">
+      <c r="E29" s="63" t="s">
         <v>381</v>
       </c>
-      <c r="F29" s="70"/>
-      <c r="G29" s="71"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="65"/>
       <c r="H29" s="60" t="s">
         <v>351</v>
       </c>
@@ -7531,11 +7537,11 @@
       <c r="D30" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E30" s="72" t="s">
+      <c r="E30" s="66" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="73"/>
-      <c r="G30" s="74"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
       <c r="H30" s="61"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7545,11 +7551,11 @@
       <c r="D31" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E31" s="75" t="s">
+      <c r="E31" s="69" t="s">
         <v>382</v>
       </c>
-      <c r="F31" s="76"/>
-      <c r="G31" s="77"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
       <c r="H31" s="62"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7563,11 +7569,11 @@
       <c r="D32" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E32" s="69" t="s">
+      <c r="E32" s="63" t="s">
         <v>383</v>
       </c>
-      <c r="F32" s="70"/>
-      <c r="G32" s="71"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="65"/>
       <c r="H32" s="60" t="s">
         <v>351</v>
       </c>
@@ -7579,11 +7585,11 @@
       <c r="D33" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E33" s="72" t="s">
+      <c r="E33" s="66" t="s">
         <v>384</v>
       </c>
-      <c r="F33" s="73"/>
-      <c r="G33" s="74"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="68"/>
       <c r="H33" s="61"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7593,11 +7599,11 @@
       <c r="D34" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E34" s="75" t="s">
+      <c r="E34" s="69" t="s">
         <v>385</v>
       </c>
-      <c r="F34" s="76"/>
-      <c r="G34" s="77"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
       <c r="H34" s="62"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7611,11 +7617,11 @@
       <c r="D35" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E35" s="69" t="s">
+      <c r="E35" s="63" t="s">
         <v>381</v>
       </c>
-      <c r="F35" s="70"/>
-      <c r="G35" s="71"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="65"/>
       <c r="H35" s="60" t="s">
         <v>351</v>
       </c>
@@ -7627,11 +7633,11 @@
       <c r="D36" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E36" s="72" t="s">
+      <c r="E36" s="66" t="s">
         <v>145</v>
       </c>
-      <c r="F36" s="73"/>
-      <c r="G36" s="74"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="68"/>
       <c r="H36" s="61"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7641,11 +7647,11 @@
       <c r="D37" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E37" s="75" t="s">
+      <c r="E37" s="69" t="s">
         <v>382</v>
       </c>
-      <c r="F37" s="76"/>
-      <c r="G37" s="77"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="71"/>
       <c r="H37" s="62"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7659,11 +7665,11 @@
       <c r="D38" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E38" s="69" t="s">
+      <c r="E38" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="F38" s="70"/>
-      <c r="G38" s="71"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="65"/>
       <c r="H38" s="60" t="s">
         <v>386</v>
       </c>
@@ -7675,11 +7681,11 @@
       <c r="D39" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E39" s="72" t="s">
+      <c r="E39" s="66" t="s">
         <v>185</v>
       </c>
-      <c r="F39" s="73"/>
-      <c r="G39" s="74"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="68"/>
       <c r="H39" s="61"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7689,11 +7695,11 @@
       <c r="D40" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E40" s="75" t="s">
+      <c r="E40" s="69" t="s">
         <v>185</v>
       </c>
-      <c r="F40" s="76"/>
-      <c r="G40" s="77"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="71"/>
       <c r="H40" s="62"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7707,11 +7713,11 @@
       <c r="D41" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E41" s="69" t="s">
+      <c r="E41" s="63" t="s">
         <v>349</v>
       </c>
-      <c r="F41" s="70"/>
-      <c r="G41" s="71"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="65"/>
       <c r="H41" s="60" t="s">
         <v>351</v>
       </c>
@@ -7723,11 +7729,11 @@
       <c r="D42" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E42" s="72" t="s">
+      <c r="E42" s="66" t="s">
         <v>387</v>
       </c>
-      <c r="F42" s="73"/>
-      <c r="G42" s="74"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="68"/>
       <c r="H42" s="61"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7737,11 +7743,11 @@
       <c r="D43" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E43" s="75" t="s">
+      <c r="E43" s="69" t="s">
         <v>388</v>
       </c>
-      <c r="F43" s="76"/>
-      <c r="G43" s="77"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="71"/>
       <c r="H43" s="62"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7755,11 +7761,11 @@
       <c r="D44" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E44" s="69" t="s">
+      <c r="E44" s="63" t="s">
         <v>389</v>
       </c>
-      <c r="F44" s="70"/>
-      <c r="G44" s="71"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="65"/>
       <c r="H44" s="60" t="s">
         <v>351</v>
       </c>
@@ -7771,11 +7777,11 @@
       <c r="D45" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E45" s="72" t="s">
+      <c r="E45" s="66" t="s">
         <v>390</v>
       </c>
-      <c r="F45" s="73"/>
-      <c r="G45" s="74"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="68"/>
       <c r="H45" s="61"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7785,11 +7791,11 @@
       <c r="D46" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E46" s="75" t="s">
+      <c r="E46" s="69" t="s">
         <v>390</v>
       </c>
-      <c r="F46" s="76"/>
-      <c r="G46" s="77"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="71"/>
       <c r="H46" s="62"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7803,11 +7809,11 @@
       <c r="D47" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E47" s="69" t="s">
+      <c r="E47" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="F47" s="70"/>
-      <c r="G47" s="71"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="65"/>
       <c r="H47" s="60" t="s">
         <v>351</v>
       </c>
@@ -7819,11 +7825,11 @@
       <c r="D48" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E48" s="72" t="s">
+      <c r="E48" s="66" t="s">
         <v>391</v>
       </c>
-      <c r="F48" s="73"/>
-      <c r="G48" s="74"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="68"/>
       <c r="H48" s="61"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7833,54 +7839,24 @@
       <c r="D49" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E49" s="75" t="s">
+      <c r="E49" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="F49" s="76"/>
-      <c r="G49" s="77"/>
+      <c r="F49" s="70"/>
+      <c r="G49" s="71"/>
       <c r="H49" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -7897,6 +7873,12 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="E32:G32"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="H20:H22"/>
@@ -7907,15 +7889,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9561,11 +9567,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V8" sqref="V8"/>
+      <selection pane="topRight" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
@@ -10461,13 +10468,82 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="W12" s="10" t="e">
+      <c r="A12" t="s">
+        <v>453</v>
+      </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>25000</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>80</v>
+      </c>
+      <c r="G12">
+        <v>115</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>15</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>30</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
+      </c>
+      <c r="M12">
+        <v>30</v>
+      </c>
+      <c r="N12">
+        <v>8</v>
+      </c>
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="Q12">
+        <v>20</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>10</v>
+      </c>
+      <c r="V12" t="s">
+        <v>12</v>
+      </c>
+      <c r="W12" s="10">
         <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V12,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X12" s="10" t="e">
+        <v>31</v>
+      </c>
+      <c r="X12" s="10">
         <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V12,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>#N/A</v>
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
M16 Scoped & M203
Scoped m16 and scoped m203
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B113A2-9D4F-48F3-888E-540CB10D1B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77401913-F93C-4B02-9F2D-5393A9A38812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="458">
   <si>
     <t>Name</t>
   </si>
@@ -1549,6 +1549,15 @@
   </si>
   <si>
     <t>[30,40]</t>
+  </si>
+  <si>
+    <t>M16A2 (Scoped)</t>
+  </si>
+  <si>
+    <t>M16A2 (M203)</t>
+  </si>
+  <si>
+    <t>Aimed</t>
   </si>
 </sst>
 </file>
@@ -2028,6 +2037,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2054,24 +2081,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2823,8 +2832,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8241084F-89A0-47CD-965A-F8C6F1FCBC05}" name="Table2" displayName="Table2" ref="A1:AA48" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A1:AA48" xr:uid="{8241084F-89A0-47CD-965A-F8C6F1FCBC05}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8241084F-89A0-47CD-965A-F8C6F1FCBC05}" name="Table2" displayName="Table2" ref="A1:AA50" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:AA50" xr:uid="{8241084F-89A0-47CD-965A-F8C6F1FCBC05}"/>
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{EA086EA1-B04D-408A-83CB-62AACD4983EB}" name="Name"/>
     <tableColumn id="2" xr3:uid="{28FB994B-34C3-478E-82FB-47025B753042}" name="weight"/>
@@ -3230,7 +3239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -7481,10 +7490,10 @@
       <c r="D26" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E26" s="72"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="75"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="66"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="61"/>
@@ -7493,10 +7502,10 @@
       <c r="D27" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E27" s="72"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="76"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="67"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="61"/>
@@ -7505,10 +7514,10 @@
       <c r="D28" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E28" s="72"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="77"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="68"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="61"/>
@@ -7521,11 +7530,11 @@
       <c r="D29" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E29" s="63" t="s">
+      <c r="E29" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="F29" s="64"/>
-      <c r="G29" s="65"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
       <c r="H29" s="60" t="s">
         <v>351</v>
       </c>
@@ -7537,11 +7546,11 @@
       <c r="D30" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E30" s="66" t="s">
+      <c r="E30" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="67"/>
-      <c r="G30" s="68"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="74"/>
       <c r="H30" s="61"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7551,11 +7560,11 @@
       <c r="D31" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E31" s="69" t="s">
+      <c r="E31" s="75" t="s">
         <v>382</v>
       </c>
-      <c r="F31" s="70"/>
-      <c r="G31" s="71"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="77"/>
       <c r="H31" s="62"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7569,11 +7578,11 @@
       <c r="D32" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E32" s="63" t="s">
+      <c r="E32" s="69" t="s">
         <v>383</v>
       </c>
-      <c r="F32" s="64"/>
-      <c r="G32" s="65"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="71"/>
       <c r="H32" s="60" t="s">
         <v>351</v>
       </c>
@@ -7585,11 +7594,11 @@
       <c r="D33" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E33" s="66" t="s">
+      <c r="E33" s="72" t="s">
         <v>384</v>
       </c>
-      <c r="F33" s="67"/>
-      <c r="G33" s="68"/>
+      <c r="F33" s="73"/>
+      <c r="G33" s="74"/>
       <c r="H33" s="61"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7599,11 +7608,11 @@
       <c r="D34" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E34" s="69" t="s">
+      <c r="E34" s="75" t="s">
         <v>385</v>
       </c>
-      <c r="F34" s="70"/>
-      <c r="G34" s="71"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="77"/>
       <c r="H34" s="62"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7617,11 +7626,11 @@
       <c r="D35" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E35" s="63" t="s">
+      <c r="E35" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="F35" s="64"/>
-      <c r="G35" s="65"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
       <c r="H35" s="60" t="s">
         <v>351</v>
       </c>
@@ -7633,11 +7642,11 @@
       <c r="D36" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E36" s="66" t="s">
+      <c r="E36" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="F36" s="67"/>
-      <c r="G36" s="68"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="74"/>
       <c r="H36" s="61"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7647,11 +7656,11 @@
       <c r="D37" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E37" s="69" t="s">
+      <c r="E37" s="75" t="s">
         <v>382</v>
       </c>
-      <c r="F37" s="70"/>
-      <c r="G37" s="71"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="77"/>
       <c r="H37" s="62"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7665,11 +7674,11 @@
       <c r="D38" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E38" s="63" t="s">
+      <c r="E38" s="69" t="s">
         <v>183</v>
       </c>
-      <c r="F38" s="64"/>
-      <c r="G38" s="65"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="71"/>
       <c r="H38" s="60" t="s">
         <v>386</v>
       </c>
@@ -7681,11 +7690,11 @@
       <c r="D39" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E39" s="66" t="s">
+      <c r="E39" s="72" t="s">
         <v>185</v>
       </c>
-      <c r="F39" s="67"/>
-      <c r="G39" s="68"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="74"/>
       <c r="H39" s="61"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7695,11 +7704,11 @@
       <c r="D40" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E40" s="69" t="s">
+      <c r="E40" s="75" t="s">
         <v>185</v>
       </c>
-      <c r="F40" s="70"/>
-      <c r="G40" s="71"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="77"/>
       <c r="H40" s="62"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7713,11 +7722,11 @@
       <c r="D41" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E41" s="63" t="s">
+      <c r="E41" s="69" t="s">
         <v>349</v>
       </c>
-      <c r="F41" s="64"/>
-      <c r="G41" s="65"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="71"/>
       <c r="H41" s="60" t="s">
         <v>351</v>
       </c>
@@ -7729,11 +7738,11 @@
       <c r="D42" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E42" s="66" t="s">
+      <c r="E42" s="72" t="s">
         <v>387</v>
       </c>
-      <c r="F42" s="67"/>
-      <c r="G42" s="68"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="74"/>
       <c r="H42" s="61"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7743,11 +7752,11 @@
       <c r="D43" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E43" s="69" t="s">
+      <c r="E43" s="75" t="s">
         <v>388</v>
       </c>
-      <c r="F43" s="70"/>
-      <c r="G43" s="71"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="77"/>
       <c r="H43" s="62"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7761,11 +7770,11 @@
       <c r="D44" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E44" s="63" t="s">
+      <c r="E44" s="69" t="s">
         <v>389</v>
       </c>
-      <c r="F44" s="64"/>
-      <c r="G44" s="65"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="71"/>
       <c r="H44" s="60" t="s">
         <v>351</v>
       </c>
@@ -7777,11 +7786,11 @@
       <c r="D45" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E45" s="66" t="s">
+      <c r="E45" s="72" t="s">
         <v>390</v>
       </c>
-      <c r="F45" s="67"/>
-      <c r="G45" s="68"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="74"/>
       <c r="H45" s="61"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7791,11 +7800,11 @@
       <c r="D46" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E46" s="69" t="s">
+      <c r="E46" s="75" t="s">
         <v>390</v>
       </c>
-      <c r="F46" s="70"/>
-      <c r="G46" s="71"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="77"/>
       <c r="H46" s="62"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7809,11 +7818,11 @@
       <c r="D47" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="E47" s="63" t="s">
+      <c r="E47" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="F47" s="64"/>
-      <c r="G47" s="65"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="71"/>
       <c r="H47" s="60" t="s">
         <v>351</v>
       </c>
@@ -7825,11 +7834,11 @@
       <c r="D48" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="E48" s="66" t="s">
+      <c r="E48" s="72" t="s">
         <v>391</v>
       </c>
-      <c r="F48" s="67"/>
-      <c r="G48" s="68"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="74"/>
       <c r="H48" s="61"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7839,24 +7848,64 @@
       <c r="D49" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="E49" s="69" t="s">
+      <c r="E49" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="F49" s="70"/>
-      <c r="G49" s="71"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="77"/>
       <c r="H49" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -7873,55 +7922,15 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9565,7 +9574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="M12" sqref="M12"/>
     </sheetView>
@@ -10576,13 +10585,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E308052D-1B88-4699-843E-12AA607B59B8}">
-  <dimension ref="A1:AA49"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L51" sqref="L51"/>
+      <selection pane="bottomRight" activeCell="Y52" sqref="Y52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14548,20 +14557,184 @@
         <v>37</v>
       </c>
       <c r="Y48" cm="1">
-        <f t="array" aca="1" ref="Y48" ca="1">INDEX(Caliber!C11:'Caliber'!D21,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B11:'Caliber'!B21,0),2)</f>
+        <f t="array" aca="1" ref="Y48" ca="1">INDEX(Caliber!C12:'Caliber'!D22,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B12:'Caliber'!B22,0),2)</f>
         <v>0.4</v>
       </c>
       <c r="Z48" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="24:25" x14ac:dyDescent="0.25">
-      <c r="X49" t="e" cm="1">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>455</v>
+      </c>
+      <c r="B49">
+        <v>24</v>
+      </c>
+      <c r="C49" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" t="s">
+        <v>76</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>50</v>
+      </c>
+      <c r="H49">
+        <v>125</v>
+      </c>
+      <c r="I49">
+        <v>60</v>
+      </c>
+      <c r="J49">
+        <v>40</v>
+      </c>
+      <c r="K49">
+        <v>60</v>
+      </c>
+      <c r="L49">
+        <v>90</v>
+      </c>
+      <c r="M49">
+        <v>50</v>
+      </c>
+      <c r="N49">
+        <v>60</v>
+      </c>
+      <c r="O49">
+        <v>60</v>
+      </c>
+      <c r="P49">
+        <v>40</v>
+      </c>
+      <c r="Q49">
+        <v>50</v>
+      </c>
+      <c r="R49">
+        <v>200</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <v>1</v>
+      </c>
+      <c r="V49">
+        <v>3</v>
+      </c>
+      <c r="W49" t="s">
+        <v>121</v>
+      </c>
+      <c r="X49" cm="1">
         <f t="array" aca="1" ref="X49" ca="1">INDEX(Caliber!B12:'Caliber'!C22,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B12:'Caliber'!B22,0),2)</f>
+        <v>37</v>
+      </c>
+      <c r="Y49" cm="1">
+        <f t="array" aca="1" ref="Y49" ca="1">INDEX(Caliber!C12:'Caliber'!D22,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B12:'Caliber'!B22,0),2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>456</v>
+      </c>
+      <c r="B50">
+        <v>30</v>
+      </c>
+      <c r="C50" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" t="s">
+        <v>457</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>50</v>
+      </c>
+      <c r="H50">
+        <v>12</v>
+      </c>
+      <c r="I50">
+        <v>70</v>
+      </c>
+      <c r="J50">
+        <v>40</v>
+      </c>
+      <c r="K50">
+        <v>55</v>
+      </c>
+      <c r="L50">
+        <v>40</v>
+      </c>
+      <c r="M50">
+        <v>60</v>
+      </c>
+      <c r="N50">
+        <v>45</v>
+      </c>
+      <c r="O50">
+        <v>16</v>
+      </c>
+      <c r="P50">
+        <v>32</v>
+      </c>
+      <c r="Q50">
+        <v>26</v>
+      </c>
+      <c r="R50">
+        <v>200</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+      <c r="V50">
+        <v>3</v>
+      </c>
+      <c r="W50" t="s">
+        <v>121</v>
+      </c>
+      <c r="X50" cm="1">
+        <f t="array" aca="1" ref="X50" ca="1">INDEX(Caliber!B12:'Caliber'!C22,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B12:'Caliber'!B22,0),2)</f>
+        <v>37</v>
+      </c>
+      <c r="Y50" cm="1">
+        <f t="array" aca="1" ref="Y50" ca="1">INDEX(Caliber!C12:'Caliber'!D22,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B12:'Caliber'!B22,0),2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X51" t="e" cm="1">
+        <f t="array" aca="1" ref="X51" ca="1">INDEX(Caliber!B12:'Caliber'!C22,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B12:'Caliber'!B22,0),2)</f>
         <v>#N/A</v>
       </c>
-      <c r="Y49" t="e" cm="1">
-        <f t="array" aca="1" ref="Y49" ca="1">INDEX(Caliber!C12:'Caliber'!D22,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B12:'Caliber'!B22,0),2)</f>
+      <c r="Y51" t="e" cm="1">
+        <f t="array" aca="1" ref="Y51" ca="1">INDEX(Caliber!C12:'Caliber'!D22,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B12:'Caliber'!B22,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Readjusted shotgun stats to work with choke
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393EE2D0-7BA1-47F4-9F0F-F579633BCC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEB7E2E-F448-4C29-846D-0EEADFC8CD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="24885" yWindow="2790" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -1953,7 +1953,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2074,6 +2074,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2107,24 +2109,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2152,12 +2136,27 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3522,7 +3521,7 @@
       <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
+      <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -3545,7 +3544,7 @@
       <c r="Q9" s="11"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
+      <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>446</v>
       </c>
@@ -3566,7 +3565,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="85"/>
+      <c r="A11" s="57"/>
       <c r="B11" t="s">
         <v>468</v>
       </c>
@@ -3599,7 +3598,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="84" t="s">
+      <c r="A12" s="56" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
@@ -4770,43 +4769,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="60" t="s">
         <v>238</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="58" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="56" t="s">
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="L1" s="56" t="s">
+      <c r="L1" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="M1" s="56" t="s">
+      <c r="M1" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="N1" s="56" t="s">
+      <c r="N1" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="O1" s="56" t="s">
+      <c r="O1" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="P1" s="56" t="s">
+      <c r="P1" s="58" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
+      <c r="A2" s="59"/>
       <c r="B2" s="21" t="s">
         <v>246</v>
       </c>
@@ -4834,12 +4833,12 @@
       <c r="J2" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
     </row>
     <row r="3" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
@@ -6402,7 +6401,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="63" t="s">
         <v>338</v>
       </c>
       <c r="B3" s="27" t="s">
@@ -6448,7 +6447,7 @@
       <c r="P3" s="40"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="33" t="s">
         <v>300</v>
       </c>
@@ -6492,7 +6491,7 @@
       <c r="P4" s="39"/>
     </row>
     <row r="5" spans="1:16" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="27" t="s">
         <v>317</v>
       </c>
@@ -6536,7 +6535,7 @@
       <c r="P5" s="40"/>
     </row>
     <row r="6" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="33" t="s">
         <v>319</v>
       </c>
@@ -6580,7 +6579,7 @@
       <c r="P6" s="39"/>
     </row>
     <row r="7" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="27" t="s">
         <v>321</v>
       </c>
@@ -6624,7 +6623,7 @@
       <c r="P7" s="40"/>
     </row>
     <row r="8" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="33" t="s">
         <v>323</v>
       </c>
@@ -6668,7 +6667,7 @@
       <c r="P8" s="39"/>
     </row>
     <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="27" t="s">
         <v>325</v>
       </c>
@@ -6712,7 +6711,7 @@
       <c r="P9" s="40"/>
     </row>
     <row r="10" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="63"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="33" t="s">
         <v>326</v>
       </c>
@@ -6756,7 +6755,7 @@
       <c r="P10" s="39"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="63" t="s">
         <v>339</v>
       </c>
       <c r="B11" s="27" t="s">
@@ -6778,7 +6777,7 @@
       <c r="P11" s="40"/>
     </row>
     <row r="12" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="33" t="s">
         <v>300</v>
       </c>
@@ -6822,7 +6821,7 @@
       <c r="P12" s="39"/>
     </row>
     <row r="13" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="27" t="s">
         <v>331</v>
       </c>
@@ -6866,7 +6865,7 @@
       <c r="P13" s="40"/>
     </row>
     <row r="14" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="33" t="s">
         <v>319</v>
       </c>
@@ -6910,7 +6909,7 @@
       <c r="P14" s="39"/>
     </row>
     <row r="15" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="27" t="s">
         <v>288</v>
       </c>
@@ -6954,7 +6953,7 @@
       <c r="P15" s="40"/>
     </row>
     <row r="16" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="33" t="s">
         <v>323</v>
       </c>
@@ -6998,7 +6997,7 @@
       <c r="P16" s="39"/>
     </row>
     <row r="17" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="62"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="27" t="s">
         <v>317</v>
       </c>
@@ -7042,7 +7041,7 @@
       <c r="P17" s="40"/>
     </row>
     <row r="18" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="63"/>
+      <c r="A18" s="65"/>
       <c r="B18" s="33" t="s">
         <v>326</v>
       </c>
@@ -7143,13 +7142,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="66" t="s">
         <v>299</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="66" t="s">
         <v>299</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7164,14 +7163,14 @@
       <c r="G2" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="47" t="s">
         <v>350</v>
       </c>
@@ -7184,12 +7183,12 @@
       <c r="G3" s="47" t="s">
         <v>351</v>
       </c>
-      <c r="H3" s="65"/>
+      <c r="H3" s="67"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="A4" s="67"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
       <c r="D4" s="48" t="s">
         <v>352</v>
       </c>
@@ -7202,14 +7201,14 @@
       <c r="G4" s="48" t="s">
         <v>354</v>
       </c>
-      <c r="H4" s="66"/>
+      <c r="H4" s="68"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="65"/>
-      <c r="B5" s="64" t="s">
+      <c r="A5" s="67"/>
+      <c r="B5" s="66" t="s">
         <v>300</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="66" t="s">
         <v>300</v>
       </c>
       <c r="D5" s="46" t="s">
@@ -7224,14 +7223,14 @@
       <c r="G5" s="46" t="s">
         <v>355</v>
       </c>
-      <c r="H5" s="64" t="s">
+      <c r="H5" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
       <c r="D6" s="47" t="s">
         <v>350</v>
       </c>
@@ -7244,12 +7243,12 @@
       <c r="G6" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="H6" s="65"/>
+      <c r="H6" s="67"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
       <c r="D7" s="48" t="s">
         <v>352</v>
       </c>
@@ -7262,14 +7261,14 @@
       <c r="G7" s="48" t="s">
         <v>353</v>
       </c>
-      <c r="H7" s="66"/>
+      <c r="H7" s="68"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
-      <c r="B8" s="64" t="s">
+      <c r="A8" s="67"/>
+      <c r="B8" s="66" t="s">
         <v>358</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="66" t="s">
         <v>317</v>
       </c>
       <c r="D8" s="46" t="s">
@@ -7284,14 +7283,14 @@
       <c r="G8" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="66" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="65"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
       <c r="D9" s="47" t="s">
         <v>350</v>
       </c>
@@ -7304,12 +7303,12 @@
       <c r="G9" s="47" t="s">
         <v>212</v>
       </c>
-      <c r="H9" s="65"/>
+      <c r="H9" s="67"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="65"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="48" t="s">
         <v>352</v>
       </c>
@@ -7322,14 +7321,14 @@
       <c r="G10" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="H10" s="66"/>
+      <c r="H10" s="68"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="65"/>
-      <c r="B11" s="64" t="s">
+      <c r="A11" s="67"/>
+      <c r="B11" s="66" t="s">
         <v>360</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="66" t="s">
         <v>319</v>
       </c>
       <c r="D11" s="46" t="s">
@@ -7344,14 +7343,14 @@
       <c r="G11" s="46" t="s">
         <v>361</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="H11" s="66" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="47" t="s">
         <v>350</v>
       </c>
@@ -7364,12 +7363,12 @@
       <c r="G12" s="47" t="s">
         <v>363</v>
       </c>
-      <c r="H12" s="65"/>
+      <c r="H12" s="67"/>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
       <c r="D13" s="48" t="s">
         <v>352</v>
       </c>
@@ -7382,14 +7381,14 @@
       <c r="G13" s="48" t="s">
         <v>353</v>
       </c>
-      <c r="H13" s="66"/>
+      <c r="H13" s="68"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="65"/>
-      <c r="B14" s="64" t="s">
+      <c r="A14" s="67"/>
+      <c r="B14" s="66" t="s">
         <v>365</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="66" t="s">
         <v>321</v>
       </c>
       <c r="D14" s="46" t="s">
@@ -7404,14 +7403,14 @@
       <c r="G14" s="46" t="s">
         <v>182</v>
       </c>
-      <c r="H14" s="64" t="s">
+      <c r="H14" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="65"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="47" t="s">
         <v>350</v>
       </c>
@@ -7424,12 +7423,12 @@
       <c r="G15" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="H15" s="65"/>
+      <c r="H15" s="67"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="65"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
+      <c r="A16" s="67"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="48" t="s">
         <v>352</v>
       </c>
@@ -7442,14 +7441,14 @@
       <c r="G16" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="H16" s="66"/>
+      <c r="H16" s="68"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="65"/>
-      <c r="B17" s="64" t="s">
+      <c r="A17" s="67"/>
+      <c r="B17" s="66" t="s">
         <v>366</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="66" t="s">
         <v>323</v>
       </c>
       <c r="D17" s="46" t="s">
@@ -7464,14 +7463,14 @@
       <c r="G17" s="46" t="s">
         <v>367</v>
       </c>
-      <c r="H17" s="64" t="s">
+      <c r="H17" s="66" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="65"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="47" t="s">
         <v>350</v>
       </c>
@@ -7484,12 +7483,12 @@
       <c r="G18" s="47" t="s">
         <v>356</v>
       </c>
-      <c r="H18" s="65"/>
+      <c r="H18" s="67"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
-      <c r="B19" s="66"/>
-      <c r="C19" s="66"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
       <c r="D19" s="48" t="s">
         <v>352</v>
       </c>
@@ -7502,14 +7501,14 @@
       <c r="G19" s="48" t="s">
         <v>368</v>
       </c>
-      <c r="H19" s="66"/>
+      <c r="H19" s="68"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="65"/>
-      <c r="B20" s="64" t="s">
+      <c r="A20" s="67"/>
+      <c r="B20" s="66" t="s">
         <v>369</v>
       </c>
-      <c r="C20" s="64" t="s">
+      <c r="C20" s="66" t="s">
         <v>325</v>
       </c>
       <c r="D20" s="46" t="s">
@@ -7524,14 +7523,14 @@
       <c r="G20" s="46" t="s">
         <v>372</v>
       </c>
-      <c r="H20" s="64" t="s">
+      <c r="H20" s="66" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
       <c r="D21" s="47" t="s">
         <v>350</v>
       </c>
@@ -7544,12 +7543,12 @@
       <c r="G21" s="47" t="s">
         <v>372</v>
       </c>
-      <c r="H21" s="65"/>
+      <c r="H21" s="67"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="65"/>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="68"/>
       <c r="D22" s="48" t="s">
         <v>352</v>
       </c>
@@ -7562,14 +7561,14 @@
       <c r="G22" s="48" t="s">
         <v>375</v>
       </c>
-      <c r="H22" s="66"/>
+      <c r="H22" s="68"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
-      <c r="B23" s="64" t="s">
+      <c r="A23" s="67"/>
+      <c r="B23" s="66" t="s">
         <v>376</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="66" t="s">
         <v>326</v>
       </c>
       <c r="D23" s="46" t="s">
@@ -7584,14 +7583,14 @@
       <c r="G23" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="H23" s="64" t="s">
+      <c r="H23" s="66" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
       <c r="D24" s="47" t="s">
         <v>350</v>
       </c>
@@ -7604,12 +7603,12 @@
       <c r="G24" s="47" t="s">
         <v>378</v>
       </c>
-      <c r="H24" s="65"/>
+      <c r="H24" s="67"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="66"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
+      <c r="A25" s="68"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="68"/>
       <c r="D25" s="48" t="s">
         <v>352</v>
       </c>
@@ -7622,421 +7621,413 @@
       <c r="G25" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="H25" s="66"/>
+      <c r="H25" s="68"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="66" t="s">
         <v>339</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="66" t="s">
         <v>299</v>
       </c>
-      <c r="C26" s="64" t="s">
+      <c r="C26" s="66" t="s">
         <v>299</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E26" s="67"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="70"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="81"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
+      <c r="A27" s="67"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
       <c r="D27" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E27" s="67"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="71"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="82"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="65"/>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
+      <c r="A28" s="67"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="68"/>
       <c r="D28" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E28" s="67"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="72"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="83"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
-      <c r="B29" s="64" t="s">
+      <c r="A29" s="67"/>
+      <c r="B29" s="66" t="s">
         <v>300</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="66" t="s">
         <v>300</v>
       </c>
       <c r="D29" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E29" s="73" t="s">
+      <c r="E29" s="69" t="s">
         <v>379</v>
       </c>
-      <c r="F29" s="74"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="64" t="s">
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
       <c r="D30" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E30" s="76" t="s">
+      <c r="E30" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="77"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="65"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="67"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="68"/>
       <c r="D31" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E31" s="79" t="s">
+      <c r="E31" s="75" t="s">
         <v>380</v>
       </c>
-      <c r="F31" s="80"/>
-      <c r="G31" s="81"/>
-      <c r="H31" s="66"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="68"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
-      <c r="B32" s="64" t="s">
+      <c r="A32" s="67"/>
+      <c r="B32" s="66" t="s">
         <v>358</v>
       </c>
-      <c r="C32" s="64" t="s">
+      <c r="C32" s="66" t="s">
         <v>331</v>
       </c>
       <c r="D32" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E32" s="73" t="s">
+      <c r="E32" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="F32" s="74"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="64" t="s">
+      <c r="F32" s="70"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="65"/>
-      <c r="B33" s="65"/>
-      <c r="C33" s="65"/>
+      <c r="A33" s="67"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
       <c r="D33" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E33" s="76" t="s">
+      <c r="E33" s="72" t="s">
         <v>382</v>
       </c>
-      <c r="F33" s="77"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="65"/>
+      <c r="F33" s="73"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="67"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
       <c r="D34" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E34" s="79" t="s">
+      <c r="E34" s="75" t="s">
         <v>383</v>
       </c>
-      <c r="F34" s="80"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="66"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="68"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="65"/>
-      <c r="B35" s="64" t="s">
+      <c r="A35" s="67"/>
+      <c r="B35" s="66" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="64" t="s">
+      <c r="C35" s="66" t="s">
         <v>319</v>
       </c>
       <c r="D35" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E35" s="73" t="s">
+      <c r="E35" s="69" t="s">
         <v>379</v>
       </c>
-      <c r="F35" s="74"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="64" t="s">
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="65"/>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65"/>
+      <c r="A36" s="67"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="67"/>
       <c r="D36" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E36" s="76" t="s">
+      <c r="E36" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="F36" s="77"/>
-      <c r="G36" s="78"/>
-      <c r="H36" s="65"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="67"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="65"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="66"/>
+      <c r="A37" s="67"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="68"/>
       <c r="D37" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E37" s="79" t="s">
+      <c r="E37" s="75" t="s">
         <v>380</v>
       </c>
-      <c r="F37" s="80"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="66"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="68"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="65"/>
-      <c r="B38" s="64" t="s">
+      <c r="A38" s="67"/>
+      <c r="B38" s="66" t="s">
         <v>365</v>
       </c>
-      <c r="C38" s="64" t="s">
+      <c r="C38" s="66" t="s">
         <v>288</v>
       </c>
       <c r="D38" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E38" s="73" t="s">
+      <c r="E38" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="F38" s="74"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="64" t="s">
+      <c r="F38" s="70"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="66" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="65"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
+      <c r="A39" s="67"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="67"/>
       <c r="D39" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E39" s="76" t="s">
+      <c r="E39" s="72" t="s">
         <v>184</v>
       </c>
-      <c r="F39" s="77"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="65"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="67"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="65"/>
-      <c r="B40" s="66"/>
-      <c r="C40" s="66"/>
+      <c r="A40" s="67"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
       <c r="D40" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E40" s="79" t="s">
+      <c r="E40" s="75" t="s">
         <v>184</v>
       </c>
-      <c r="F40" s="80"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="66"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="68"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="65"/>
-      <c r="B41" s="64" t="s">
+      <c r="A41" s="67"/>
+      <c r="B41" s="66" t="s">
         <v>366</v>
       </c>
-      <c r="C41" s="64" t="s">
+      <c r="C41" s="66" t="s">
         <v>323</v>
       </c>
       <c r="D41" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E41" s="73" t="s">
+      <c r="E41" s="69" t="s">
         <v>347</v>
       </c>
-      <c r="F41" s="74"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="64" t="s">
+      <c r="F41" s="70"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="65"/>
-      <c r="B42" s="65"/>
-      <c r="C42" s="65"/>
+      <c r="A42" s="67"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="67"/>
       <c r="D42" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E42" s="76" t="s">
+      <c r="E42" s="72" t="s">
         <v>385</v>
       </c>
-      <c r="F42" s="77"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="65"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="67"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="65"/>
-      <c r="B43" s="66"/>
-      <c r="C43" s="66"/>
+      <c r="A43" s="67"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
       <c r="D43" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E43" s="79" t="s">
+      <c r="E43" s="75" t="s">
         <v>386</v>
       </c>
-      <c r="F43" s="80"/>
-      <c r="G43" s="81"/>
-      <c r="H43" s="66"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="68"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="65"/>
-      <c r="B44" s="64" t="s">
+      <c r="A44" s="67"/>
+      <c r="B44" s="66" t="s">
         <v>369</v>
       </c>
-      <c r="C44" s="64" t="s">
+      <c r="C44" s="66" t="s">
         <v>317</v>
       </c>
       <c r="D44" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E44" s="73" t="s">
+      <c r="E44" s="69" t="s">
         <v>387</v>
       </c>
-      <c r="F44" s="74"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="64" t="s">
+      <c r="F44" s="70"/>
+      <c r="G44" s="71"/>
+      <c r="H44" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="65"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
+      <c r="A45" s="67"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
       <c r="D45" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E45" s="76" t="s">
+      <c r="E45" s="72" t="s">
         <v>388</v>
       </c>
-      <c r="F45" s="77"/>
-      <c r="G45" s="78"/>
-      <c r="H45" s="65"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="67"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="65"/>
-      <c r="B46" s="66"/>
-      <c r="C46" s="66"/>
+      <c r="A46" s="67"/>
+      <c r="B46" s="68"/>
+      <c r="C46" s="68"/>
       <c r="D46" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E46" s="79" t="s">
+      <c r="E46" s="75" t="s">
         <v>388</v>
       </c>
-      <c r="F46" s="80"/>
-      <c r="G46" s="81"/>
-      <c r="H46" s="66"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="77"/>
+      <c r="H46" s="68"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="65"/>
-      <c r="B47" s="64" t="s">
+      <c r="A47" s="67"/>
+      <c r="B47" s="66" t="s">
         <v>376</v>
       </c>
-      <c r="C47" s="64" t="s">
+      <c r="C47" s="66" t="s">
         <v>326</v>
       </c>
       <c r="D47" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E47" s="73" t="s">
+      <c r="E47" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="F47" s="74"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="64" t="s">
+      <c r="F47" s="70"/>
+      <c r="G47" s="71"/>
+      <c r="H47" s="66" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="65"/>
-      <c r="B48" s="65"/>
-      <c r="C48" s="65"/>
+      <c r="A48" s="67"/>
+      <c r="B48" s="67"/>
+      <c r="C48" s="67"/>
       <c r="D48" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E48" s="76" t="s">
+      <c r="E48" s="72" t="s">
         <v>389</v>
       </c>
-      <c r="F48" s="77"/>
-      <c r="G48" s="78"/>
-      <c r="H48" s="65"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="67"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="66"/>
-      <c r="B49" s="66"/>
-      <c r="C49" s="66"/>
+      <c r="A49" s="68"/>
+      <c r="B49" s="68"/>
+      <c r="C49" s="68"/>
       <c r="D49" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E49" s="79" t="s">
+      <c r="E49" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="F49" s="80"/>
-      <c r="G49" s="81"/>
-      <c r="H49" s="66"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="77"/>
+      <c r="H49" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8053,31 +8044,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8575,24 +8574,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="84" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="82"/>
+      <c r="B1" s="84"/>
       <c r="C1" s="52"/>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="82"/>
-      <c r="B3" s="82"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="84"/>
       <c r="C3" s="52"/>
       <c r="D3" s="52"/>
       <c r="E3" s="52"/>
@@ -9882,9 +9881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17566,7 +17565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0094531B-7BBB-4DD3-8835-99962592A6C6}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="P9" sqref="P9"/>
     </sheetView>

</xml_diff>

<commit_message>
MP7 Floor & Hand sprites
Just need mag sprites now, also updated spreadsheet to have the proper mags for the mp7
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17BA872-6057-4B56-883C-2772185146CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4F21D9-561B-4CB6-8FAA-2C3669571EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -2112,24 +2112,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2156,6 +2138,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3323,8 +3323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7639,10 +7639,10 @@
       <c r="D26" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E26" s="69"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="72"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="81"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="67"/>
@@ -7651,10 +7651,10 @@
       <c r="D27" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E27" s="69"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="73"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="80"/>
+      <c r="H27" s="82"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="67"/>
@@ -7663,10 +7663,10 @@
       <c r="D28" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E28" s="69"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="74"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="83"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="67"/>
@@ -7679,11 +7679,11 @@
       <c r="D29" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E29" s="75" t="s">
+      <c r="E29" s="69" t="s">
         <v>379</v>
       </c>
-      <c r="F29" s="76"/>
-      <c r="G29" s="77"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
       <c r="H29" s="66" t="s">
         <v>349</v>
       </c>
@@ -7695,11 +7695,11 @@
       <c r="D30" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E30" s="78" t="s">
+      <c r="E30" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="F30" s="79"/>
-      <c r="G30" s="80"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="74"/>
       <c r="H30" s="67"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7709,11 +7709,11 @@
       <c r="D31" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E31" s="81" t="s">
+      <c r="E31" s="75" t="s">
         <v>380</v>
       </c>
-      <c r="F31" s="82"/>
-      <c r="G31" s="83"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="77"/>
       <c r="H31" s="68"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7727,11 +7727,11 @@
       <c r="D32" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E32" s="75" t="s">
+      <c r="E32" s="69" t="s">
         <v>381</v>
       </c>
-      <c r="F32" s="76"/>
-      <c r="G32" s="77"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="71"/>
       <c r="H32" s="66" t="s">
         <v>349</v>
       </c>
@@ -7743,11 +7743,11 @@
       <c r="D33" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E33" s="78" t="s">
+      <c r="E33" s="72" t="s">
         <v>382</v>
       </c>
-      <c r="F33" s="79"/>
-      <c r="G33" s="80"/>
+      <c r="F33" s="73"/>
+      <c r="G33" s="74"/>
       <c r="H33" s="67"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7757,11 +7757,11 @@
       <c r="D34" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E34" s="81" t="s">
+      <c r="E34" s="75" t="s">
         <v>383</v>
       </c>
-      <c r="F34" s="82"/>
-      <c r="G34" s="83"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="77"/>
       <c r="H34" s="68"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7775,11 +7775,11 @@
       <c r="D35" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E35" s="75" t="s">
+      <c r="E35" s="69" t="s">
         <v>379</v>
       </c>
-      <c r="F35" s="76"/>
-      <c r="G35" s="77"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="71"/>
       <c r="H35" s="66" t="s">
         <v>349</v>
       </c>
@@ -7791,11 +7791,11 @@
       <c r="D36" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E36" s="78" t="s">
+      <c r="E36" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="F36" s="79"/>
-      <c r="G36" s="80"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="74"/>
       <c r="H36" s="67"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7805,11 +7805,11 @@
       <c r="D37" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E37" s="81" t="s">
+      <c r="E37" s="75" t="s">
         <v>380</v>
       </c>
-      <c r="F37" s="82"/>
-      <c r="G37" s="83"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="77"/>
       <c r="H37" s="68"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7823,11 +7823,11 @@
       <c r="D38" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E38" s="75" t="s">
+      <c r="E38" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="F38" s="76"/>
-      <c r="G38" s="77"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="71"/>
       <c r="H38" s="66" t="s">
         <v>384</v>
       </c>
@@ -7839,11 +7839,11 @@
       <c r="D39" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E39" s="78" t="s">
+      <c r="E39" s="72" t="s">
         <v>184</v>
       </c>
-      <c r="F39" s="79"/>
-      <c r="G39" s="80"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="74"/>
       <c r="H39" s="67"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7853,11 +7853,11 @@
       <c r="D40" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E40" s="81" t="s">
+      <c r="E40" s="75" t="s">
         <v>184</v>
       </c>
-      <c r="F40" s="82"/>
-      <c r="G40" s="83"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="77"/>
       <c r="H40" s="68"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7871,11 +7871,11 @@
       <c r="D41" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E41" s="75" t="s">
+      <c r="E41" s="69" t="s">
         <v>347</v>
       </c>
-      <c r="F41" s="76"/>
-      <c r="G41" s="77"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="71"/>
       <c r="H41" s="66" t="s">
         <v>349</v>
       </c>
@@ -7887,11 +7887,11 @@
       <c r="D42" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E42" s="78" t="s">
+      <c r="E42" s="72" t="s">
         <v>385</v>
       </c>
-      <c r="F42" s="79"/>
-      <c r="G42" s="80"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="74"/>
       <c r="H42" s="67"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7901,11 +7901,11 @@
       <c r="D43" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E43" s="81" t="s">
+      <c r="E43" s="75" t="s">
         <v>386</v>
       </c>
-      <c r="F43" s="82"/>
-      <c r="G43" s="83"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="77"/>
       <c r="H43" s="68"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7919,11 +7919,11 @@
       <c r="D44" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E44" s="75" t="s">
+      <c r="E44" s="69" t="s">
         <v>387</v>
       </c>
-      <c r="F44" s="76"/>
-      <c r="G44" s="77"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="71"/>
       <c r="H44" s="66" t="s">
         <v>349</v>
       </c>
@@ -7935,11 +7935,11 @@
       <c r="D45" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E45" s="78" t="s">
+      <c r="E45" s="72" t="s">
         <v>388</v>
       </c>
-      <c r="F45" s="79"/>
-      <c r="G45" s="80"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="74"/>
       <c r="H45" s="67"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7949,11 +7949,11 @@
       <c r="D46" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E46" s="81" t="s">
+      <c r="E46" s="75" t="s">
         <v>388</v>
       </c>
-      <c r="F46" s="82"/>
-      <c r="G46" s="83"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="77"/>
       <c r="H46" s="68"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7967,11 +7967,11 @@
       <c r="D47" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="E47" s="75" t="s">
+      <c r="E47" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="F47" s="76"/>
-      <c r="G47" s="77"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="71"/>
       <c r="H47" s="66" t="s">
         <v>349</v>
       </c>
@@ -7983,11 +7983,11 @@
       <c r="D48" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="E48" s="78" t="s">
+      <c r="E48" s="72" t="s">
         <v>389</v>
       </c>
-      <c r="F48" s="79"/>
-      <c r="G48" s="80"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="74"/>
       <c r="H48" s="67"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7997,48 +7997,40 @@
       <c r="D49" s="48" t="s">
         <v>352</v>
       </c>
-      <c r="E49" s="81" t="s">
+      <c r="E49" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="F49" s="82"/>
-      <c r="G49" s="83"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="77"/>
       <c r="H49" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8055,31 +8047,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9883,9 +9883,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G24" sqref="G24"/>
+      <selection pane="topRight" activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10215,18 +10215,18 @@
         <v>7</v>
       </c>
       <c r="V4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="W4">
         <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V4,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X4">
         <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V4,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="Y4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="Z4" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
Pistol double tap added
Might need some balancing. Also fixed 5.7 ammo list order.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A7CBD3-9A73-4A2F-A905-21E5DF5229FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9711C4-44BD-42E3-9BD9-7A58D366F919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="3285" windowWidth="21600" windowHeight="11385" firstSheet="9" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="5985" yWindow="3285" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="475">
   <si>
     <t>Name</t>
   </si>
@@ -1579,12 +1579,6 @@
     <t>[30,100]</t>
   </si>
   <si>
-    <t>Pistol double tap?</t>
-  </si>
-  <si>
-    <t>Was mentioned at one point, don’t know if we had plans though</t>
-  </si>
-  <si>
     <t>CBJ-MS SAW</t>
   </si>
   <si>
@@ -1594,9 +1588,6 @@
     <t>M3</t>
   </si>
   <si>
-    <t>Add MP7 &amp; Inc shotgun ammo to drawio file</t>
-  </si>
-  <si>
     <t>12G Incendiary</t>
   </si>
   <si>
@@ -1616,6 +1607,9 @@
   </si>
   <si>
     <t>NL, Slug &amp; Inc ammo</t>
+  </si>
+  <si>
+    <t>Add MP7 &amp; Inc shotgun ammo to drawio file, needs an update in general</t>
   </si>
 </sst>
 </file>
@@ -1968,7 +1962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2173,7 +2167,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4207,7 +4200,7 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C28">
         <v>15</v>
@@ -4228,7 +4221,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="M28" s="16" t="s">
         <v>39</v>
@@ -4255,28 +4248,28 @@
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
-        <v>473</v>
-      </c>
-      <c r="C29" s="86">
+        <v>470</v>
+      </c>
+      <c r="C29">
         <v>10</v>
       </c>
-      <c r="D29" s="86">
+      <c r="D29">
         <v>4</v>
       </c>
       <c r="E29">
         <v>25</v>
       </c>
-      <c r="F29" s="86">
-        <v>0</v>
-      </c>
-      <c r="G29" s="86">
-        <v>1</v>
-      </c>
-      <c r="H29" s="86">
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -4760,7 +4753,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
@@ -8635,7 +8628,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8687,16 +8680,11 @@
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>464</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>465</v>
-      </c>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="B10" s="14"/>
     </row>
@@ -8789,7 +8777,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X3" sqref="X3"/>
+      <selection pane="topRight" activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8958,7 +8946,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U2">
         <v>3</v>
@@ -9037,7 +9025,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U3">
         <v>3</v>
@@ -9119,7 +9107,7 @@
         <v>1</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U4">
         <v>3</v>
@@ -9280,7 +9268,7 @@
         <v>1</v>
       </c>
       <c r="T6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U6">
         <v>3</v>
@@ -9359,7 +9347,7 @@
         <v>1</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U7">
         <v>3</v>
@@ -9438,7 +9426,7 @@
         <v>1</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U8">
         <v>3</v>
@@ -9517,7 +9505,7 @@
         <v>1</v>
       </c>
       <c r="T9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9">
         <v>3</v>
@@ -9675,7 +9663,7 @@
         <v>1</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11">
         <v>3</v>
@@ -9912,7 +9900,7 @@
         <v>1</v>
       </c>
       <c r="T14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U14">
         <v>3</v>
@@ -10529,7 +10517,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B8">
         <v>21</v>
@@ -16990,7 +16978,7 @@
         <v>160</v>
       </c>
       <c r="AB3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -17079,7 +17067,7 @@
         <v>178</v>
       </c>
       <c r="AB4" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -17168,7 +17156,7 @@
         <v>178</v>
       </c>
       <c r="AB5" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -17618,7 +17606,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B11">
         <v>24</v>
@@ -17702,7 +17690,7 @@
         <v>178</v>
       </c>
       <c r="AB11" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -18407,7 +18395,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B9">
         <v>24</v>

</xml_diff>

<commit_message>
MCD fixes, P90 SOPMOD
Also fixed some buy requirements that were not updated
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DA5476-6EBA-49E4-B037-F16092165484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E524502F-078B-4F59-9AD0-0B46F28B6368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="480">
   <si>
     <t>Name</t>
   </si>
@@ -1619,6 +1619,12 @@
   </si>
   <si>
     <t>Mk 18 Mod 0 SOPMOD</t>
+  </si>
+  <si>
+    <t>Set up campaign tech tree with new weapons</t>
+  </si>
+  <si>
+    <t>P90 (Sopmod)</t>
   </si>
 </sst>
 </file>
@@ -2163,7 +2169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2287,6 +2293,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2311,7 +2329,7 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2320,20 +2338,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2353,11 +2365,53 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2368,57 +2422,10 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3134,10 +3141,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB47442F-754D-45A1-BC57-BBE7964D0858}" name="Table10" displayName="Table10" ref="A1:Z14" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
-  <autoFilter ref="A1:Z14" xr:uid="{EB47442F-754D-45A1-BC57-BBE7964D0858}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z14">
-    <sortCondition descending="1" ref="M1:M14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB47442F-754D-45A1-BC57-BBE7964D0858}" name="Table10" displayName="Table10" ref="A1:Z15" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A1:Z15" xr:uid="{EB47442F-754D-45A1-BC57-BBE7964D0858}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z15">
+    <sortCondition descending="1" ref="M1:M15"/>
   </sortState>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{5824021B-BC67-48E1-A206-55414C872ECA}" name="Name"/>
@@ -5069,7 +5076,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -5085,43 +5092,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="63" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="61" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="65" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="59" t="s">
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="63" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="63" t="s">
         <v>240</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="63" t="s">
         <v>241</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="63" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="63" t="s">
         <v>243</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="63" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
+      <c r="A2" s="64"/>
       <c r="B2" s="21" t="s">
         <v>245</v>
       </c>
@@ -5149,12 +5156,12 @@
       <c r="J2" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
     </row>
     <row r="3" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
@@ -6717,7 +6724,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="68" t="s">
         <v>337</v>
       </c>
       <c r="B3" s="27" t="s">
@@ -6763,7 +6770,7 @@
       <c r="P3" s="40"/>
     </row>
     <row r="4" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="65"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="33" t="s">
         <v>299</v>
       </c>
@@ -6807,7 +6814,7 @@
       <c r="P4" s="39"/>
     </row>
     <row r="5" spans="1:16" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="65"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="27" t="s">
         <v>316</v>
       </c>
@@ -6851,7 +6858,7 @@
       <c r="P5" s="40"/>
     </row>
     <row r="6" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="65"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="33" t="s">
         <v>318</v>
       </c>
@@ -6895,7 +6902,7 @@
       <c r="P6" s="39"/>
     </row>
     <row r="7" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="65"/>
+      <c r="A7" s="69"/>
       <c r="B7" s="27" t="s">
         <v>320</v>
       </c>
@@ -6939,7 +6946,7 @@
       <c r="P7" s="40"/>
     </row>
     <row r="8" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="33" t="s">
         <v>322</v>
       </c>
@@ -6983,7 +6990,7 @@
       <c r="P8" s="39"/>
     </row>
     <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="65"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="27" t="s">
         <v>324</v>
       </c>
@@ -7027,7 +7034,7 @@
       <c r="P9" s="40"/>
     </row>
     <row r="10" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="33" t="s">
         <v>325</v>
       </c>
@@ -7071,7 +7078,7 @@
       <c r="P10" s="39"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="68" t="s">
         <v>338</v>
       </c>
       <c r="B11" s="27" t="s">
@@ -7093,7 +7100,7 @@
       <c r="P11" s="40"/>
     </row>
     <row r="12" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="33" t="s">
         <v>299</v>
       </c>
@@ -7137,7 +7144,7 @@
       <c r="P12" s="39"/>
     </row>
     <row r="13" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="27" t="s">
         <v>330</v>
       </c>
@@ -7181,7 +7188,7 @@
       <c r="P13" s="40"/>
     </row>
     <row r="14" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="65"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="33" t="s">
         <v>318</v>
       </c>
@@ -7225,7 +7232,7 @@
       <c r="P14" s="39"/>
     </row>
     <row r="15" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="65"/>
+      <c r="A15" s="69"/>
       <c r="B15" s="27" t="s">
         <v>287</v>
       </c>
@@ -7269,7 +7276,7 @@
       <c r="P15" s="40"/>
     </row>
     <row r="16" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="65"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="33" t="s">
         <v>322</v>
       </c>
@@ -7313,7 +7320,7 @@
       <c r="P16" s="39"/>
     </row>
     <row r="17" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="65"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="27" t="s">
         <v>316</v>
       </c>
@@ -7357,7 +7364,7 @@
       <c r="P17" s="40"/>
     </row>
     <row r="18" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="66"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="33" t="s">
         <v>325</v>
       </c>
@@ -7413,8 +7420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7458,13 +7465,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="86" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7479,14 +7486,14 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="86" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
       <c r="D3" s="47" t="s">
         <v>349</v>
       </c>
@@ -7499,54 +7506,54 @@
       <c r="G3" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="H3" s="68"/>
+      <c r="H3" s="72"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="91" t="s">
+      <c r="A4" s="72"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="61" t="s">
         <v>352</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="61" t="s">
         <v>352</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="61" t="s">
         <v>353</v>
       </c>
-      <c r="H4" s="68"/>
+      <c r="H4" s="72"/>
     </row>
     <row r="5" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68"/>
-      <c r="B5" s="95" t="s">
+      <c r="A5" s="72"/>
+      <c r="B5" s="71" t="s">
         <v>299</v>
       </c>
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="71" t="s">
         <v>299</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E5" s="96" t="s">
+      <c r="E5" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="96" t="s">
+      <c r="F5" s="62" t="s">
         <v>354</v>
       </c>
-      <c r="G5" s="96" t="s">
+      <c r="G5" s="62" t="s">
         <v>354</v>
       </c>
-      <c r="H5" s="95" t="s">
+      <c r="H5" s="71" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="68"/>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
       <c r="D6" s="47" t="s">
         <v>349</v>
       </c>
@@ -7559,54 +7566,54 @@
       <c r="G6" s="47" t="s">
         <v>354</v>
       </c>
-      <c r="H6" s="68"/>
+      <c r="H6" s="72"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="87" t="s">
+      <c r="A7" s="72"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E7" s="87" t="s">
+      <c r="E7" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="60" t="s">
         <v>356</v>
       </c>
-      <c r="G7" s="87" t="s">
+      <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="86"/>
+      <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="68"/>
-      <c r="B8" s="95" t="s">
+      <c r="A8" s="72"/>
+      <c r="B8" s="71" t="s">
         <v>357</v>
       </c>
-      <c r="C8" s="95" t="s">
+      <c r="C8" s="71" t="s">
         <v>316</v>
       </c>
-      <c r="D8" s="96" t="s">
+      <c r="D8" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E8" s="96" t="s">
+      <c r="E8" s="62" t="s">
         <v>354</v>
       </c>
-      <c r="F8" s="96" t="s">
+      <c r="F8" s="62" t="s">
         <v>354</v>
       </c>
-      <c r="G8" s="96" t="s">
+      <c r="G8" s="62" t="s">
         <v>220</v>
       </c>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="71" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
       <c r="D9" s="47" t="s">
         <v>349</v>
       </c>
@@ -7619,54 +7626,54 @@
       <c r="G9" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="H9" s="68"/>
+      <c r="H9" s="72"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="68"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="87" t="s">
+      <c r="A10" s="72"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E10" s="87" t="s">
+      <c r="E10" s="60" t="s">
         <v>356</v>
       </c>
-      <c r="F10" s="87" t="s">
+      <c r="F10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="G10" s="87" t="s">
+      <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="86"/>
+      <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="68"/>
-      <c r="B11" s="95" t="s">
+      <c r="A11" s="72"/>
+      <c r="B11" s="71" t="s">
         <v>359</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="71" t="s">
         <v>318</v>
       </c>
-      <c r="D11" s="96" t="s">
+      <c r="D11" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E11" s="96" t="s">
+      <c r="E11" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="F11" s="96" t="s">
+      <c r="F11" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="G11" s="96" t="s">
+      <c r="G11" s="62" t="s">
         <v>360</v>
       </c>
-      <c r="H11" s="95" t="s">
+      <c r="H11" s="71" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="68"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="47" t="s">
         <v>349</v>
       </c>
@@ -7679,54 +7686,54 @@
       <c r="G12" s="47" t="s">
         <v>362</v>
       </c>
-      <c r="H12" s="68"/>
+      <c r="H12" s="72"/>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68"/>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="91" t="s">
+      <c r="A13" s="72"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E13" s="91" t="s">
+      <c r="E13" s="61" t="s">
         <v>363</v>
       </c>
-      <c r="F13" s="91" t="s">
+      <c r="F13" s="61" t="s">
         <v>356</v>
       </c>
-      <c r="G13" s="91" t="s">
+      <c r="G13" s="61" t="s">
         <v>352</v>
       </c>
-      <c r="H13" s="68"/>
+      <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="68"/>
-      <c r="B14" s="95" t="s">
+      <c r="A14" s="72"/>
+      <c r="B14" s="71" t="s">
         <v>364</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="71" t="s">
         <v>320</v>
       </c>
-      <c r="D14" s="96" t="s">
+      <c r="D14" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E14" s="96" t="s">
+      <c r="E14" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="F14" s="96" t="s">
+      <c r="F14" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="G14" s="96" t="s">
+      <c r="G14" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="H14" s="95" t="s">
+      <c r="H14" s="71" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="68"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72"/>
       <c r="D15" s="47" t="s">
         <v>349</v>
       </c>
@@ -7739,54 +7746,54 @@
       <c r="G15" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="H15" s="68"/>
+      <c r="H15" s="72"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="87" t="s">
+      <c r="A16" s="72"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E16" s="87" t="s">
+      <c r="E16" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="F16" s="87" t="s">
+      <c r="F16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="G16" s="87" t="s">
+      <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="86"/>
+      <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="68"/>
-      <c r="B17" s="95" t="s">
+      <c r="A17" s="72"/>
+      <c r="B17" s="71" t="s">
         <v>365</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="71" t="s">
         <v>322</v>
       </c>
-      <c r="D17" s="96" t="s">
+      <c r="D17" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E17" s="96" t="s">
+      <c r="E17" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="96" t="s">
+      <c r="F17" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="96" t="s">
+      <c r="G17" s="62" t="s">
         <v>366</v>
       </c>
-      <c r="H17" s="95" t="s">
+      <c r="H17" s="71" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="68"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
       <c r="D18" s="47" t="s">
         <v>349</v>
       </c>
@@ -7799,54 +7806,54 @@
       <c r="G18" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="H18" s="68"/>
+      <c r="H18" s="72"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="87" t="s">
+      <c r="A19" s="72"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E19" s="87" t="s">
+      <c r="E19" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="87" t="s">
+      <c r="F19" s="60" t="s">
         <v>355</v>
       </c>
-      <c r="G19" s="87" t="s">
+      <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="86"/>
+      <c r="H19" s="87"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="68"/>
-      <c r="B20" s="95" t="s">
+      <c r="A20" s="72"/>
+      <c r="B20" s="71" t="s">
         <v>368</v>
       </c>
-      <c r="C20" s="95" t="s">
+      <c r="C20" s="71" t="s">
         <v>324</v>
       </c>
-      <c r="D20" s="96" t="s">
+      <c r="D20" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E20" s="96" t="s">
+      <c r="E20" s="62" t="s">
         <v>369</v>
       </c>
-      <c r="F20" s="96" t="s">
+      <c r="F20" s="62" t="s">
         <v>370</v>
       </c>
-      <c r="G20" s="96" t="s">
+      <c r="G20" s="62" t="s">
         <v>371</v>
       </c>
-      <c r="H20" s="95" t="s">
+      <c r="H20" s="71" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="68"/>
-      <c r="B21" s="68"/>
-      <c r="C21" s="68"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
       <c r="D21" s="47" t="s">
         <v>349</v>
       </c>
@@ -7859,54 +7866,54 @@
       <c r="G21" s="47" t="s">
         <v>371</v>
       </c>
-      <c r="H21" s="68"/>
+      <c r="H21" s="72"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="68"/>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="91" t="s">
+      <c r="A22" s="72"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E22" s="91" t="s">
+      <c r="E22" s="61" t="s">
         <v>372</v>
       </c>
-      <c r="F22" s="91" t="s">
+      <c r="F22" s="61" t="s">
         <v>373</v>
       </c>
-      <c r="G22" s="91" t="s">
+      <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="69"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="68"/>
-      <c r="B23" s="95" t="s">
+      <c r="A23" s="72"/>
+      <c r="B23" s="71" t="s">
         <v>375</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="71" t="s">
         <v>325</v>
       </c>
-      <c r="D23" s="96" t="s">
+      <c r="D23" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E23" s="96" t="s">
+      <c r="E23" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="F23" s="96" t="s">
+      <c r="F23" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="G23" s="96" t="s">
+      <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="67" t="s">
+      <c r="H23" s="86" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="68"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="47" t="s">
         <v>349</v>
       </c>
@@ -7919,12 +7926,12 @@
       <c r="G24" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="H24" s="68"/>
+      <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="69"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7937,421 +7944,413 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="69"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="86" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="67" t="s">
+      <c r="B26" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="70"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="73"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="68"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="70"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="74"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="92"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="68"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="91" t="s">
+      <c r="A28" s="72"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="92"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="74"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="92"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="68"/>
-      <c r="B29" s="95" t="s">
+      <c r="A29" s="72"/>
+      <c r="B29" s="71" t="s">
         <v>299</v>
       </c>
-      <c r="C29" s="95" t="s">
+      <c r="C29" s="71" t="s">
         <v>299</v>
       </c>
-      <c r="D29" s="96" t="s">
+      <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="97" t="s">
+      <c r="E29" s="74" t="s">
         <v>474</v>
       </c>
-      <c r="F29" s="98"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="95" t="s">
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="68"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="75" t="s">
+      <c r="E30" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="76"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="68"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="87" t="s">
+      <c r="A31" s="72"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="88" t="s">
+      <c r="E31" s="96" t="s">
         <v>476</v>
       </c>
-      <c r="F31" s="89"/>
-      <c r="G31" s="90"/>
-      <c r="H31" s="86"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="87"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="68"/>
-      <c r="B32" s="68" t="s">
+      <c r="A32" s="72"/>
+      <c r="B32" s="72" t="s">
         <v>357</v>
       </c>
-      <c r="C32" s="68" t="s">
+      <c r="C32" s="72" t="s">
         <v>330</v>
       </c>
-      <c r="D32" s="82" t="s">
+      <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="83" t="s">
+      <c r="E32" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="84"/>
-      <c r="G32" s="85"/>
-      <c r="H32" s="68" t="s">
+      <c r="F32" s="100"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="68"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
+      <c r="A33" s="72"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="75" t="s">
+      <c r="E33" s="77" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="76"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="68"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="68"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="91" t="s">
+      <c r="A34" s="72"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="100" t="s">
+      <c r="E34" s="83" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="101"/>
-      <c r="G34" s="102"/>
-      <c r="H34" s="68"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="68"/>
-      <c r="B35" s="95" t="s">
+      <c r="A35" s="72"/>
+      <c r="B35" s="71" t="s">
         <v>359</v>
       </c>
-      <c r="C35" s="95" t="s">
+      <c r="C35" s="71" t="s">
         <v>318</v>
       </c>
-      <c r="D35" s="96" t="s">
+      <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="97" t="s">
+      <c r="E35" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="98"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="95" t="s">
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="68"/>
-      <c r="B36" s="68"/>
-      <c r="C36" s="68"/>
+      <c r="A36" s="72"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="75" t="s">
+      <c r="E36" s="77" t="s">
         <v>475</v>
       </c>
-      <c r="F36" s="76"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="68"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="68"/>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="91" t="s">
+      <c r="A37" s="72"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="100" t="s">
+      <c r="E37" s="83" t="s">
         <v>477</v>
       </c>
-      <c r="F37" s="101"/>
-      <c r="G37" s="102"/>
-      <c r="H37" s="68"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
+      <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="68"/>
-      <c r="B38" s="95" t="s">
+      <c r="A38" s="72"/>
+      <c r="B38" s="71" t="s">
         <v>364</v>
       </c>
-      <c r="C38" s="95" t="s">
+      <c r="C38" s="71" t="s">
         <v>287</v>
       </c>
-      <c r="D38" s="96" t="s">
+      <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="97" t="s">
+      <c r="E38" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="98"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="95" t="s">
+      <c r="F38" s="75"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="68"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="68"/>
+      <c r="A39" s="72"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="75" t="s">
+      <c r="E39" s="77" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="76"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="68"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="68"/>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="91" t="s">
+      <c r="A40" s="72"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="100" t="s">
+      <c r="E40" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="101"/>
-      <c r="G40" s="102"/>
-      <c r="H40" s="68"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
+      <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="68"/>
-      <c r="B41" s="95" t="s">
+      <c r="A41" s="72"/>
+      <c r="B41" s="71" t="s">
         <v>365</v>
       </c>
-      <c r="C41" s="95" t="s">
+      <c r="C41" s="71" t="s">
         <v>322</v>
       </c>
-      <c r="D41" s="96" t="s">
+      <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="97" t="s">
+      <c r="E41" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="98"/>
-      <c r="G41" s="99"/>
-      <c r="H41" s="95" t="s">
+      <c r="F41" s="75"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="68"/>
-      <c r="B42" s="68"/>
-      <c r="C42" s="68"/>
+      <c r="A42" s="72"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="75" t="s">
+      <c r="E42" s="77" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="76"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="68"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="79"/>
+      <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="68"/>
-      <c r="B43" s="68"/>
-      <c r="C43" s="68"/>
-      <c r="D43" s="91" t="s">
+      <c r="A43" s="72"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="100" t="s">
+      <c r="E43" s="83" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="101"/>
-      <c r="G43" s="102"/>
-      <c r="H43" s="68"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="68"/>
-      <c r="B44" s="95" t="s">
+      <c r="A44" s="72"/>
+      <c r="B44" s="71" t="s">
         <v>368</v>
       </c>
-      <c r="C44" s="95" t="s">
+      <c r="C44" s="71" t="s">
         <v>316</v>
       </c>
-      <c r="D44" s="96" t="s">
+      <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="97" t="s">
+      <c r="E44" s="74" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="98"/>
-      <c r="G44" s="99"/>
-      <c r="H44" s="95" t="s">
+      <c r="F44" s="75"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="68"/>
-      <c r="B45" s="68"/>
-      <c r="C45" s="68"/>
+      <c r="A45" s="72"/>
+      <c r="B45" s="72"/>
+      <c r="C45" s="72"/>
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="75" t="s">
+      <c r="E45" s="77" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="76"/>
-      <c r="G45" s="77"/>
-      <c r="H45" s="68"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
+      <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="68"/>
-      <c r="B46" s="68"/>
-      <c r="C46" s="68"/>
-      <c r="D46" s="91" t="s">
+      <c r="A46" s="72"/>
+      <c r="B46" s="72"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="100" t="s">
+      <c r="E46" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="101"/>
-      <c r="G46" s="102"/>
-      <c r="H46" s="68"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="85"/>
+      <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="68"/>
-      <c r="B47" s="95" t="s">
+      <c r="A47" s="72"/>
+      <c r="B47" s="71" t="s">
         <v>375</v>
       </c>
-      <c r="C47" s="95" t="s">
+      <c r="C47" s="71" t="s">
         <v>325</v>
       </c>
-      <c r="D47" s="96" t="s">
+      <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="97" t="s">
+      <c r="E47" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="98"/>
-      <c r="G47" s="99"/>
-      <c r="H47" s="95" t="s">
+      <c r="F47" s="75"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="68"/>
-      <c r="B48" s="68"/>
-      <c r="C48" s="68"/>
+      <c r="A48" s="72"/>
+      <c r="B48" s="72"/>
+      <c r="C48" s="72"/>
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="75" t="s">
+      <c r="E48" s="77" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="76"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="68"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="79"/>
+      <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="69"/>
-      <c r="B49" s="69"/>
-      <c r="C49" s="69"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="78" t="s">
+      <c r="E49" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="79"/>
-      <c r="G49" s="80"/>
-      <c r="H49" s="69"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8368,31 +8367,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8880,7 +8887,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8890,24 +8897,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="102" t="s">
         <v>457</v>
       </c>
-      <c r="B1" s="81"/>
+      <c r="B1" s="102"/>
       <c r="C1" s="52"/>
       <c r="D1" s="52"/>
       <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="81"/>
-      <c r="B2" s="81"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
       <c r="C2" s="52"/>
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
-      <c r="B3" s="81"/>
+      <c r="A3" s="102"/>
+      <c r="B3" s="102"/>
       <c r="C3" s="52"/>
       <c r="D3" s="52"/>
       <c r="E3" s="52"/>
@@ -8917,6 +8924,9 @@
       <c r="B4" s="53"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>478</v>
+      </c>
       <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -9028,7 +9038,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
@@ -10182,16 +10192,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
@@ -10611,7 +10621,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>479</v>
       </c>
       <c r="B6">
         <v>23</v>
@@ -10619,8 +10629,8 @@
       <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="D6">
-        <v>17000</v>
+      <c r="D6" t="s">
+        <v>76</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
@@ -10632,34 +10642,34 @@
         <v>115</v>
       </c>
       <c r="H6">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="I6">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J6">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K6">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="L6">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="M6">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="N6">
+        <v>13</v>
+      </c>
+      <c r="O6">
+        <v>20</v>
+      </c>
+      <c r="P6">
         <v>9</v>
       </c>
-      <c r="O6">
-        <v>11</v>
-      </c>
-      <c r="P6">
-        <v>6</v>
-      </c>
       <c r="Q6">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -10674,32 +10684,32 @@
         <v>7</v>
       </c>
       <c r="V6" t="s">
-        <v>12</v>
-      </c>
-      <c r="W6" s="10">
-        <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V6,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>31</v>
-      </c>
-      <c r="X6" s="10">
-        <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V6,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="W6" s="103" cm="1">
+        <f t="array" aca="1" ref="W6" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
+        <v>33</v>
+      </c>
+      <c r="X6" s="103" cm="1">
+        <f t="array" aca="1" ref="X6" ca="1">INDEX(Caliber!C2:'Caliber'!D11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B2:'Caliber'!B11,0),2)</f>
+        <v>0.4</v>
       </c>
       <c r="Y6" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>90</v>
       </c>
       <c r="D7">
-        <v>15000</v>
+        <v>17000</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -10714,31 +10724,31 @@
         <v>25</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J7">
         <v>35</v>
       </c>
       <c r="K7">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="L7">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="M7">
         <v>40</v>
       </c>
       <c r="N7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P7">
         <v>6</v>
       </c>
       <c r="Q7">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -10755,30 +10765,30 @@
       <c r="V7" t="s">
         <v>12</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="10">
         <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V7,Caliber!B2:'Caliber'!B9,0),2)</f>
         <v>31</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="10">
         <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V7,Caliber!B2:'Caliber'!B9,0),2)</f>
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>464</v>
+        <v>106</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="D8">
-        <v>20000</v>
+        <v>15000</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -10796,10 +10806,10 @@
         <v>20</v>
       </c>
       <c r="J8">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="K8">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L8">
         <v>70</v>
@@ -10808,13 +10818,13 @@
         <v>40</v>
       </c>
       <c r="N8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q8">
         <v>30</v>
@@ -10832,71 +10842,71 @@
         <v>7</v>
       </c>
       <c r="V8" t="s">
-        <v>461</v>
-      </c>
-      <c r="W8" s="10" cm="1">
-        <f t="array" aca="1" ref="W8" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
-        <v>30</v>
-      </c>
-      <c r="X8" s="10" cm="1">
-        <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!C2:'Caliber'!D11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B2:'Caliber'!B11,0),2)</f>
-        <v>0.35</v>
+        <v>12</v>
+      </c>
+      <c r="W8">
+        <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V8,Caliber!B2:'Caliber'!B9,0),2)</f>
+        <v>31</v>
+      </c>
+      <c r="X8">
+        <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V8,Caliber!B2:'Caliber'!B9,0),2)</f>
+        <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>462</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>464</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>75</v>
       </c>
       <c r="D9">
-        <v>23000</v>
+        <v>20000</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="G9">
         <v>115</v>
       </c>
       <c r="H9">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I9">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J9">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="K9">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L9">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="M9">
         <v>40</v>
       </c>
       <c r="N9">
+        <v>11</v>
+      </c>
+      <c r="O9">
+        <v>13</v>
+      </c>
+      <c r="P9">
         <v>8</v>
       </c>
-      <c r="O9">
-        <v>10</v>
-      </c>
-      <c r="P9">
-        <v>5</v>
-      </c>
       <c r="Q9">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -10911,32 +10921,32 @@
         <v>7</v>
       </c>
       <c r="V9" t="s">
-        <v>16</v>
-      </c>
-      <c r="W9">
-        <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V9,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>34</v>
-      </c>
-      <c r="X9">
-        <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V9,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>0.4</v>
+        <v>461</v>
+      </c>
+      <c r="W9" s="10" cm="1">
+        <f t="array" aca="1" ref="W9" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
+        <v>30</v>
+      </c>
+      <c r="X9" s="10" cm="1">
+        <f t="array" aca="1" ref="X9" ca="1">INDEX(Caliber!C2:'Caliber'!D11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B2:'Caliber'!B11,0),2)</f>
+        <v>0.35</v>
       </c>
       <c r="Y9" t="s">
-        <v>119</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B10">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>75</v>
       </c>
       <c r="D10">
-        <v>14000</v>
+        <v>23000</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -10948,34 +10958,34 @@
         <v>115</v>
       </c>
       <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10">
         <v>25</v>
       </c>
-      <c r="I10">
-        <v>20</v>
-      </c>
       <c r="J10">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K10">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L10">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="M10">
         <v>40</v>
       </c>
       <c r="N10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O10">
         <v>10</v>
       </c>
       <c r="P10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q10">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -10990,32 +11000,32 @@
         <v>7</v>
       </c>
       <c r="V10" t="s">
-        <v>12</v>
-      </c>
-      <c r="W10" s="10">
+        <v>16</v>
+      </c>
+      <c r="W10">
         <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V10,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>31</v>
-      </c>
-      <c r="X10" s="10">
+        <v>34</v>
+      </c>
+      <c r="X10">
         <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V10,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="Y10" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>75</v>
       </c>
-      <c r="D11" t="s">
-        <v>76</v>
+      <c r="D11">
+        <v>14000</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -11027,25 +11037,25 @@
         <v>115</v>
       </c>
       <c r="H11">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11">
         <v>30</v>
       </c>
-      <c r="J11">
+      <c r="K11">
+        <v>45</v>
+      </c>
+      <c r="L11">
+        <v>55</v>
+      </c>
+      <c r="M11">
         <v>40</v>
       </c>
-      <c r="K11">
-        <v>50</v>
-      </c>
-      <c r="L11">
-        <v>60</v>
-      </c>
-      <c r="M11">
-        <v>35</v>
-      </c>
       <c r="N11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O11">
         <v>10</v>
@@ -11069,47 +11079,47 @@
         <v>7</v>
       </c>
       <c r="V11" t="s">
-        <v>95</v>
-      </c>
-      <c r="W11">
+        <v>12</v>
+      </c>
+      <c r="W11" s="10">
         <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V11,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>29</v>
-      </c>
-      <c r="X11">
+        <v>31</v>
+      </c>
+      <c r="X11" s="10">
         <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V11,Caliber!B2:'Caliber'!B9,0),2)</f>
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12">
-        <v>19000</v>
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G12">
         <v>115</v>
       </c>
       <c r="H12">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I12">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J12">
         <v>40</v>
@@ -11118,22 +11128,22 @@
         <v>50</v>
       </c>
       <c r="L12">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="M12">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N12">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O12">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="P12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Q12">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -11148,32 +11158,32 @@
         <v>7</v>
       </c>
       <c r="V12" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="W12">
         <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V12,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="X12">
         <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V12,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B13">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>76</v>
+        <v>90</v>
+      </c>
+      <c r="D13">
+        <v>19000</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -11185,34 +11195,34 @@
         <v>115</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I13">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J13">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="K13">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="L13">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M13">
         <v>30</v>
       </c>
       <c r="N13">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="O13">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q13">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -11227,32 +11237,32 @@
         <v>7</v>
       </c>
       <c r="V13" t="s">
-        <v>12</v>
-      </c>
-      <c r="W13" s="10">
+        <v>14</v>
+      </c>
+      <c r="W13">
         <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V13,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>31</v>
-      </c>
-      <c r="X13" s="10">
+        <v>35</v>
+      </c>
+      <c r="X13">
         <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V13,Caliber!B2:'Caliber'!B9,0),2)</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Y13" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>449</v>
+        <v>104</v>
       </c>
       <c r="B14">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14">
-        <v>25000</v>
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -11264,31 +11274,31 @@
         <v>115</v>
       </c>
       <c r="H14">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I14">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J14">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="K14">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="L14">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="M14">
         <v>30</v>
       </c>
       <c r="N14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O14">
         <v>10</v>
       </c>
       <c r="P14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q14">
         <v>20</v>
@@ -11297,13 +11307,13 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T14">
         <v>1</v>
       </c>
       <c r="U14">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="V14" t="s">
         <v>12</v>
@@ -11317,6 +11327,85 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>449</v>
+      </c>
+      <c r="B15">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15">
+        <v>25000</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>80</v>
+      </c>
+      <c r="G15">
+        <v>115</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+      <c r="J15">
+        <v>25</v>
+      </c>
+      <c r="K15">
+        <v>30</v>
+      </c>
+      <c r="L15">
+        <v>50</v>
+      </c>
+      <c r="M15">
+        <v>30</v>
+      </c>
+      <c r="N15">
+        <v>8</v>
+      </c>
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <v>20</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>10</v>
+      </c>
+      <c r="V15" t="s">
+        <v>12</v>
+      </c>
+      <c r="W15" s="10">
+        <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V15,Caliber!B2:'Caliber'!B9,0),2)</f>
+        <v>31</v>
+      </c>
+      <c r="X15" s="10">
+        <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V15,Caliber!B2:'Caliber'!B9,0),2)</f>
+        <v>0</v>
+      </c>
+      <c r="Y15" t="s">
         <v>450</v>
       </c>
     </row>
@@ -11333,10 +11422,10 @@
   <dimension ref="A1:AA53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N39" sqref="N39"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A31:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Lots of bug fixes, moved versek to private contract
Fixed some items not being obtained when researching them, fixed starting with 4.6x30mm rounds, fixed incorrect naming of some Private Contract researches. Moved versek to private smg contract. Updated tech tree drawio file. Fixed Vityaz sprite id.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34AC1F6-CE38-4C01-9CA6-F91FDF247CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CCCC03-E05D-4406-9A95-9AA362534C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="7" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="2" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="479">
   <si>
     <t>Name</t>
   </si>
@@ -1619,6 +1619,9 @@
   </si>
   <si>
     <t>P90 (Sopmod)</t>
+  </si>
+  <si>
+    <t>Prison cell sprite</t>
   </si>
 </sst>
 </file>
@@ -8879,8 +8882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8913,7 +8916,9 @@
       <c r="E3" s="52"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>478</v>
+      </c>
       <c r="B4" s="53"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -10181,9 +10186,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10462,7 +10467,7 @@
         <v>17500</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>100</v>
@@ -11409,7 +11414,7 @@
   <dimension ref="A1:AA53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A34" sqref="A31:XFD34"/>

</xml_diff>

<commit_message>
Lots of bugfixes, and some small changes
Moved vektor acquisition to private contract, Also fixed vityaz sprite hand/floor ids. fixed issue in spreadsheet with p226's snap cost. Fixed 38 special and 9mm gyurza not being purchasable. GM-94 ufopaedia only showing up with research fixed. Fixed clipping through wall on DAWNURBAN10.MAP and DAWNURBAN13.MAP.
Enemies now give points for capture (kill points +10).
Mission markers now display the mission name.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CCCC03-E05D-4406-9A95-9AA362534C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ED4794-3141-4109-9D54-16B336904B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="2" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="7" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="481">
   <si>
     <t>Name</t>
   </si>
@@ -1622,6 +1622,12 @@
   </si>
   <si>
     <t>Prison cell sprite</t>
+  </si>
+  <si>
+    <t>Uniform w/ NVGs &amp; Adv. NVGs</t>
+  </si>
+  <si>
+    <t>RPG-7 hand sprite fix</t>
   </si>
 </sst>
 </file>
@@ -8882,8 +8888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8922,9 +8928,15 @@
       <c r="B4" s="53"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>479</v>
+      </c>
       <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>480</v>
+      </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -9030,8 +9042,8 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T16" sqref="T16"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9884,7 +9896,7 @@
         <v>45</v>
       </c>
       <c r="I11">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J11">
         <v>50</v>
@@ -10186,9 +10198,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed capitalization in breaching tool researches
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ED4794-3141-4109-9D54-16B336904B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B47498B-0870-4824-A0AE-744A4C6BB907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="7" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="1" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="482">
   <si>
     <t>Name</t>
   </si>
@@ -1628,6 +1628,9 @@
   </si>
   <si>
     <t>RPG-7 hand sprite fix</t>
+  </si>
+  <si>
+    <t>Quick weapon attachment researches when you get a weapon that can use them (ie get m4 from enemy + have sopmod unlocked -&gt; research -&gt; can apply sopmod despite not doing m4 acquisition).</t>
   </si>
 </sst>
 </file>
@@ -2338,13 +2341,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2371,24 +2410,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2405,24 +2426,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7467,13 +7470,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="86" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7488,7 +7491,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="86" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7572,8 +7575,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7586,7 +7589,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7632,8 +7635,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7646,7 +7649,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="73"/>
+      <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7752,8 +7755,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7766,7 +7769,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="73"/>
+      <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7812,8 +7815,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7826,7 +7829,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="73"/>
+      <c r="H19" s="87"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7886,7 +7889,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="75"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7908,7 +7911,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="74" t="s">
+      <c r="H23" s="86" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7931,9 +7934,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7946,25 +7949,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="75"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="86" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="76"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7973,10 +7976,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="80"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="92"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7985,10 +7988,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="80"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="92"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8001,11 +8004,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="84" t="s">
+      <c r="E29" s="74" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8017,26 +8020,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="90" t="s">
+      <c r="E31" s="96" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="91"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="73"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="87"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8049,11 +8052,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="93" t="s">
+      <c r="E32" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="94"/>
-      <c r="G32" s="95"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="101"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8065,11 +8068,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="87" t="s">
+      <c r="E33" s="77" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8079,11 +8082,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="96" t="s">
+      <c r="E34" s="83" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="97"/>
-      <c r="G34" s="98"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="85"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8097,11 +8100,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="84" t="s">
+      <c r="E35" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="85"/>
-      <c r="G35" s="86"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8113,11 +8116,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="87" t="s">
+      <c r="E36" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="79"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8127,11 +8130,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="83" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="97"/>
-      <c r="G37" s="98"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8145,11 +8148,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="84" t="s">
+      <c r="E38" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="85"/>
-      <c r="G38" s="86"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="76"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8161,11 +8164,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="87" t="s">
+      <c r="E39" s="77" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8175,11 +8178,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="96" t="s">
+      <c r="E40" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="97"/>
-      <c r="G40" s="98"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8193,11 +8196,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="84" t="s">
+      <c r="E41" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="85"/>
-      <c r="G41" s="86"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="76"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8209,11 +8212,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="87" t="s">
+      <c r="E42" s="77" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="79"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8223,11 +8226,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="96" t="s">
+      <c r="E43" s="83" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="97"/>
-      <c r="G43" s="98"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="85"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8241,11 +8244,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="84" t="s">
+      <c r="E44" s="74" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="85"/>
-      <c r="G44" s="86"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="76"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8257,11 +8260,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="87" t="s">
+      <c r="E45" s="77" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="88"/>
-      <c r="G45" s="89"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8271,11 +8274,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="96" t="s">
+      <c r="E46" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="97"/>
-      <c r="G46" s="98"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="85"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8289,11 +8292,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="84" t="s">
+      <c r="E47" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="85"/>
-      <c r="G47" s="86"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="76"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8305,62 +8308,54 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="87" t="s">
+      <c r="E48" s="77" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="89"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="79"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="99" t="s">
+      <c r="E49" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="100"/>
-      <c r="G49" s="101"/>
-      <c r="H49" s="75"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8377,31 +8372,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8888,8 +8891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8946,6 +8949,9 @@
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>481</v>
+      </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -9041,8 +9047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FC119D-A7BC-46FE-BE1D-3900F19AB624}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rebalanced pistol snap costs
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B47498B-0870-4824-A0AE-744A4C6BB907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0EFFBA-8C50-47EB-B93F-2260AAD2D31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="1" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
@@ -2341,49 +2341,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2410,6 +2374,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2426,6 +2408,24 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7470,13 +7470,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="74" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7491,7 +7491,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="H2" s="74" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7575,8 +7575,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7589,7 +7589,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="87"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7635,8 +7635,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="87"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7649,7 +7649,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="87"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7755,8 +7755,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7769,7 +7769,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="87"/>
+      <c r="H16" s="73"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7815,8 +7815,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="87"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7829,7 +7829,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="87"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7889,7 +7889,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="73"/>
+      <c r="H22" s="75"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7911,7 +7911,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="86" t="s">
+      <c r="H23" s="74" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7934,9 +7934,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7949,25 +7949,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="73"/>
+      <c r="H25" s="75"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="86" t="s">
+      <c r="A26" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="88"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="91"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7976,10 +7976,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="88"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="92"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="80"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7988,10 +7988,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="93"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="92"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="80"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8004,11 +8004,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="74" t="s">
+      <c r="E29" s="84" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="86"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8020,26 +8020,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="77" t="s">
+      <c r="E30" s="87" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="89"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="96" t="s">
+      <c r="E31" s="90" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="97"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="87"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="73"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8052,11 +8052,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="99" t="s">
+      <c r="E32" s="93" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="100"/>
-      <c r="G32" s="101"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="95"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8068,11 +8068,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="77" t="s">
+      <c r="E33" s="87" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8082,11 +8082,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="83" t="s">
+      <c r="E34" s="96" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="84"/>
-      <c r="G34" s="85"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8100,11 +8100,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="74" t="s">
+      <c r="E35" s="84" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="86"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8116,11 +8116,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="77" t="s">
+      <c r="E36" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="78"/>
-      <c r="G36" s="79"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="89"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8130,11 +8130,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="83" t="s">
+      <c r="E37" s="96" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
+      <c r="F37" s="97"/>
+      <c r="G37" s="98"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8148,11 +8148,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="74" t="s">
+      <c r="E38" s="84" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="75"/>
-      <c r="G38" s="76"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="86"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8164,11 +8164,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="77" t="s">
+      <c r="E39" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="78"/>
-      <c r="G39" s="79"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="89"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8178,11 +8178,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="83" t="s">
+      <c r="E40" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="84"/>
-      <c r="G40" s="85"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="98"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8196,11 +8196,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="74" t="s">
+      <c r="E41" s="84" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="75"/>
-      <c r="G41" s="76"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="86"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8212,11 +8212,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="77" t="s">
+      <c r="E42" s="87" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="78"/>
-      <c r="G42" s="79"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="89"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8226,11 +8226,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="83" t="s">
+      <c r="E43" s="96" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="84"/>
-      <c r="G43" s="85"/>
+      <c r="F43" s="97"/>
+      <c r="G43" s="98"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8244,11 +8244,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="74" t="s">
+      <c r="E44" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="75"/>
-      <c r="G44" s="76"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="86"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8260,11 +8260,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="77" t="s">
+      <c r="E45" s="87" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="78"/>
-      <c r="G45" s="79"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="89"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8274,11 +8274,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="83" t="s">
+      <c r="E46" s="96" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="84"/>
-      <c r="G46" s="85"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="98"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8292,11 +8292,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="74" t="s">
+      <c r="E47" s="84" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="75"/>
-      <c r="G47" s="76"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="86"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8308,38 +8308,78 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="77" t="s">
+      <c r="E48" s="87" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="78"/>
-      <c r="G48" s="79"/>
+      <c r="F48" s="88"/>
+      <c r="G48" s="89"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
+      <c r="A49" s="75"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="80" t="s">
+      <c r="E49" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="81"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="73"/>
+      <c r="F49" s="100"/>
+      <c r="G49" s="101"/>
+      <c r="H49" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8356,55 +8396,15 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9048,8 +9048,8 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J14" sqref="J14"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9507,7 +9507,7 @@
         <v>50</v>
       </c>
       <c r="I6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J6">
         <v>50</v>
@@ -9586,7 +9586,7 @@
         <v>50</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J7">
         <v>60</v>
@@ -9665,7 +9665,7 @@
         <v>50</v>
       </c>
       <c r="I8">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J8">
         <v>65</v>
@@ -9902,7 +9902,7 @@
         <v>45</v>
       </c>
       <c r="I11">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J11">
         <v>50</v>
@@ -10139,7 +10139,7 @@
         <v>40</v>
       </c>
       <c r="I14">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="J14">
         <v>45</v>

</xml_diff>

<commit_message>
more bugfixes, underbarrel weapons now show their stats on the ufopaedia page for a weapon
Spreadsheet fixes, fixed breaching hammer capitalization, fixed ufopaedia pages for serbu and m16a2 m203& scoped, fixed 5_45 ammo not unlocking w/ rpk, fixed HK416 MASS & M320 aimed shot not matching base HK416. Added 2nd pages in ufopaedia for weapons with underbarreled attachments
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0EFFBA-8C50-47EB-B93F-2260AAD2D31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5554D76-2549-4EAB-83AA-4D6494DFD7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="1" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="3" activeTab="3" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="483">
   <si>
     <t>Name</t>
   </si>
@@ -1631,6 +1631,9 @@
   </si>
   <si>
     <t>Quick weapon attachment researches when you get a weapon that can use them (ie get m4 from enemy + have sopmod unlocked -&gt; research -&gt; can apply sopmod despite not doing m4 acquisition).</t>
+  </si>
+  <si>
+    <t>add manufacturing to swap out NVGs for adv. NVGs on armor</t>
   </si>
 </sst>
 </file>
@@ -2341,13 +2344,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2374,24 +2413,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2408,24 +2429,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7470,13 +7473,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="86" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7491,7 +7494,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="86" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7575,8 +7578,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7589,7 +7592,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7635,8 +7638,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7649,7 +7652,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="73"/>
+      <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7755,8 +7758,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7769,7 +7772,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="73"/>
+      <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7815,8 +7818,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7829,7 +7832,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="73"/>
+      <c r="H19" s="87"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7889,7 +7892,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="75"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7911,7 +7914,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="74" t="s">
+      <c r="H23" s="86" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7934,9 +7937,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7949,25 +7952,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="75"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="86" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="76"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7976,10 +7979,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="80"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="92"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7988,10 +7991,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="80"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="92"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8004,11 +8007,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="84" t="s">
+      <c r="E29" s="74" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8020,26 +8023,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="90" t="s">
+      <c r="E31" s="96" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="91"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="73"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="87"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8052,11 +8055,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="93" t="s">
+      <c r="E32" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="94"/>
-      <c r="G32" s="95"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="101"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8068,11 +8071,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="87" t="s">
+      <c r="E33" s="77" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8082,11 +8085,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="96" t="s">
+      <c r="E34" s="83" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="97"/>
-      <c r="G34" s="98"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="85"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8100,11 +8103,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="84" t="s">
+      <c r="E35" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="85"/>
-      <c r="G35" s="86"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8116,11 +8119,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="87" t="s">
+      <c r="E36" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="79"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8130,11 +8133,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="83" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="97"/>
-      <c r="G37" s="98"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8148,11 +8151,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="84" t="s">
+      <c r="E38" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="85"/>
-      <c r="G38" s="86"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="76"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8164,11 +8167,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="87" t="s">
+      <c r="E39" s="77" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8178,11 +8181,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="96" t="s">
+      <c r="E40" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="97"/>
-      <c r="G40" s="98"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8196,11 +8199,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="84" t="s">
+      <c r="E41" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="85"/>
-      <c r="G41" s="86"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="76"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8212,11 +8215,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="87" t="s">
+      <c r="E42" s="77" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="79"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8226,11 +8229,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="96" t="s">
+      <c r="E43" s="83" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="97"/>
-      <c r="G43" s="98"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="85"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8244,11 +8247,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="84" t="s">
+      <c r="E44" s="74" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="85"/>
-      <c r="G44" s="86"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="76"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8260,11 +8263,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="87" t="s">
+      <c r="E45" s="77" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="88"/>
-      <c r="G45" s="89"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8274,11 +8277,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="96" t="s">
+      <c r="E46" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="97"/>
-      <c r="G46" s="98"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="85"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8292,11 +8295,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="84" t="s">
+      <c r="E47" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="85"/>
-      <c r="G47" s="86"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="76"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8308,62 +8311,54 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="87" t="s">
+      <c r="E48" s="77" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="89"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="79"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="99" t="s">
+      <c r="E49" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="100"/>
-      <c r="G49" s="101"/>
-      <c r="H49" s="75"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8380,31 +8375,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8892,7 +8895,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8955,6 +8958,9 @@
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>482</v>
+      </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -9047,7 +9053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FC119D-A7BC-46FE-BE1D-3900F19AB624}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I14" sqref="I14"/>
     </sheetView>
@@ -11431,11 +11437,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E308052D-1B88-4699-843E-12AA607B59B8}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A31:XFD34"/>
+      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13138,7 +13144,7 @@
         <v>125</v>
       </c>
       <c r="I21">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="J21">
         <v>32</v>
@@ -13220,7 +13226,7 @@
         <v>125</v>
       </c>
       <c r="I22">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="J22">
         <v>32</v>

</xml_diff>

<commit_message>
Fixed infinite money glitch, nerfed versek + other changes
Fixed milkor sell price, nerfed versek, fixed gold deagle ufopaedia text
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5554D76-2549-4EAB-83AA-4D6494DFD7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68813F7-6DC7-40DE-AF4F-A025E7A03F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="3" activeTab="3" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="6" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -2344,49 +2344,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2413,6 +2377,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2429,6 +2411,24 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3597,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7428,8 +7428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7473,13 +7473,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="74" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7494,7 +7494,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="H2" s="74" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7578,8 +7578,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7592,7 +7592,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="87"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7638,8 +7638,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="87"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7652,7 +7652,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="87"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7758,8 +7758,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7772,7 +7772,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="87"/>
+      <c r="H16" s="73"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7818,8 +7818,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="87"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7832,7 +7832,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="87"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7892,7 +7892,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="73"/>
+      <c r="H22" s="75"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7914,7 +7914,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="86" t="s">
+      <c r="H23" s="74" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7937,9 +7937,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7952,25 +7952,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="73"/>
+      <c r="H25" s="75"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="86" t="s">
+      <c r="A26" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="88"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="91"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7979,10 +7979,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="88"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="92"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="80"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7991,10 +7991,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="93"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="92"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="80"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8007,11 +8007,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="74" t="s">
+      <c r="E29" s="84" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="86"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8023,26 +8023,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="77" t="s">
+      <c r="E30" s="87" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="89"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="96" t="s">
+      <c r="E31" s="90" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="97"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="87"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="73"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8055,11 +8055,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="99" t="s">
+      <c r="E32" s="93" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="100"/>
-      <c r="G32" s="101"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="95"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8071,11 +8071,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="77" t="s">
+      <c r="E33" s="87" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8085,11 +8085,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="83" t="s">
+      <c r="E34" s="96" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="84"/>
-      <c r="G34" s="85"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8103,11 +8103,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="74" t="s">
+      <c r="E35" s="84" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="86"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8119,11 +8119,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="77" t="s">
+      <c r="E36" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="78"/>
-      <c r="G36" s="79"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="89"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8133,11 +8133,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="83" t="s">
+      <c r="E37" s="96" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
+      <c r="F37" s="97"/>
+      <c r="G37" s="98"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8151,11 +8151,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="74" t="s">
+      <c r="E38" s="84" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="75"/>
-      <c r="G38" s="76"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="86"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8167,11 +8167,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="77" t="s">
+      <c r="E39" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="78"/>
-      <c r="G39" s="79"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="89"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8181,11 +8181,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="83" t="s">
+      <c r="E40" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="84"/>
-      <c r="G40" s="85"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="98"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8199,11 +8199,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="74" t="s">
+      <c r="E41" s="84" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="75"/>
-      <c r="G41" s="76"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="86"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8215,11 +8215,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="77" t="s">
+      <c r="E42" s="87" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="78"/>
-      <c r="G42" s="79"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="89"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8229,11 +8229,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="83" t="s">
+      <c r="E43" s="96" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="84"/>
-      <c r="G43" s="85"/>
+      <c r="F43" s="97"/>
+      <c r="G43" s="98"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8247,11 +8247,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="74" t="s">
+      <c r="E44" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="75"/>
-      <c r="G44" s="76"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="86"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8263,11 +8263,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="77" t="s">
+      <c r="E45" s="87" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="78"/>
-      <c r="G45" s="79"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="89"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8277,11 +8277,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="83" t="s">
+      <c r="E46" s="96" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="84"/>
-      <c r="G46" s="85"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="98"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8295,11 +8295,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="74" t="s">
+      <c r="E47" s="84" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="75"/>
-      <c r="G47" s="76"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="86"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8311,38 +8311,78 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="77" t="s">
+      <c r="E48" s="87" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="78"/>
-      <c r="G48" s="79"/>
+      <c r="F48" s="88"/>
+      <c r="G48" s="89"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
+      <c r="A49" s="75"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="80" t="s">
+      <c r="E49" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="81"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="73"/>
+      <c r="F49" s="100"/>
+      <c r="G49" s="101"/>
+      <c r="H49" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8359,55 +8399,15 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -10211,8 +10211,8 @@
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10:XFD10"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A5" activeCellId="1" sqref="A4:XFD4 A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10983,22 +10983,22 @@
         <v>35</v>
       </c>
       <c r="K10">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="L10">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M10">
         <v>40</v>
       </c>
       <c r="N10">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O10">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <v>25</v>
@@ -11437,8 +11437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E308052D-1B88-4699-843E-12AA607B59B8}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K21" sqref="K21"/>

</xml_diff>

<commit_message>
Fixed major RPG-7 sprite bugs, added unloaded floor and hand RPG-7 sprites
Also fixed minor issues with M60 sprites and Carl Gustaf sprites
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68813F7-6DC7-40DE-AF4F-A025E7A03F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836745D3-B0C1-4EF1-A028-21388FFF7633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="6" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="3" activeTab="3" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -2344,13 +2344,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2377,24 +2413,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2411,24 +2429,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7428,8 +7428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7473,13 +7473,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="86" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7494,7 +7494,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="86" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7578,8 +7578,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7592,7 +7592,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7638,8 +7638,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7652,7 +7652,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="73"/>
+      <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7758,8 +7758,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7772,7 +7772,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="73"/>
+      <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7818,8 +7818,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7832,7 +7832,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="73"/>
+      <c r="H19" s="87"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7892,7 +7892,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="75"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7914,7 +7914,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="74" t="s">
+      <c r="H23" s="86" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7937,9 +7937,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7952,25 +7952,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="75"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="86" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="76"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7979,10 +7979,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="80"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="92"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7991,10 +7991,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="80"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="92"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8007,11 +8007,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="84" t="s">
+      <c r="E29" s="74" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8023,26 +8023,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="90" t="s">
+      <c r="E31" s="96" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="91"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="73"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="87"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8055,11 +8055,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="93" t="s">
+      <c r="E32" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="94"/>
-      <c r="G32" s="95"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="101"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8071,11 +8071,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="87" t="s">
+      <c r="E33" s="77" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8085,11 +8085,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="96" t="s">
+      <c r="E34" s="83" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="97"/>
-      <c r="G34" s="98"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="85"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8103,11 +8103,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="84" t="s">
+      <c r="E35" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="85"/>
-      <c r="G35" s="86"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8119,11 +8119,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="87" t="s">
+      <c r="E36" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="79"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8133,11 +8133,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="83" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="97"/>
-      <c r="G37" s="98"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8151,11 +8151,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="84" t="s">
+      <c r="E38" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="85"/>
-      <c r="G38" s="86"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="76"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8167,11 +8167,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="87" t="s">
+      <c r="E39" s="77" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8181,11 +8181,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="96" t="s">
+      <c r="E40" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="97"/>
-      <c r="G40" s="98"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8199,11 +8199,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="84" t="s">
+      <c r="E41" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="85"/>
-      <c r="G41" s="86"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="76"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8215,11 +8215,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="87" t="s">
+      <c r="E42" s="77" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="79"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8229,11 +8229,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="96" t="s">
+      <c r="E43" s="83" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="97"/>
-      <c r="G43" s="98"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="85"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8247,11 +8247,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="84" t="s">
+      <c r="E44" s="74" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="85"/>
-      <c r="G44" s="86"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="76"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8263,11 +8263,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="87" t="s">
+      <c r="E45" s="77" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="88"/>
-      <c r="G45" s="89"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8277,11 +8277,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="96" t="s">
+      <c r="E46" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="97"/>
-      <c r="G46" s="98"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="85"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8295,11 +8295,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="84" t="s">
+      <c r="E47" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="85"/>
-      <c r="G47" s="86"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="76"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8311,62 +8311,54 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="87" t="s">
+      <c r="E48" s="77" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="89"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="79"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="99" t="s">
+      <c r="E49" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="100"/>
-      <c r="G49" s="101"/>
-      <c r="H49" s="75"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8383,31 +8375,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11437,11 +11437,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E308052D-1B88-4699-843E-12AA607B59B8}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed issues on plane map
Windows on main floor can no longer be walked through, hole on left side under plane patched, patched visibility through right side panels on front of plane. 3rd floor now accessible. Fixed doors on plane facing wrong direction, open doors on 3rd floor now can be shot
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836745D3-B0C1-4EF1-A028-21388FFF7633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6451AE-E063-4A84-B211-5377C837D8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="3" activeTab="3" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="7" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="482">
   <si>
     <t>Name</t>
   </si>
@@ -1625,9 +1625,6 @@
   </si>
   <si>
     <t>Uniform w/ NVGs &amp; Adv. NVGs</t>
-  </si>
-  <si>
-    <t>RPG-7 hand sprite fix</t>
   </si>
   <si>
     <t>Quick weapon attachment researches when you get a weapon that can use them (ie get m4 from enemy + have sopmod unlocked -&gt; research -&gt; can apply sopmod despite not doing m4 acquisition).</t>
@@ -2344,49 +2341,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2413,6 +2374,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2429,6 +2408,24 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7473,13 +7470,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="74" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7494,7 +7491,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="H2" s="74" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7578,8 +7575,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7592,7 +7589,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="87"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7638,8 +7635,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="87"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7652,7 +7649,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="87"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7758,8 +7755,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7772,7 +7769,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="87"/>
+      <c r="H16" s="73"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7818,8 +7815,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="87"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7832,7 +7829,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="87"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7892,7 +7889,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="73"/>
+      <c r="H22" s="75"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7914,7 +7911,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="86" t="s">
+      <c r="H23" s="74" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7937,9 +7934,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7952,25 +7949,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="73"/>
+      <c r="H25" s="75"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="86" t="s">
+      <c r="A26" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="88"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="91"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7979,10 +7976,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="88"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="92"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="80"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7991,10 +7988,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="93"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="92"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="80"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8007,11 +8004,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="74" t="s">
+      <c r="E29" s="84" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="86"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8023,26 +8020,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="77" t="s">
+      <c r="E30" s="87" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="89"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="96" t="s">
+      <c r="E31" s="90" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="97"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="87"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="73"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8055,11 +8052,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="99" t="s">
+      <c r="E32" s="93" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="100"/>
-      <c r="G32" s="101"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="95"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8071,11 +8068,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="77" t="s">
+      <c r="E33" s="87" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8085,11 +8082,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="83" t="s">
+      <c r="E34" s="96" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="84"/>
-      <c r="G34" s="85"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8103,11 +8100,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="74" t="s">
+      <c r="E35" s="84" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="86"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8119,11 +8116,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="77" t="s">
+      <c r="E36" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="78"/>
-      <c r="G36" s="79"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="89"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8133,11 +8130,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="83" t="s">
+      <c r="E37" s="96" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
+      <c r="F37" s="97"/>
+      <c r="G37" s="98"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8151,11 +8148,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="74" t="s">
+      <c r="E38" s="84" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="75"/>
-      <c r="G38" s="76"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="86"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8167,11 +8164,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="77" t="s">
+      <c r="E39" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="78"/>
-      <c r="G39" s="79"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="89"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8181,11 +8178,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="83" t="s">
+      <c r="E40" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="84"/>
-      <c r="G40" s="85"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="98"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8199,11 +8196,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="74" t="s">
+      <c r="E41" s="84" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="75"/>
-      <c r="G41" s="76"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="86"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8215,11 +8212,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="77" t="s">
+      <c r="E42" s="87" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="78"/>
-      <c r="G42" s="79"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="89"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8229,11 +8226,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="83" t="s">
+      <c r="E43" s="96" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="84"/>
-      <c r="G43" s="85"/>
+      <c r="F43" s="97"/>
+      <c r="G43" s="98"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8247,11 +8244,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="74" t="s">
+      <c r="E44" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="75"/>
-      <c r="G44" s="76"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="86"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8263,11 +8260,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="77" t="s">
+      <c r="E45" s="87" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="78"/>
-      <c r="G45" s="79"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="89"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8277,11 +8274,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="83" t="s">
+      <c r="E46" s="96" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="84"/>
-      <c r="G46" s="85"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="98"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8295,11 +8292,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="74" t="s">
+      <c r="E47" s="84" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="75"/>
-      <c r="G47" s="76"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="86"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8311,38 +8308,78 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="77" t="s">
+      <c r="E48" s="87" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="78"/>
-      <c r="G48" s="79"/>
+      <c r="F48" s="88"/>
+      <c r="G48" s="89"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
+      <c r="A49" s="75"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="80" t="s">
+      <c r="E49" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="81"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="73"/>
+      <c r="F49" s="100"/>
+      <c r="G49" s="101"/>
+      <c r="H49" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8359,55 +8396,15 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8894,8 +8891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8940,9 +8937,6 @@
       <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>480</v>
-      </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -8953,13 +8947,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B9" s="14"/>
     </row>
@@ -11437,7 +11431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E308052D-1B88-4699-843E-12AA607B59B8}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Fixed one way staircase in skyscraper map
there was also a minor issue where some floor tiles were missing causing a pathfinding issue
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6451AE-E063-4A84-B211-5377C837D8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBA5C65-D374-496D-8FC3-132989EFA4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="7" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -2341,13 +2341,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2374,24 +2410,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2408,24 +2426,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7470,13 +7470,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="86" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7491,7 +7491,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="86" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7575,8 +7575,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7589,7 +7589,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7635,8 +7635,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7649,7 +7649,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="73"/>
+      <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7755,8 +7755,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7769,7 +7769,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="73"/>
+      <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7815,8 +7815,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7829,7 +7829,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="73"/>
+      <c r="H19" s="87"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7889,7 +7889,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="75"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7911,7 +7911,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="74" t="s">
+      <c r="H23" s="86" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7934,9 +7934,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7949,25 +7949,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="75"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="86" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="76"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7976,10 +7976,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="80"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="92"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7988,10 +7988,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="80"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="92"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8004,11 +8004,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="84" t="s">
+      <c r="E29" s="74" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8020,26 +8020,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="90" t="s">
+      <c r="E31" s="96" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="91"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="73"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="87"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8052,11 +8052,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="93" t="s">
+      <c r="E32" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="94"/>
-      <c r="G32" s="95"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="101"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8068,11 +8068,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="87" t="s">
+      <c r="E33" s="77" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8082,11 +8082,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="96" t="s">
+      <c r="E34" s="83" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="97"/>
-      <c r="G34" s="98"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="85"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8100,11 +8100,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="84" t="s">
+      <c r="E35" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="85"/>
-      <c r="G35" s="86"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8116,11 +8116,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="87" t="s">
+      <c r="E36" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="79"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8130,11 +8130,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="83" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="97"/>
-      <c r="G37" s="98"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8148,11 +8148,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="84" t="s">
+      <c r="E38" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="85"/>
-      <c r="G38" s="86"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="76"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8164,11 +8164,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="87" t="s">
+      <c r="E39" s="77" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8178,11 +8178,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="96" t="s">
+      <c r="E40" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="97"/>
-      <c r="G40" s="98"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8196,11 +8196,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="84" t="s">
+      <c r="E41" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="85"/>
-      <c r="G41" s="86"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="76"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8212,11 +8212,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="87" t="s">
+      <c r="E42" s="77" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="79"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8226,11 +8226,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="96" t="s">
+      <c r="E43" s="83" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="97"/>
-      <c r="G43" s="98"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="85"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8244,11 +8244,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="84" t="s">
+      <c r="E44" s="74" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="85"/>
-      <c r="G44" s="86"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="76"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8260,11 +8260,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="87" t="s">
+      <c r="E45" s="77" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="88"/>
-      <c r="G45" s="89"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8274,11 +8274,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="96" t="s">
+      <c r="E46" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="97"/>
-      <c r="G46" s="98"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="85"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8292,11 +8292,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="84" t="s">
+      <c r="E47" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="85"/>
-      <c r="G47" s="86"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="76"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8308,62 +8308,54 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="87" t="s">
+      <c r="E48" s="77" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="89"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="79"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="99" t="s">
+      <c r="E49" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="100"/>
-      <c r="G49" s="101"/>
-      <c r="H49" s="75"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8380,31 +8372,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8891,7 +8891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -9047,9 +9047,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FC119D-A7BC-46FE-BE1D-3900F19AB624}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
G11 buffs, Inc shotgun shell buff
Buffed G11 giving 3 shot snap shot and more aimed accuracy, incendiary shotgun shells had a damage increase to match normal shells.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBA5C65-D374-496D-8FC3-132989EFA4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DBF638-4A34-497F-8069-4C9722EECBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -2341,49 +2341,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2410,6 +2374,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2426,6 +2408,24 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3594,8 +3594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4467,7 +4467,7 @@
         <v>466</v>
       </c>
       <c r="C28">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -7426,7 +7426,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7470,13 +7470,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="74" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7491,7 +7491,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="H2" s="74" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7575,8 +7575,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7589,7 +7589,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="87"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7635,8 +7635,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="87"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7649,7 +7649,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="87"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7755,8 +7755,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7769,7 +7769,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="87"/>
+      <c r="H16" s="73"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7815,8 +7815,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="87"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7829,7 +7829,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="87"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7889,7 +7889,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="73"/>
+      <c r="H22" s="75"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7911,7 +7911,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="86" t="s">
+      <c r="H23" s="74" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7934,9 +7934,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
+      <c r="A25" s="75"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7949,25 +7949,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="73"/>
+      <c r="H25" s="75"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="86" t="s">
+      <c r="A26" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="74" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="74" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="88"/>
-      <c r="F26" s="89"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="91"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="78"/>
+      <c r="H26" s="79"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7976,10 +7976,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="88"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="92"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="80"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7988,10 +7988,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="93"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="92"/>
+      <c r="E28" s="81"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="80"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8004,11 +8004,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="74" t="s">
+      <c r="E29" s="84" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="86"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8020,26 +8020,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="77" t="s">
+      <c r="E30" s="87" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="78"/>
-      <c r="G30" s="79"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="89"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="96" t="s">
+      <c r="E31" s="90" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="97"/>
-      <c r="G31" s="98"/>
-      <c r="H31" s="87"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="73"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8052,11 +8052,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="99" t="s">
+      <c r="E32" s="93" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="100"/>
-      <c r="G32" s="101"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="95"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8068,11 +8068,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="77" t="s">
+      <c r="E33" s="87" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="78"/>
-      <c r="G33" s="79"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8082,11 +8082,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="83" t="s">
+      <c r="E34" s="96" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="84"/>
-      <c r="G34" s="85"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="98"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8100,11 +8100,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="74" t="s">
+      <c r="E35" s="84" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="86"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8116,11 +8116,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="77" t="s">
+      <c r="E36" s="87" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="78"/>
-      <c r="G36" s="79"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="89"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8130,11 +8130,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="83" t="s">
+      <c r="E37" s="96" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="84"/>
-      <c r="G37" s="85"/>
+      <c r="F37" s="97"/>
+      <c r="G37" s="98"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8148,11 +8148,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="74" t="s">
+      <c r="E38" s="84" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="75"/>
-      <c r="G38" s="76"/>
+      <c r="F38" s="85"/>
+      <c r="G38" s="86"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8164,11 +8164,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="77" t="s">
+      <c r="E39" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="78"/>
-      <c r="G39" s="79"/>
+      <c r="F39" s="88"/>
+      <c r="G39" s="89"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8178,11 +8178,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="83" t="s">
+      <c r="E40" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="84"/>
-      <c r="G40" s="85"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="98"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8196,11 +8196,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="74" t="s">
+      <c r="E41" s="84" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="75"/>
-      <c r="G41" s="76"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="86"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8212,11 +8212,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="77" t="s">
+      <c r="E42" s="87" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="78"/>
-      <c r="G42" s="79"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="89"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8226,11 +8226,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="83" t="s">
+      <c r="E43" s="96" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="84"/>
-      <c r="G43" s="85"/>
+      <c r="F43" s="97"/>
+      <c r="G43" s="98"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8244,11 +8244,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="74" t="s">
+      <c r="E44" s="84" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="75"/>
-      <c r="G44" s="76"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="86"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8260,11 +8260,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="77" t="s">
+      <c r="E45" s="87" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="78"/>
-      <c r="G45" s="79"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="89"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8274,11 +8274,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="83" t="s">
+      <c r="E46" s="96" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="84"/>
-      <c r="G46" s="85"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="98"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8292,11 +8292,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="74" t="s">
+      <c r="E47" s="84" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="75"/>
-      <c r="G47" s="76"/>
+      <c r="F47" s="85"/>
+      <c r="G47" s="86"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8308,38 +8308,78 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="77" t="s">
+      <c r="E48" s="87" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="78"/>
-      <c r="G48" s="79"/>
+      <c r="F48" s="88"/>
+      <c r="G48" s="89"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
-      <c r="C49" s="73"/>
+      <c r="A49" s="75"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="80" t="s">
+      <c r="E49" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="81"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="73"/>
+      <c r="F49" s="100"/>
+      <c r="G49" s="101"/>
+      <c r="H49" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8356,55 +8396,15 @@
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9047,7 +9047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FC119D-A7BC-46FE-BE1D-3900F19AB624}">
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="K12" sqref="K12"/>
     </sheetView>
@@ -11432,10 +11432,10 @@
   <dimension ref="A1:AA53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
+      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12655,19 +12655,19 @@
         <v>45</v>
       </c>
       <c r="L15">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="M15">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N15">
         <v>55</v>
       </c>
       <c r="O15">
+        <v>45</v>
+      </c>
+      <c r="P15">
         <v>35</v>
-      </c>
-      <c r="P15">
-        <v>45</v>
       </c>
       <c r="Q15">
         <v>15</v>
@@ -12682,7 +12682,7 @@
         <v>3</v>
       </c>
       <c r="U15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V15">
         <v>5</v>

</xml_diff>

<commit_message>
Fixed fmg9 and famas being unbuyable
-fmg9 and famas can now be bought
-Glock 18 (stock) and famas (scoped) now now longer have a redundant buy requirement
-PMC armor now has listed default damageModifier values to fix issue with wiki
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DBF638-4A34-497F-8069-4C9722EECBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA45EB1-FA0F-4103-98E4-0A9CF20B405A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="482">
   <si>
     <t>Name</t>
   </si>
@@ -2341,13 +2341,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2374,24 +2410,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2408,24 +2426,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3594,7 +3594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -7470,13 +7470,13 @@
       <c r="I1" s="49"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="86" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="46" t="s">
@@ -7491,7 +7491,7 @@
       <c r="G2" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="86" t="s">
         <v>348</v>
       </c>
     </row>
@@ -7575,8 +7575,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="60" t="s">
         <v>351</v>
       </c>
@@ -7589,7 +7589,7 @@
       <c r="G7" s="60" t="s">
         <v>352</v>
       </c>
-      <c r="H7" s="73"/>
+      <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
@@ -7635,8 +7635,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="60" t="s">
         <v>351</v>
       </c>
@@ -7649,7 +7649,7 @@
       <c r="G10" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="73"/>
+      <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
@@ -7755,8 +7755,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="60" t="s">
         <v>351</v>
       </c>
@@ -7769,7 +7769,7 @@
       <c r="G16" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="H16" s="73"/>
+      <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
@@ -7815,8 +7815,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="60" t="s">
         <v>351</v>
       </c>
@@ -7829,7 +7829,7 @@
       <c r="G19" s="60" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="73"/>
+      <c r="H19" s="87"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
@@ -7889,7 +7889,7 @@
       <c r="G22" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="H22" s="75"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
@@ -7911,7 +7911,7 @@
       <c r="G23" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="H23" s="74" t="s">
+      <c r="H23" s="86" t="s">
         <v>358</v>
       </c>
     </row>
@@ -7934,9 +7934,9 @@
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="48" t="s">
         <v>351</v>
       </c>
@@ -7949,25 +7949,25 @@
       <c r="G25" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H25" s="75"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="86" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="76"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7976,10 +7976,10 @@
       <c r="D27" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="80"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="92"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
@@ -7988,10 +7988,10 @@
       <c r="D28" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="80"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="92"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8004,11 +8004,11 @@
       <c r="D29" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="84" t="s">
+      <c r="E29" s="74" t="s">
         <v>473</v>
       </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="86"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8020,26 +8020,26 @@
       <c r="D30" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="E31" s="90" t="s">
+      <c r="E31" s="96" t="s">
         <v>475</v>
       </c>
-      <c r="F31" s="91"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="73"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="87"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
@@ -8052,11 +8052,11 @@
       <c r="D32" s="59" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="93" t="s">
+      <c r="E32" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="F32" s="94"/>
-      <c r="G32" s="95"/>
+      <c r="F32" s="100"/>
+      <c r="G32" s="101"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8068,11 +8068,11 @@
       <c r="D33" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="87" t="s">
+      <c r="E33" s="77" t="s">
         <v>380</v>
       </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8082,11 +8082,11 @@
       <c r="D34" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E34" s="96" t="s">
+      <c r="E34" s="83" t="s">
         <v>381</v>
       </c>
-      <c r="F34" s="97"/>
-      <c r="G34" s="98"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="85"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8100,11 +8100,11 @@
       <c r="D35" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="84" t="s">
+      <c r="E35" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="85"/>
-      <c r="G35" s="86"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8116,11 +8116,11 @@
       <c r="D36" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="87" t="s">
+      <c r="E36" s="77" t="s">
         <v>474</v>
       </c>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="79"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8130,11 +8130,11 @@
       <c r="D37" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="96" t="s">
+      <c r="E37" s="83" t="s">
         <v>476</v>
       </c>
-      <c r="F37" s="97"/>
-      <c r="G37" s="98"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8148,11 +8148,11 @@
       <c r="D38" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="84" t="s">
+      <c r="E38" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="85"/>
-      <c r="G38" s="86"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="76"/>
       <c r="H38" s="71" t="s">
         <v>382</v>
       </c>
@@ -8164,11 +8164,11 @@
       <c r="D39" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="87" t="s">
+      <c r="E39" s="77" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8178,11 +8178,11 @@
       <c r="D40" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E40" s="96" t="s">
+      <c r="E40" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="97"/>
-      <c r="G40" s="98"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8196,11 +8196,11 @@
       <c r="D41" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="84" t="s">
+      <c r="E41" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="85"/>
-      <c r="G41" s="86"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="76"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8212,11 +8212,11 @@
       <c r="D42" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="87" t="s">
+      <c r="E42" s="77" t="s">
         <v>383</v>
       </c>
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="79"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8226,11 +8226,11 @@
       <c r="D43" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E43" s="96" t="s">
+      <c r="E43" s="83" t="s">
         <v>384</v>
       </c>
-      <c r="F43" s="97"/>
-      <c r="G43" s="98"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="85"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8244,11 +8244,11 @@
       <c r="D44" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="84" t="s">
+      <c r="E44" s="74" t="s">
         <v>385</v>
       </c>
-      <c r="F44" s="85"/>
-      <c r="G44" s="86"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="76"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8260,11 +8260,11 @@
       <c r="D45" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="87" t="s">
+      <c r="E45" s="77" t="s">
         <v>386</v>
       </c>
-      <c r="F45" s="88"/>
-      <c r="G45" s="89"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8274,11 +8274,11 @@
       <c r="D46" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="E46" s="96" t="s">
+      <c r="E46" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="97"/>
-      <c r="G46" s="98"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="85"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8292,11 +8292,11 @@
       <c r="D47" s="62" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="84" t="s">
+      <c r="E47" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="85"/>
-      <c r="G47" s="86"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="76"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8308,62 +8308,54 @@
       <c r="D48" s="47" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="87" t="s">
+      <c r="E48" s="77" t="s">
         <v>387</v>
       </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="89"/>
+      <c r="F48" s="78"/>
+      <c r="G48" s="79"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="48" t="s">
         <v>351</v>
       </c>
-      <c r="E49" s="99" t="s">
+      <c r="E49" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="100"/>
-      <c r="G49" s="101"/>
-      <c r="H49" s="75"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8380,31 +8372,39 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11432,10 +11432,10 @@
   <dimension ref="A1:AA53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13696,8 +13696,8 @@
       <c r="C28" t="s">
         <v>90</v>
       </c>
-      <c r="D28" t="s">
-        <v>76</v>
+      <c r="D28">
+        <v>12000</v>
       </c>
       <c r="E28" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Item set rarity implementation
Implemented item set rarity mentioned in dev cto chat. As a side effect, enemy location can be selected in battle mode and weapons are tied to the enemies you are fighting and not the mission, so in battle mode you can select west EU PMCs in a east EU terror attack mission and they will have the proper weapons.

Also m9 hand sprites.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00B2D90-5D49-4F24-964A-CBDE289FED0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8071537C-BBA2-426E-A29A-2200D0791974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -49,30 +49,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Ethan McLaughlin</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C9B7DDB6-8D77-48F2-B62C-4C122D4443D0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Data on this page needs to be verified</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ethan McLaughlin</author>
@@ -119,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="481">
   <si>
     <t>Name</t>
   </si>
@@ -1559,9 +1535,6 @@
   </si>
   <si>
     <t>Just a list of things that are planing on being done in no particular order or priority so we don’t forget about them</t>
-  </si>
-  <si>
-    <t>RK 62 sprite(s)</t>
   </si>
   <si>
     <t>Launched blade</t>
@@ -1637,7 +1610,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1664,6 +1637,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2175,7 +2154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2429,6 +2408,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3840,7 +3822,7 @@
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="B11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C11">
         <v>30</v>
@@ -4463,7 +4445,7 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C28">
         <v>25</v>
@@ -4484,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M28" s="16" t="s">
         <v>39</v>
@@ -4511,7 +4493,7 @@
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -4532,7 +4514,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -5016,7 +4998,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="53" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
@@ -5046,7 +5028,7 @@
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="54"/>
       <c r="B46" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C46">
         <v>40</v>
@@ -5061,7 +5043,7 @@
         <v>7</v>
       </c>
       <c r="I46" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -7421,12 +7403,12 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7493,6 +7475,7 @@
       <c r="H2" s="85" t="s">
         <v>348</v>
       </c>
+      <c r="I2" s="102"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="71"/>
@@ -8004,7 +7987,7 @@
         <v>345</v>
       </c>
       <c r="E29" s="73" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F29" s="74"/>
       <c r="G29" s="75"/>
@@ -8034,7 +8017,7 @@
         <v>351</v>
       </c>
       <c r="E31" s="95" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F31" s="96"/>
       <c r="G31" s="97"/>
@@ -8116,7 +8099,7 @@
         <v>349</v>
       </c>
       <c r="E36" s="76" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F36" s="77"/>
       <c r="G36" s="78"/>
@@ -8130,7 +8113,7 @@
         <v>351</v>
       </c>
       <c r="E37" s="82" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F37" s="83"/>
       <c r="G37" s="84"/>
@@ -8406,7 +8389,6 @@
     <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8414,7 +8396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC8BAE7-4B1E-4B8C-8AF9-C5EAA5B2467F}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -8891,7 +8873,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8925,13 +8907,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B4" s="52"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B5" s="14"/>
     </row>
@@ -8939,20 +8921,17 @@
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>458</v>
-      </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B9" s="14"/>
     </row>
@@ -10630,7 +10609,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B6">
         <v>23</v>
@@ -10867,7 +10846,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -10930,7 +10909,7 @@
         <v>7</v>
       </c>
       <c r="V9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="W9" s="10" cm="1">
         <f t="array" aca="1" ref="W9" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
@@ -10941,7 +10920,7 @@
         <v>0.35</v>
       </c>
       <c r="Y9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -11430,7 +11409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E308052D-1B88-4699-843E-12AA607B59B8}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -17328,7 +17307,7 @@
         <v>160</v>
       </c>
       <c r="AB3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -17417,7 +17396,7 @@
         <v>178</v>
       </c>
       <c r="AB4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -17506,7 +17485,7 @@
         <v>178</v>
       </c>
       <c r="AB5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -17956,7 +17935,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B11">
         <v>24</v>
@@ -18040,7 +18019,7 @@
         <v>178</v>
       </c>
       <c r="AB11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -18745,7 +18724,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B9">
         <v>24</v>
@@ -18811,7 +18790,7 @@
         <v>15</v>
       </c>
       <c r="W9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="X9" cm="1">
         <f t="array" aca="1" ref="X9" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
@@ -18822,7 +18801,7 @@
         <v>0.35</v>
       </c>
       <c r="Z9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more item sets
Added quite a few more item sets.
Updated enemy sniper values.
Added APAV40 research.
Fixed Negev not updating sprite with ammo.
Fixed Stechkin sprite having the wrong indexes.
Removed STR_UNOBTAINABLE tags on some weapons that are now obtainable.
Fixed some spreadsheet values.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4C07FB-67F7-4FA9-BA80-8C9AB6AF9343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BCEB03-83D8-4358-A2B5-E296AFFB9F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="1" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,30 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ethan McLaughlin</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{25CD22B6-3B72-484D-8ECD-F3C21230A65F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>to do</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ethan McLaughlin</author>
@@ -95,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1602" uniqueCount="514">
   <si>
     <t>Name</t>
   </si>
@@ -1188,16 +1212,10 @@
     <t>Western Europe</t>
   </si>
   <si>
-    <t>FN SCAR</t>
-  </si>
-  <si>
     <t>North America</t>
   </si>
   <si>
     <t>M4 Carbine</t>
-  </si>
-  <si>
-    <t>Origin-12</t>
   </si>
   <si>
     <t>AK-74</t>
@@ -1222,9 +1240,6 @@
 </t>
   </si>
   <si>
-    <t>AR-18</t>
-  </si>
-  <si>
     <t>AR-180</t>
   </si>
   <si>
@@ -1262,12 +1277,6 @@
   </si>
   <si>
     <t>Terrorist 2</t>
-  </si>
-  <si>
-    <t>FN FAL (scoped)</t>
-  </si>
-  <si>
-    <t>M82 Barrett</t>
   </si>
   <si>
     <t>AK-15</t>
@@ -1615,17 +1624,116 @@
     <t>AKM/AKs-74u/?</t>
   </si>
   <si>
-    <t>AK-74 (1 Grenade)/?/Aks-74u SOPMOD</t>
-  </si>
-  <si>
     <t>M1911/M9/Dual M9s</t>
+  </si>
+  <si>
+    <t>Remington 870/M3/Remington (slug)</t>
+  </si>
+  <si>
+    <t>Spas12/Remington 870/Spas12(slug)</t>
+  </si>
+  <si>
+    <t>Spas12/Remington 870 (slug)/Spas12 (inc)</t>
+  </si>
+  <si>
+    <t>Remington 870/M3 (slug)/M3 (inc)</t>
+  </si>
+  <si>
+    <t>KS-23/KS-23 (slug)/KS-23(NL)</t>
+  </si>
+  <si>
+    <t>Skorpion/Uzi/Skorpion</t>
+  </si>
+  <si>
+    <t>Double Barrel/Skorpion/Uzi</t>
+  </si>
+  <si>
+    <t>M16 (Scoped)/SKS/M14 (Scoped)</t>
+  </si>
+  <si>
+    <t>SKS/Dragunov/SKS</t>
+  </si>
+  <si>
+    <t>FN FAL (scoped)/Dragunov/FN FAL (scoped)</t>
+  </si>
+  <si>
+    <t>M82 Barret/M24 SWS/AWM</t>
+  </si>
+  <si>
+    <t>Sako TRG/M82 Barrett/AWP</t>
+  </si>
+  <si>
+    <t>VSS/OSV 96/OSV 96</t>
+  </si>
+  <si>
+    <t>(1 Grenade) + AK-74/?/AKs-74u</t>
+  </si>
+  <si>
+    <t>AK-12/Aks-74u (Sopmod)/RK-62</t>
+  </si>
+  <si>
+    <t>HK416/G36/Famas</t>
+  </si>
+  <si>
+    <t>FN SCAR L/FN SCAR H/?</t>
+  </si>
+  <si>
+    <t>M4 Carbine/SCAR L/FX-05</t>
+  </si>
+  <si>
+    <t>AK-74/G3?</t>
+  </si>
+  <si>
+    <t>AR-18/G3?</t>
+  </si>
+  <si>
+    <t>Origin-12/Deagle/Gold Deagle</t>
+  </si>
+  <si>
+    <t>M4 Carbine/SCAR L/Deagle</t>
+  </si>
+  <si>
+    <t>Remington 870/M9/Deagle</t>
+  </si>
+  <si>
+    <t>Skorpion/Stechkin/Glock 17</t>
+  </si>
+  <si>
+    <t>TEC-9/Glock18/Spas 12</t>
+  </si>
+  <si>
+    <t>M16/M16 (m203 Smoke)/Deagle</t>
+  </si>
+  <si>
+    <t>M4 Carbine/M4 (M320 Smoke)/M4 (UBS)</t>
+  </si>
+  <si>
+    <t>AR-18/Spas 12/G3</t>
+  </si>
+  <si>
+    <t>AR-18/G3/Spas 12</t>
+  </si>
+  <si>
+    <t>AKM/AK-74</t>
+  </si>
+  <si>
+    <t>RPK/RPK/AKM</t>
+  </si>
+  <si>
+    <t>AKs-74u/AK-74/Glock 17</t>
+  </si>
+  <si>
+    <t>M249/M60/M60</t>
+  </si>
+  <si>
+    <t>Negev/M60/M60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1659,6 +1767,13 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="25">
@@ -2337,13 +2452,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2370,24 +2521,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2404,24 +2537,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3590,8 +3705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3816,7 +3931,7 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -3831,13 +3946,13 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="56"/>
       <c r="B11" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="C11">
         <v>30</v>
@@ -4019,7 +4134,7 @@
         <v>23</v>
       </c>
       <c r="C16">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -4460,7 +4575,7 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="C28">
         <v>25</v>
@@ -4481,7 +4596,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="M28" s="16" t="s">
         <v>39</v>
@@ -4508,7 +4623,7 @@
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -4529,7 +4644,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -5013,7 +5128,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="53" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
@@ -5043,7 +5158,7 @@
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="54"/>
       <c r="B46" s="14" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C46">
         <v>40</v>
@@ -5058,7 +5173,7 @@
         <v>7</v>
       </c>
       <c r="I46" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -7418,12 +7533,12 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7431,9 +7546,9 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="34.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="30.140625" customWidth="1"/>
   </cols>
@@ -7466,28 +7581,28 @@
       <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="86" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>345</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>346</v>
+        <v>494</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>346</v>
+        <v>494</v>
       </c>
       <c r="G2" s="45" t="s">
         <v>347</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="86" t="s">
         <v>348</v>
       </c>
       <c r="I2" s="62"/>
@@ -7500,13 +7615,13 @@
         <v>349</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>144</v>
+        <v>495</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>144</v>
+        <v>495</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>350</v>
+        <v>496</v>
       </c>
       <c r="H3" s="72"/>
     </row>
@@ -7515,16 +7630,16 @@
       <c r="B4" s="72"/>
       <c r="C4" s="72"/>
       <c r="D4" s="60" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>352</v>
+        <v>497</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>352</v>
+        <v>501</v>
       </c>
       <c r="G4" s="60" t="s">
-        <v>353</v>
+        <v>500</v>
       </c>
       <c r="H4" s="72"/>
     </row>
@@ -7540,13 +7655,13 @@
         <v>345</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>111</v>
+        <v>503</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>354</v>
+        <v>511</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>354</v>
+        <v>511</v>
       </c>
       <c r="H5" s="71" t="s">
         <v>348</v>
@@ -7560,38 +7675,38 @@
         <v>349</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>355</v>
+        <v>504</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>354</v>
+        <v>507</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>354</v>
+        <v>508</v>
       </c>
       <c r="H6" s="72"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="72"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="59" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>177</v>
+        <v>502</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>356</v>
+        <v>505</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>352</v>
-      </c>
-      <c r="H7" s="73"/>
+        <v>506</v>
+      </c>
+      <c r="H7" s="87"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="72"/>
       <c r="B8" s="71" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C8" s="71" t="s">
         <v>316</v>
@@ -7600,16 +7715,16 @@
         <v>345</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>354</v>
+        <v>509</v>
       </c>
       <c r="F8" s="61" t="s">
-        <v>354</v>
+        <v>510</v>
       </c>
       <c r="G8" s="61" t="s">
         <v>220</v>
       </c>
       <c r="H8" s="71" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7620,38 +7735,38 @@
         <v>349</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F9" s="46" t="s">
         <v>211</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>211</v>
+        <v>513</v>
       </c>
       <c r="H9" s="72"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="72"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
       <c r="D10" s="59" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F10" s="59" t="s">
         <v>211</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>211</v>
-      </c>
-      <c r="H10" s="73"/>
+        <v>512</v>
+      </c>
+      <c r="H10" s="87"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="72"/>
       <c r="B11" s="71" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C11" s="71" t="s">
         <v>318</v>
@@ -7660,16 +7775,16 @@
         <v>345</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="F11" s="61" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
       <c r="H11" s="71" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7683,10 +7798,10 @@
         <v>203</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>354</v>
+        <v>498</v>
       </c>
       <c r="G12" s="46" t="s">
-        <v>361</v>
+        <v>499</v>
       </c>
       <c r="H12" s="72"/>
     </row>
@@ -7695,23 +7810,23 @@
       <c r="B13" s="72"/>
       <c r="C13" s="72"/>
       <c r="D13" s="60" t="s">
+        <v>350</v>
+      </c>
+      <c r="E13" s="60" t="s">
+        <v>359</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>354</v>
+      </c>
+      <c r="G13" s="60" t="s">
         <v>351</v>
-      </c>
-      <c r="E13" s="60" t="s">
-        <v>362</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>356</v>
-      </c>
-      <c r="G13" s="60" t="s">
-        <v>352</v>
       </c>
       <c r="H13" s="72"/>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="72"/>
       <c r="B14" s="71" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C14" s="71" t="s">
         <v>320</v>
@@ -7720,13 +7835,13 @@
         <v>345</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>168</v>
+        <v>486</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>168</v>
+        <v>486</v>
       </c>
       <c r="G14" s="61" t="s">
-        <v>181</v>
+        <v>484</v>
       </c>
       <c r="H14" s="71" t="s">
         <v>348</v>
@@ -7740,38 +7855,38 @@
         <v>349</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>111</v>
+        <v>485</v>
       </c>
       <c r="F15" s="46" t="s">
-        <v>177</v>
+        <v>481</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>177</v>
+        <v>482</v>
       </c>
       <c r="H15" s="72"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="72"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="59" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E16" s="59" t="s">
         <v>168</v>
       </c>
       <c r="F16" s="59" t="s">
-        <v>177</v>
+        <v>480</v>
       </c>
       <c r="G16" s="59" t="s">
-        <v>177</v>
-      </c>
-      <c r="H16" s="73"/>
+        <v>483</v>
+      </c>
+      <c r="H16" s="87"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="72"/>
       <c r="B17" s="71" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C17" s="71" t="s">
         <v>322</v>
@@ -7786,10 +7901,10 @@
         <v>111</v>
       </c>
       <c r="G17" s="61" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="H17" s="71" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7806,32 +7921,32 @@
         <v>111</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="H18" s="72"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
       <c r="D19" s="59" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E19" s="59" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G19" s="59" t="s">
-        <v>366</v>
-      </c>
-      <c r="H19" s="73"/>
+        <v>363</v>
+      </c>
+      <c r="H19" s="87"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="72"/>
       <c r="B20" s="71" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C20" s="71" t="s">
         <v>324</v>
@@ -7840,16 +7955,16 @@
         <v>345</v>
       </c>
       <c r="E20" s="61" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F20" s="61" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G20" s="61" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H20" s="71" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7860,13 +7975,13 @@
         <v>349</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G21" s="46" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="H21" s="72"/>
     </row>
@@ -7875,23 +7990,23 @@
       <c r="B22" s="72"/>
       <c r="C22" s="72"/>
       <c r="D22" s="60" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E22" s="60" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F22" s="60" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G22" s="60" t="s">
-        <v>373</v>
-      </c>
-      <c r="H22" s="75"/>
+        <v>370</v>
+      </c>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="72"/>
       <c r="B23" s="71" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C23" s="71" t="s">
         <v>325</v>
@@ -7903,13 +8018,13 @@
         <v>148</v>
       </c>
       <c r="F23" s="61" t="s">
-        <v>151</v>
+        <v>488</v>
       </c>
       <c r="G23" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="H23" s="74" t="s">
-        <v>358</v>
+        <v>492</v>
+      </c>
+      <c r="H23" s="86" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7923,48 +8038,48 @@
         <v>148</v>
       </c>
       <c r="F24" s="46" t="s">
-        <v>375</v>
+        <v>489</v>
       </c>
       <c r="G24" s="46" t="s">
-        <v>376</v>
+        <v>491</v>
       </c>
       <c r="H24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="75"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="75"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
       <c r="D25" s="47" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E25" s="47" t="s">
         <v>148</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>148</v>
+        <v>487</v>
       </c>
       <c r="G25" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="H25" s="75"/>
+        <v>490</v>
+      </c>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="86" t="s">
         <v>338</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="86" t="s">
         <v>298</v>
       </c>
       <c r="D26" s="45" t="s">
         <v>345</v>
       </c>
-      <c r="E26" s="76"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="79"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="91"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="72"/>
@@ -7973,22 +8088,22 @@
       <c r="D27" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="80"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="92"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
       <c r="B28" s="72"/>
       <c r="C28" s="72"/>
       <c r="D28" s="60" t="s">
-        <v>351</v>
-      </c>
-      <c r="E28" s="81"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="80"/>
+        <v>350</v>
+      </c>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="92"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="72"/>
@@ -8001,11 +8116,11 @@
       <c r="D29" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="E29" s="84" t="s">
-        <v>471</v>
-      </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="86"/>
+      <c r="E29" s="74" t="s">
+        <v>466</v>
+      </c>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
       <c r="H29" s="71" t="s">
         <v>348</v>
       </c>
@@ -8017,31 +8132,31 @@
       <c r="D30" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
       <c r="H30" s="72"/>
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="59" t="s">
-        <v>351</v>
-      </c>
-      <c r="E31" s="90" t="s">
-        <v>473</v>
-      </c>
-      <c r="F31" s="91"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="73"/>
+        <v>350</v>
+      </c>
+      <c r="E31" s="96" t="s">
+        <v>468</v>
+      </c>
+      <c r="F31" s="97"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="87"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="72"/>
       <c r="B32" s="72" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C32" s="72" t="s">
         <v>330</v>
@@ -8049,11 +8164,11 @@
       <c r="D32" s="58" t="s">
         <v>345</v>
       </c>
-      <c r="E32" s="93" t="s">
-        <v>378</v>
-      </c>
-      <c r="F32" s="94"/>
-      <c r="G32" s="95"/>
+      <c r="E32" s="99" t="s">
+        <v>373</v>
+      </c>
+      <c r="F32" s="100"/>
+      <c r="G32" s="101"/>
       <c r="H32" s="72" t="s">
         <v>348</v>
       </c>
@@ -8065,11 +8180,11 @@
       <c r="D33" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="E33" s="87" t="s">
-        <v>379</v>
-      </c>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
+      <c r="E33" s="77" t="s">
+        <v>374</v>
+      </c>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="72"/>
     </row>
     <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8077,19 +8192,19 @@
       <c r="B34" s="72"/>
       <c r="C34" s="72"/>
       <c r="D34" s="60" t="s">
-        <v>351</v>
-      </c>
-      <c r="E34" s="96" t="s">
-        <v>380</v>
-      </c>
-      <c r="F34" s="97"/>
-      <c r="G34" s="98"/>
+        <v>350</v>
+      </c>
+      <c r="E34" s="83" t="s">
+        <v>375</v>
+      </c>
+      <c r="F34" s="84"/>
+      <c r="G34" s="85"/>
       <c r="H34" s="72"/>
     </row>
     <row r="35" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="72"/>
       <c r="B35" s="71" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C35" s="71" t="s">
         <v>318</v>
@@ -8097,11 +8212,11 @@
       <c r="D35" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="E35" s="84" t="s">
-        <v>377</v>
-      </c>
-      <c r="F35" s="85"/>
-      <c r="G35" s="86"/>
+      <c r="E35" s="74" t="s">
+        <v>372</v>
+      </c>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
       <c r="H35" s="71" t="s">
         <v>348</v>
       </c>
@@ -8113,11 +8228,11 @@
       <c r="D36" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="87" t="s">
-        <v>472</v>
-      </c>
-      <c r="F36" s="88"/>
-      <c r="G36" s="89"/>
+      <c r="E36" s="77" t="s">
+        <v>467</v>
+      </c>
+      <c r="F36" s="78"/>
+      <c r="G36" s="79"/>
       <c r="H36" s="72"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8125,19 +8240,19 @@
       <c r="B37" s="72"/>
       <c r="C37" s="72"/>
       <c r="D37" s="60" t="s">
-        <v>351</v>
-      </c>
-      <c r="E37" s="96" t="s">
-        <v>474</v>
-      </c>
-      <c r="F37" s="97"/>
-      <c r="G37" s="98"/>
+        <v>350</v>
+      </c>
+      <c r="E37" s="83" t="s">
+        <v>469</v>
+      </c>
+      <c r="F37" s="84"/>
+      <c r="G37" s="85"/>
       <c r="H37" s="72"/>
     </row>
     <row r="38" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="72"/>
       <c r="B38" s="71" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C38" s="71" t="s">
         <v>287</v>
@@ -8145,13 +8260,13 @@
       <c r="D38" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="E38" s="84" t="s">
+      <c r="E38" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="85"/>
-      <c r="G38" s="86"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="76"/>
       <c r="H38" s="71" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8161,11 +8276,11 @@
       <c r="D39" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="E39" s="87" t="s">
+      <c r="E39" s="77" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="88"/>
-      <c r="G39" s="89"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
       <c r="H39" s="72"/>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8173,19 +8288,19 @@
       <c r="B40" s="72"/>
       <c r="C40" s="72"/>
       <c r="D40" s="60" t="s">
-        <v>351</v>
-      </c>
-      <c r="E40" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="E40" s="83" t="s">
         <v>186</v>
       </c>
-      <c r="F40" s="97"/>
-      <c r="G40" s="98"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="85"/>
       <c r="H40" s="72"/>
     </row>
     <row r="41" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="72"/>
       <c r="B41" s="71" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C41" s="71" t="s">
         <v>322</v>
@@ -8193,11 +8308,11 @@
       <c r="D41" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="E41" s="84" t="s">
+      <c r="E41" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="F41" s="85"/>
-      <c r="G41" s="86"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="76"/>
       <c r="H41" s="71" t="s">
         <v>348</v>
       </c>
@@ -8209,11 +8324,11 @@
       <c r="D42" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="E42" s="87" t="s">
-        <v>382</v>
-      </c>
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
+      <c r="E42" s="77" t="s">
+        <v>377</v>
+      </c>
+      <c r="F42" s="78"/>
+      <c r="G42" s="79"/>
       <c r="H42" s="72"/>
     </row>
     <row r="43" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8221,19 +8336,19 @@
       <c r="B43" s="72"/>
       <c r="C43" s="72"/>
       <c r="D43" s="60" t="s">
-        <v>351</v>
-      </c>
-      <c r="E43" s="96" t="s">
-        <v>383</v>
-      </c>
-      <c r="F43" s="97"/>
-      <c r="G43" s="98"/>
+        <v>350</v>
+      </c>
+      <c r="E43" s="83" t="s">
+        <v>378</v>
+      </c>
+      <c r="F43" s="84"/>
+      <c r="G43" s="85"/>
       <c r="H43" s="72"/>
     </row>
     <row r="44" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="72"/>
       <c r="B44" s="71" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C44" s="71" t="s">
         <v>316</v>
@@ -8241,11 +8356,11 @@
       <c r="D44" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="E44" s="84" t="s">
-        <v>384</v>
-      </c>
-      <c r="F44" s="85"/>
-      <c r="G44" s="86"/>
+      <c r="E44" s="74" t="s">
+        <v>379</v>
+      </c>
+      <c r="F44" s="75"/>
+      <c r="G44" s="76"/>
       <c r="H44" s="71" t="s">
         <v>348</v>
       </c>
@@ -8257,11 +8372,11 @@
       <c r="D45" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="E45" s="87" t="s">
-        <v>385</v>
-      </c>
-      <c r="F45" s="88"/>
-      <c r="G45" s="89"/>
+      <c r="E45" s="77" t="s">
+        <v>380</v>
+      </c>
+      <c r="F45" s="78"/>
+      <c r="G45" s="79"/>
       <c r="H45" s="72"/>
     </row>
     <row r="46" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8269,19 +8384,19 @@
       <c r="B46" s="72"/>
       <c r="C46" s="72"/>
       <c r="D46" s="60" t="s">
-        <v>351</v>
-      </c>
-      <c r="E46" s="96" t="s">
+        <v>350</v>
+      </c>
+      <c r="E46" s="83" t="s">
         <v>215</v>
       </c>
-      <c r="F46" s="97"/>
-      <c r="G46" s="98"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="85"/>
       <c r="H46" s="72"/>
     </row>
     <row r="47" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="72"/>
       <c r="B47" s="71" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C47" s="71" t="s">
         <v>325</v>
@@ -8289,11 +8404,11 @@
       <c r="D47" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="E47" s="84" t="s">
+      <c r="E47" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="F47" s="85"/>
-      <c r="G47" s="86"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="76"/>
       <c r="H47" s="71" t="s">
         <v>348</v>
       </c>
@@ -8305,62 +8420,54 @@
       <c r="D48" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="E48" s="87" t="s">
-        <v>386</v>
-      </c>
-      <c r="F48" s="88"/>
-      <c r="G48" s="89"/>
+      <c r="E48" s="77" t="s">
+        <v>381</v>
+      </c>
+      <c r="F48" s="78"/>
+      <c r="G48" s="79"/>
       <c r="H48" s="72"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="47" t="s">
-        <v>351</v>
-      </c>
-      <c r="E49" s="99" t="s">
+        <v>350</v>
+      </c>
+      <c r="E49" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="100"/>
-      <c r="G49" s="101"/>
-      <c r="H49" s="75"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8377,33 +8484,42 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:H37"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E49:G49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8433,63 +8549,63 @@
         <v>236</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>388</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="L1" s="20" t="s">
         <v>392</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="N1" s="20" t="s">
         <v>394</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="O1" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>396</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>397</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>398</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>399</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>400</v>
-      </c>
-      <c r="P1" s="20" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C2" s="32">
         <v>3</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="E2" s="32">
         <v>0</v>
@@ -8501,13 +8617,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="49" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I2" s="49" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="J2" s="49" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="K2" s="49">
         <v>0</v>
@@ -8516,128 +8632,128 @@
         <v>0</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="O2" s="32">
         <v>300</v>
       </c>
       <c r="P2" s="32" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="26">
         <v>12</v>
       </c>
       <c r="D3" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="E3" s="26">
+        <v>0</v>
+      </c>
+      <c r="F3" s="26">
+        <v>0</v>
+      </c>
+      <c r="G3" s="50">
+        <v>0</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>422</v>
+      </c>
+      <c r="I3" s="50" t="s">
+        <v>422</v>
+      </c>
+      <c r="J3" s="50" t="s">
+        <v>422</v>
+      </c>
+      <c r="K3" s="50">
+        <v>0</v>
+      </c>
+      <c r="L3" s="50">
+        <v>0</v>
+      </c>
+      <c r="M3" s="26" t="s">
         <v>404</v>
       </c>
-      <c r="E3" s="26">
-        <v>0</v>
-      </c>
-      <c r="F3" s="26">
-        <v>0</v>
-      </c>
-      <c r="G3" s="50">
-        <v>0</v>
-      </c>
-      <c r="H3" s="50" t="s">
-        <v>427</v>
-      </c>
-      <c r="I3" s="50" t="s">
-        <v>427</v>
-      </c>
-      <c r="J3" s="50" t="s">
-        <v>427</v>
-      </c>
-      <c r="K3" s="50">
-        <v>0</v>
-      </c>
-      <c r="L3" s="50">
-        <v>0</v>
-      </c>
-      <c r="M3" s="26" t="s">
-        <v>409</v>
-      </c>
       <c r="N3" s="26" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="O3" s="26">
         <v>400</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C4" s="32">
         <v>0</v>
       </c>
       <c r="D4" s="32" t="s">
+        <v>399</v>
+      </c>
+      <c r="E4" s="32">
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <v>1</v>
+      </c>
+      <c r="G4" s="49">
+        <v>1</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>423</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>423</v>
+      </c>
+      <c r="J4" s="49" t="s">
+        <v>431</v>
+      </c>
+      <c r="K4" s="49">
+        <v>0</v>
+      </c>
+      <c r="L4" s="49">
+        <v>0</v>
+      </c>
+      <c r="M4" s="32" t="s">
         <v>404</v>
       </c>
-      <c r="E4" s="32">
-        <v>0</v>
-      </c>
-      <c r="F4" s="32">
-        <v>1</v>
-      </c>
-      <c r="G4" s="49">
-        <v>1</v>
-      </c>
-      <c r="H4" s="49" t="s">
-        <v>428</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>428</v>
-      </c>
-      <c r="J4" s="49" t="s">
-        <v>436</v>
-      </c>
-      <c r="K4" s="49">
-        <v>0</v>
-      </c>
-      <c r="L4" s="49">
-        <v>0</v>
-      </c>
-      <c r="M4" s="32" t="s">
-        <v>409</v>
-      </c>
       <c r="N4" s="32" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="O4" s="32" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="P4" s="32" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C5" s="26">
         <v>20</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="E5" s="26">
         <v>0</v>
@@ -8646,98 +8762,98 @@
         <v>1</v>
       </c>
       <c r="G5" s="50" t="s">
+        <v>427</v>
+      </c>
+      <c r="H5" s="50" t="s">
+        <v>424</v>
+      </c>
+      <c r="I5" s="50" t="s">
+        <v>424</v>
+      </c>
+      <c r="J5" s="50" t="s">
         <v>432</v>
       </c>
-      <c r="H5" s="50" t="s">
-        <v>429</v>
-      </c>
-      <c r="I5" s="50" t="s">
-        <v>429</v>
-      </c>
-      <c r="J5" s="50" t="s">
-        <v>437</v>
-      </c>
       <c r="K5" s="50" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="N5" s="26" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="O5" s="26" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C6" s="32">
         <v>10</v>
       </c>
       <c r="D6" s="32" t="s">
+        <v>399</v>
+      </c>
+      <c r="E6" s="32">
+        <v>0</v>
+      </c>
+      <c r="F6" s="32">
+        <v>0</v>
+      </c>
+      <c r="G6" s="49">
+        <v>0</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>423</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>429</v>
+      </c>
+      <c r="J6" s="49" t="s">
+        <v>423</v>
+      </c>
+      <c r="K6" s="49">
+        <v>0</v>
+      </c>
+      <c r="L6" s="49">
+        <v>0</v>
+      </c>
+      <c r="M6" s="32" t="s">
         <v>404</v>
       </c>
-      <c r="E6" s="32">
-        <v>0</v>
-      </c>
-      <c r="F6" s="32">
-        <v>0</v>
-      </c>
-      <c r="G6" s="49">
-        <v>0</v>
-      </c>
-      <c r="H6" s="49" t="s">
-        <v>428</v>
-      </c>
-      <c r="I6" s="49" t="s">
-        <v>434</v>
-      </c>
-      <c r="J6" s="49" t="s">
-        <v>428</v>
-      </c>
-      <c r="K6" s="49">
-        <v>0</v>
-      </c>
-      <c r="L6" s="49">
-        <v>0</v>
-      </c>
-      <c r="M6" s="32" t="s">
-        <v>409</v>
-      </c>
       <c r="N6" s="32" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="O6" s="32">
         <v>500</v>
       </c>
       <c r="P6" s="32" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C7" s="26">
         <v>0</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="E7" s="26">
         <v>1</v>
@@ -8746,48 +8862,48 @@
         <v>2</v>
       </c>
       <c r="G7" s="50" t="s">
+        <v>428</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>425</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>430</v>
+      </c>
+      <c r="J7" s="50" t="s">
         <v>433</v>
       </c>
-      <c r="H7" s="50" t="s">
-        <v>430</v>
-      </c>
-      <c r="I7" s="50" t="s">
+      <c r="K7" s="50" t="s">
         <v>435</v>
       </c>
-      <c r="J7" s="50" t="s">
-        <v>438</v>
-      </c>
-      <c r="K7" s="50" t="s">
-        <v>440</v>
-      </c>
       <c r="L7" s="50" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="M7" s="26" t="s">
+        <v>410</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="O7" s="26" t="s">
         <v>415</v>
       </c>
-      <c r="N7" s="26" t="s">
-        <v>423</v>
-      </c>
-      <c r="O7" s="26" t="s">
-        <v>420</v>
-      </c>
       <c r="P7" s="26" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C8" s="32">
         <v>4</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="E8" s="32">
         <v>0</v>
@@ -8799,13 +8915,13 @@
         <v>0</v>
       </c>
       <c r="H8" s="49" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="I8" s="49" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="J8" s="49" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="K8" s="49">
         <v>0</v>
@@ -8814,64 +8930,64 @@
         <v>0</v>
       </c>
       <c r="M8" s="32" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="N8" s="32" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="O8" s="32" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="P8" s="32" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B9" s="39"/>
       <c r="C9" s="26">
         <v>24</v>
       </c>
       <c r="D9" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="E9" s="26">
+        <v>0</v>
+      </c>
+      <c r="F9" s="50" t="s">
         <v>422</v>
       </c>
-      <c r="E9" s="26">
-        <v>0</v>
-      </c>
-      <c r="F9" s="50" t="s">
+      <c r="G9" s="50" t="s">
+        <v>423</v>
+      </c>
+      <c r="H9" s="50" t="s">
+        <v>426</v>
+      </c>
+      <c r="I9" s="50" t="s">
+        <v>431</v>
+      </c>
+      <c r="J9" s="50" t="s">
+        <v>434</v>
+      </c>
+      <c r="K9" s="50" t="s">
         <v>427</v>
       </c>
-      <c r="G9" s="50" t="s">
-        <v>428</v>
-      </c>
-      <c r="H9" s="50" t="s">
-        <v>431</v>
-      </c>
-      <c r="I9" s="50" t="s">
+      <c r="L9" s="50" t="s">
         <v>436</v>
       </c>
-      <c r="J9" s="50" t="s">
-        <v>439</v>
-      </c>
-      <c r="K9" s="50" t="s">
-        <v>432</v>
-      </c>
-      <c r="L9" s="50" t="s">
-        <v>441</v>
-      </c>
       <c r="M9" s="26" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="N9" s="26">
         <v>999</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -8899,7 +9015,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="102" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="B1" s="102"/>
       <c r="C1" s="51"/>
@@ -8922,13 +9038,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B4" s="52"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="B5" s="14"/>
     </row>
@@ -8940,13 +9056,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B9" s="14"/>
     </row>
@@ -9042,7 +9158,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J17" sqref="J17"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9233,7 +9349,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B3">
         <v>16</v>
@@ -9296,7 +9412,7 @@
         <v>76</v>
       </c>
       <c r="V3" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="W3" cm="1">
         <f t="array" aca="1" ref="W3" ca="1">INDEX(Caliber!B2:'Caliber'!C10,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B10,0),2)</f>
@@ -9310,7 +9426,7 @@
         <v>92</v>
       </c>
       <c r="Z3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -10187,7 +10303,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -10276,9 +10392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A5" activeCellId="1" sqref="A4:XFD4 A5:XFD5"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10466,7 +10582,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -10703,7 +10819,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B6">
         <v>23</v>
@@ -10940,7 +11056,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -11003,7 +11119,7 @@
         <v>7</v>
       </c>
       <c r="V9" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="W9" s="10" cm="1">
         <f t="array" aca="1" ref="W9" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
@@ -11014,7 +11130,7 @@
         <v>0.35</v>
       </c>
       <c r="Y9" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -11414,7 +11530,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B15">
         <v>22</v>
@@ -11488,7 +11604,7 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -11504,10 +11620,10 @@
   <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13022,7 +13138,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B19">
         <v>23</v>
@@ -13596,7 +13712,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B26">
         <v>30</v>
@@ -13678,7 +13794,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B27">
         <v>32</v>
@@ -13842,7 +13958,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B29">
         <v>30</v>
@@ -13854,7 +13970,7 @@
         <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
@@ -13924,7 +14040,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B30">
         <v>24</v>
@@ -15810,7 +15926,7 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="B53">
         <v>21</v>
@@ -15892,7 +16008,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B54">
         <v>19</v>
@@ -15995,8 +16111,8 @@
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:AA1"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16177,15 +16293,15 @@
         <v>76</v>
       </c>
       <c r="W2" t="s">
-        <v>120</v>
+        <v>23</v>
       </c>
       <c r="X2">
         <f>INDEX(Caliber!B13:'Caliber'!C23,MATCH(W2,Caliber!B13:'Caliber'!B23,0),2)</f>
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="Y2">
         <f>INDEX(Caliber!C13:'Caliber'!D23,MATCH(W2,Caliber!B13:'Caliber'!B23,0),2)</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="s">
         <v>101</v>
@@ -16940,7 +17056,7 @@
         <v>90</v>
       </c>
       <c r="D12">
-        <v>4400</v>
+        <v>44000</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
@@ -17565,7 +17681,7 @@
         <v>160</v>
       </c>
       <c r="AB3" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -17654,7 +17770,7 @@
         <v>178</v>
       </c>
       <c r="AB4" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -17743,7 +17859,7 @@
         <v>178</v>
       </c>
       <c r="AB5" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -18193,7 +18309,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B11">
         <v>24</v>
@@ -18277,7 +18393,7 @@
         <v>178</v>
       </c>
       <c r="AB11" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -18293,8 +18409,8 @@
   <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K5" sqref="K5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" activeCellId="1" sqref="A6:XFD6 A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18435,10 +18551,10 @@
         <v>76</v>
       </c>
       <c r="J2">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K2">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s">
         <v>76</v>
@@ -18982,7 +19098,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B9">
         <v>24</v>
@@ -19048,7 +19164,7 @@
         <v>15</v>
       </c>
       <c r="W9" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="X9" cm="1">
         <f t="array" aca="1" ref="X9" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
@@ -19059,7 +19175,7 @@
         <v>0.35</v>
       </c>
       <c r="Z9" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -19811,7 +19927,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
M27 LAW, Uniform w/ NVG & Adv. NVG
Added M27A7 LAW
Renamed Uniform (Kevlar) [and all other relevant armor options] to Kevlar Vest.
Added new armor options: Uniform w/ NVG, Uniform (NV, BP) Uniform w/ Adv. NVG, and Uniform (Adv. NV, BP).
Added manufacturing option to swap directly to Adv. NV from kevlar (NV).
Removed Aim to Head tracks.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A60AC8B-BC46-4CDE-B483-B4AB4078797C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F1857E-5A3A-4503-9335-5CBEA08AFC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="10" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="560">
   <si>
     <t>Name</t>
   </si>
@@ -1663,15 +1663,9 @@
     <t>Prison cell sprite</t>
   </si>
   <si>
-    <t>Uniform w/ NVGs &amp; Adv. NVGs</t>
-  </si>
-  <si>
     <t>Quick weapon attachment researches when you get a weapon that can use them (ie get m4 from enemy + have sopmod unlocked -&gt; research -&gt; can apply sopmod despite not doing m4 acquisition).</t>
   </si>
   <si>
-    <t>add manufacturing to swap out NVGs for adv. NVGs on armor</t>
-  </si>
-  <si>
     <t>Aks-74u</t>
   </si>
   <si>
@@ -1961,6 +1955,15 @@
   </si>
   <si>
     <t>Mac 10</t>
+  </si>
+  <si>
+    <t>SMAW</t>
+  </si>
+  <si>
+    <t>Built in Ammo, Not reloadable</t>
+  </si>
+  <si>
+    <t>Single Use</t>
   </si>
 </sst>
 </file>
@@ -4091,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5508,6 +5511,27 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
+      <c r="B43" t="s">
+        <v>551</v>
+      </c>
+      <c r="C43">
+        <v>95</v>
+      </c>
+      <c r="D43">
+        <v>0.75</v>
+      </c>
+      <c r="E43">
+        <v>6</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
@@ -7980,10 +8004,10 @@
         <v>345</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G2" s="45" t="s">
         <v>346</v>
@@ -8001,13 +8025,13 @@
         <v>348</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H3" s="100"/>
     </row>
@@ -8019,13 +8043,13 @@
         <v>349</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G4" s="60" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H4" s="100"/>
     </row>
@@ -8041,13 +8065,13 @@
         <v>345</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H5" s="99" t="s">
         <v>347</v>
@@ -8061,13 +8085,13 @@
         <v>348</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H6" s="100"/>
     </row>
@@ -8079,13 +8103,13 @@
         <v>349</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H7" s="103"/>
     </row>
@@ -8101,10 +8125,10 @@
         <v>345</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F8" s="61" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="G8" s="61" t="s">
         <v>220</v>
@@ -8127,7 +8151,7 @@
         <v>211</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H9" s="100"/>
     </row>
@@ -8145,7 +8169,7 @@
         <v>211</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H10" s="103"/>
     </row>
@@ -8161,13 +8185,13 @@
         <v>345</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F11" s="61" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H11" s="99" t="s">
         <v>357</v>
@@ -8184,10 +8208,10 @@
         <v>203</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G12" s="46" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H12" s="100"/>
     </row>
@@ -8221,13 +8245,13 @@
         <v>345</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G14" s="61" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H14" s="99" t="s">
         <v>347</v>
@@ -8241,13 +8265,13 @@
         <v>348</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F15" s="46" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H15" s="100"/>
     </row>
@@ -8262,10 +8286,10 @@
         <v>168</v>
       </c>
       <c r="F16" s="59" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G16" s="59" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H16" s="103"/>
     </row>
@@ -8319,7 +8343,7 @@
         <v>349</v>
       </c>
       <c r="E19" s="59" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F19" s="59" t="s">
         <v>352</v>
@@ -8404,10 +8428,10 @@
         <v>148</v>
       </c>
       <c r="F23" s="61" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G23" s="61" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H23" s="102" t="s">
         <v>355</v>
@@ -8424,10 +8448,10 @@
         <v>148</v>
       </c>
       <c r="F24" s="46" t="s">
+        <v>474</v>
+      </c>
+      <c r="G24" s="46" t="s">
         <v>476</v>
-      </c>
-      <c r="G24" s="46" t="s">
-        <v>478</v>
       </c>
       <c r="H24" s="100"/>
     </row>
@@ -8442,10 +8466,10 @@
         <v>148</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G25" s="47" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H25" s="101"/>
     </row>
@@ -8503,10 +8527,10 @@
         <v>345</v>
       </c>
       <c r="E29" s="75" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F29" s="64" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="G29" s="76" t="s">
         <v>456</v>
@@ -8523,10 +8547,10 @@
         <v>348</v>
       </c>
       <c r="E30" s="79" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F30" s="71" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="G30" s="77" t="s">
         <v>209</v>
@@ -8541,13 +8565,13 @@
         <v>349</v>
       </c>
       <c r="E31" s="78" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H31" s="103"/>
     </row>
@@ -8563,13 +8587,13 @@
         <v>345</v>
       </c>
       <c r="E32" s="73" t="s">
+        <v>537</v>
+      </c>
+      <c r="F32" s="80" t="s">
+        <v>538</v>
+      </c>
+      <c r="G32" s="73" t="s">
         <v>539</v>
-      </c>
-      <c r="F32" s="80" t="s">
-        <v>540</v>
-      </c>
-      <c r="G32" s="73" t="s">
-        <v>541</v>
       </c>
       <c r="H32" s="100" t="s">
         <v>347</v>
@@ -8583,13 +8607,13 @@
         <v>348</v>
       </c>
       <c r="E33" s="79" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F33" s="71" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="G33" s="79" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="H33" s="100"/>
     </row>
@@ -8601,13 +8625,13 @@
         <v>349</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F34" s="81" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="G34" s="67" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="H34" s="100"/>
     </row>
@@ -8623,13 +8647,13 @@
         <v>345</v>
       </c>
       <c r="E35" s="75" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="G35" s="75" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H35" s="99" t="s">
         <v>347</v>
@@ -8643,13 +8667,13 @@
         <v>348</v>
       </c>
       <c r="E36" s="79" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F36" s="79" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="G36" s="79" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H36" s="100"/>
     </row>
@@ -8661,13 +8685,13 @@
         <v>349</v>
       </c>
       <c r="E37" s="90" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F37" s="90" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G37" s="90" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="H37" s="100"/>
     </row>
@@ -8683,13 +8707,13 @@
         <v>345</v>
       </c>
       <c r="E38" s="63" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F38" s="85" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="G38" s="63" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H38" s="99" t="s">
         <v>371</v>
@@ -8703,13 +8727,13 @@
         <v>348</v>
       </c>
       <c r="E39" s="79" t="s">
+        <v>508</v>
+      </c>
+      <c r="F39" s="71" t="s">
         <v>510</v>
       </c>
-      <c r="F39" s="71" t="s">
-        <v>512</v>
-      </c>
       <c r="G39" s="79" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H39" s="100"/>
     </row>
@@ -8721,13 +8745,13 @@
         <v>349</v>
       </c>
       <c r="E40" s="67" t="s">
+        <v>509</v>
+      </c>
+      <c r="F40" s="81" t="s">
         <v>511</v>
       </c>
-      <c r="F40" s="81" t="s">
-        <v>513</v>
-      </c>
       <c r="G40" s="67" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H40" s="100"/>
     </row>
@@ -8743,13 +8767,13 @@
         <v>345</v>
       </c>
       <c r="E41" s="86" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F41" s="80" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="G41" s="86" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H41" s="99" t="s">
         <v>347</v>
@@ -8763,13 +8787,13 @@
         <v>348</v>
       </c>
       <c r="E42" s="87" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F42" s="88" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G42" s="87" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H42" s="100"/>
     </row>
@@ -8781,13 +8805,13 @@
         <v>349</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F43" s="89" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="G43" s="67" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H43" s="100"/>
     </row>
@@ -8803,13 +8827,13 @@
         <v>345</v>
       </c>
       <c r="E44" s="68" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="G44" s="68" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H44" s="99" t="s">
         <v>347</v>
@@ -8823,13 +8847,13 @@
         <v>348</v>
       </c>
       <c r="E45" s="69" t="s">
+        <v>527</v>
+      </c>
+      <c r="F45" s="69" t="s">
         <v>529</v>
       </c>
-      <c r="F45" s="69" t="s">
-        <v>531</v>
-      </c>
       <c r="G45" s="69" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H45" s="100"/>
     </row>
@@ -8841,13 +8865,13 @@
         <v>349</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F46" s="81" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="G46" s="67" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H46" s="100"/>
     </row>
@@ -8866,10 +8890,10 @@
         <v>158</v>
       </c>
       <c r="F47" s="80" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="G47" s="63" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H47" s="99" t="s">
         <v>347</v>
@@ -8883,13 +8907,13 @@
         <v>348</v>
       </c>
       <c r="E48" s="70" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F48" s="83" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="G48" s="70" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H48" s="100"/>
     </row>
@@ -8901,31 +8925,27 @@
         <v>349</v>
       </c>
       <c r="E49" s="84" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F49" s="72" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G49" s="84" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H49" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="H11:H13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8954,6 +8974,10 @@
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="H23:H25"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="H41:H43"/>
@@ -9453,7 +9477,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9492,9 +9516,6 @@
       <c r="B4" s="52"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>459</v>
-      </c>
       <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -9505,14 +9526,11 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>461</v>
-      </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -9520,53 +9538,53 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>553</v>
-      </c>
       <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>557</v>
+      </c>
       <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -9629,9 +9647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FC119D-A7BC-46FE-BE1D-3900F19AB624}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E31" sqref="E31"/>
+      <selection pane="topRight" activeCell="A6" activeCellId="1" sqref="A7:XFD7 A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10776,7 +10794,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -16399,7 +16417,7 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B53">
         <v>21</v>
@@ -16481,7 +16499,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B54">
         <v>19</v>
@@ -19665,8 +19683,8 @@
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y8" sqref="Y8"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20288,13 +20306,88 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="X8" t="e" cm="1">
-        <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y8" t="e" cm="1">
-        <f t="array" aca="1" ref="Y8" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
-        <v>#N/A</v>
+      <c r="A8" t="s">
+        <v>551</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>15000</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8">
+        <v>150</v>
+      </c>
+      <c r="I8">
+        <v>50</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>60</v>
+      </c>
+      <c r="N8" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8">
+        <v>11</v>
+      </c>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8">
+        <v>200</v>
+      </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8" t="s">
+        <v>76</v>
+      </c>
+      <c r="W8" t="s">
+        <v>551</v>
+      </c>
+      <c r="X8" cm="1">
+        <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B34:'Caliber'!C44,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B44,0),2)</f>
+        <v>95</v>
+      </c>
+      <c r="Y8" cm="1">
+        <f t="array" aca="1" ref="Y8" ca="1">INDEX(Caliber!C34:'Caliber'!D44,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B44,0),2)</f>
+        <v>0.75</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Breaching test map, M3 Grease gun, More item sets
Breaching test map available in battle mode.
M3 Grease gun added.
Further updated enemy weapon sets.
Golden deagle sell price increased.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F1857E-5A3A-4503-9335-5CBEA08AFC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBBAFDB-0DEE-4FDF-9716-7000B645EE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="6" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -68,105 +68,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{F961D446-80F7-4740-8D09-8E547E874BD0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>not done</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{413C27F9-840C-445F-AE1C-9C72748498BE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>To do</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C35" authorId="0" shapeId="0" xr:uid="{79B2E535-7BE6-4DF7-9994-F181BCCBC2B1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Todo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C38" authorId="0" shapeId="0" xr:uid="{E5162356-75C5-4120-B89A-CCF95984A146}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Not done</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C41" authorId="0" shapeId="0" xr:uid="{5EE6B0E6-6D2A-4BD6-8636-DF8E146E6D4C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Not implemented
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C44" authorId="0" shapeId="0" xr:uid="{AB5D669A-4A56-4B99-80F1-E0326CBC8A62}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>not done</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C47" authorId="0" shapeId="0" xr:uid="{C488CF59-D99C-43D3-8A24-69628144FAD3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Not done</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -218,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="563">
   <si>
     <t>Name</t>
   </si>
@@ -1813,9 +1714,6 @@
     <t>Origin 12 (NL)/USAS 12(NL)/USAS 12</t>
   </si>
   <si>
-    <t>AA-12(NL)/Serbu (Breach)/Serbu</t>
-  </si>
-  <si>
     <t>Origin 12/USAS 12/Origin 12 (Slug)</t>
   </si>
   <si>
@@ -1834,9 +1732,6 @@
     <t>Mk 18 Mod 0 (SOPMOD)/Scar L (Sopmod)/Scar H</t>
   </si>
   <si>
-    <t>SCAR L/M4 Carbine/FX-05</t>
-  </si>
-  <si>
     <t>AK-12/AK-12 (Scoped)/?</t>
   </si>
   <si>
@@ -1867,15 +1762,9 @@
     <t>RPK</t>
   </si>
   <si>
-    <t>Negev/M60/Negev</t>
-  </si>
-  <si>
     <t>M249/M60/M249</t>
   </si>
   <si>
-    <t>Mk48/Negev/M60</t>
-  </si>
-  <si>
     <t>MK48/Negev/MK48</t>
   </si>
   <si>
@@ -1964,6 +1853,27 @@
   </si>
   <si>
     <t>Single Use</t>
+  </si>
+  <si>
+    <t>M3 Grease Gun</t>
+  </si>
+  <si>
+    <t>M3 Grease Gun/TEC-9/M3 Grease Gun</t>
+  </si>
+  <si>
+    <t>M3 Grease Gun/Double Barrel/Skorpion</t>
+  </si>
+  <si>
+    <t>M3 Grease Gun/TEC-9/M3 Grease Gun + (1 Grenade)</t>
+  </si>
+  <si>
+    <t>AA-12(NL)/Serbu/Serbu (Breach)</t>
+  </si>
+  <si>
+    <t>Negev/M60/CBJ-MS (SAW)</t>
+  </si>
+  <si>
+    <t>Mk48/Negev/CBJ-MS (SAW)</t>
   </si>
 </sst>
 </file>
@@ -2643,7 +2553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2895,13 +2805,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2931,6 +2841,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3646,8 +3557,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB47442F-754D-45A1-BC57-BBE7964D0858}" name="Table10" displayName="Table10" ref="A1:Z15" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
-  <autoFilter ref="A1:Z15" xr:uid="{EB47442F-754D-45A1-BC57-BBE7964D0858}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{EB47442F-754D-45A1-BC57-BBE7964D0858}" name="Table10" displayName="Table10" ref="A1:Z16" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A1:Z16" xr:uid="{EB47442F-754D-45A1-BC57-BBE7964D0858}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z15">
     <sortCondition descending="1" ref="M1:M15"/>
   </sortState>
@@ -5512,7 +5423,7 @@
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C43">
         <v>95</v>
@@ -5530,7 +5441,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -7946,9 +7857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7956,9 +7867,9 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" customWidth="1"/>
+    <col min="7" max="7" width="46.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="30.140625" customWidth="1"/>
   </cols>
@@ -8097,8 +8008,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
@@ -8111,7 +8022,7 @@
       <c r="G7" s="59" t="s">
         <v>491</v>
       </c>
-      <c r="H7" s="103"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="100"/>
@@ -8157,8 +8068,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8171,7 +8082,7 @@
       <c r="G10" s="59" t="s">
         <v>497</v>
       </c>
-      <c r="H10" s="103"/>
+      <c r="H10" s="101"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="100"/>
@@ -8277,13 +8188,13 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="103"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="101"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>168</v>
+        <v>558</v>
       </c>
       <c r="F16" s="59" t="s">
         <v>465</v>
@@ -8291,7 +8202,7 @@
       <c r="G16" s="59" t="s">
         <v>468</v>
       </c>
-      <c r="H16" s="103"/>
+      <c r="H16" s="101"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="100"/>
@@ -8328,17 +8239,17 @@
         <v>11</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>111</v>
+        <v>352</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="H18" s="100"/>
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
-      <c r="B19" s="103"/>
-      <c r="C19" s="103"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="101"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8346,12 +8257,12 @@
         <v>464</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>352</v>
+        <v>557</v>
       </c>
       <c r="G19" s="59" t="s">
-        <v>362</v>
-      </c>
-      <c r="H19" s="103"/>
+        <v>559</v>
+      </c>
+      <c r="H19" s="101"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="100"/>
@@ -8411,7 +8322,7 @@
       <c r="G22" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="H22" s="101"/>
+      <c r="H22" s="103"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="100"/>
@@ -8456,9 +8367,9 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="101"/>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
@@ -8471,7 +8382,7 @@
       <c r="G25" s="47" t="s">
         <v>475</v>
       </c>
-      <c r="H25" s="101"/>
+      <c r="H25" s="103"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="102" t="s">
@@ -8527,10 +8438,10 @@
         <v>345</v>
       </c>
       <c r="E29" s="75" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="F29" s="64" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="G29" s="76" t="s">
         <v>456</v>
@@ -8547,10 +8458,10 @@
         <v>348</v>
       </c>
       <c r="E30" s="79" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="F30" s="71" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="G30" s="77" t="s">
         <v>209</v>
@@ -8559,21 +8470,21 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="100"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E31" s="78" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>542</v>
-      </c>
-      <c r="H31" s="103"/>
+        <v>538</v>
+      </c>
+      <c r="H31" s="101"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="100"/>
@@ -8587,13 +8498,13 @@
         <v>345</v>
       </c>
       <c r="E32" s="73" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="F32" s="80" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="G32" s="73" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="H32" s="100" t="s">
         <v>347</v>
@@ -8607,13 +8518,13 @@
         <v>348</v>
       </c>
       <c r="E33" s="79" t="s">
+        <v>532</v>
+      </c>
+      <c r="F33" s="71" t="s">
         <v>536</v>
       </c>
-      <c r="F33" s="71" t="s">
-        <v>540</v>
-      </c>
       <c r="G33" s="79" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="H33" s="100"/>
     </row>
@@ -8625,13 +8536,13 @@
         <v>349</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="F34" s="81" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="G34" s="67" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="H34" s="100"/>
     </row>
@@ -8647,13 +8558,13 @@
         <v>345</v>
       </c>
       <c r="E35" s="75" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G35" s="75" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H35" s="99" t="s">
         <v>347</v>
@@ -8667,13 +8578,13 @@
         <v>348</v>
       </c>
       <c r="E36" s="79" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F36" s="79" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G36" s="79" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H36" s="100"/>
     </row>
@@ -8685,13 +8596,13 @@
         <v>349</v>
       </c>
       <c r="E37" s="90" t="s">
-        <v>516</v>
+        <v>482</v>
       </c>
       <c r="F37" s="90" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G37" s="90" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H37" s="100"/>
     </row>
@@ -8713,7 +8624,7 @@
         <v>506</v>
       </c>
       <c r="G38" s="63" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H38" s="99" t="s">
         <v>371</v>
@@ -8730,10 +8641,10 @@
         <v>508</v>
       </c>
       <c r="F39" s="71" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G39" s="79" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H39" s="100"/>
     </row>
@@ -8745,13 +8656,13 @@
         <v>349</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>509</v>
+        <v>560</v>
       </c>
       <c r="F40" s="81" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G40" s="67" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H40" s="100"/>
     </row>
@@ -8827,13 +8738,13 @@
         <v>345</v>
       </c>
       <c r="E44" s="68" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="G44" s="68" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="H44" s="99" t="s">
         <v>347</v>
@@ -8847,13 +8758,13 @@
         <v>348</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>527</v>
+        <v>561</v>
       </c>
       <c r="F45" s="69" t="s">
-        <v>529</v>
+        <v>562</v>
       </c>
       <c r="G45" s="69" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="H45" s="100"/>
     </row>
@@ -8865,13 +8776,13 @@
         <v>349</v>
       </c>
       <c r="E46" s="67" t="s">
+        <v>525</v>
+      </c>
+      <c r="F46" s="81" t="s">
+        <v>527</v>
+      </c>
+      <c r="G46" s="67" t="s">
         <v>528</v>
-      </c>
-      <c r="F46" s="81" t="s">
-        <v>531</v>
-      </c>
-      <c r="G46" s="67" t="s">
-        <v>532</v>
       </c>
       <c r="H46" s="100"/>
     </row>
@@ -8890,7 +8801,7 @@
         <v>158</v>
       </c>
       <c r="F47" s="80" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="G47" s="63" t="s">
         <v>477</v>
@@ -8907,45 +8818,64 @@
         <v>348</v>
       </c>
       <c r="E48" s="70" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F48" s="83" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="G48" s="70" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="101"/>
-      <c r="B49" s="101"/>
-      <c r="C49" s="101"/>
+      <c r="A49" s="103"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="103"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
       <c r="E49" s="84" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F49" s="72" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="G49" s="84" t="s">
-        <v>520</v>
-      </c>
-      <c r="H49" s="101"/>
+        <v>518</v>
+      </c>
+      <c r="H49" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8962,34 +8892,15 @@
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="H35:H37"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9476,7 +9387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -9538,13 +9449,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="B12" s="14"/>
     </row>
@@ -9553,37 +9464,37 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B19" s="14"/>
     </row>
@@ -9647,7 +9558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FC119D-A7BC-46FE-BE1D-3900F19AB624}">
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A6" activeCellId="1" sqref="A7:XFD7 A6:XFD6"/>
     </sheetView>
@@ -10881,16 +10792,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
@@ -12098,6 +12009,85 @@
         <v>434</v>
       </c>
     </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>556</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>80</v>
+      </c>
+      <c r="G16">
+        <v>115</v>
+      </c>
+      <c r="H16">
+        <v>40</v>
+      </c>
+      <c r="I16">
+        <v>35</v>
+      </c>
+      <c r="J16">
+        <v>45</v>
+      </c>
+      <c r="K16">
+        <v>55</v>
+      </c>
+      <c r="L16">
+        <v>65</v>
+      </c>
+      <c r="M16">
+        <v>35</v>
+      </c>
+      <c r="N16">
+        <v>9</v>
+      </c>
+      <c r="O16">
+        <v>11</v>
+      </c>
+      <c r="P16">
+        <v>7</v>
+      </c>
+      <c r="Q16">
+        <v>30</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>6</v>
+      </c>
+      <c r="V16" t="s">
+        <v>14</v>
+      </c>
+      <c r="W16" s="113">
+        <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V16,Caliber!B2:'Caliber'!B9,0),2)</f>
+        <v>35</v>
+      </c>
+      <c r="X16" s="113">
+        <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V16,Caliber!B2:'Caliber'!B9,0),2)</f>
+        <v>0.1</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -12111,7 +12101,7 @@
   <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
@@ -20307,7 +20297,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -20373,7 +20363,7 @@
         <v>76</v>
       </c>
       <c r="W8" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="X8" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B34:'Caliber'!C44,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B44,0),2)</f>
@@ -20387,7 +20377,7 @@
         <v>82</v>
       </c>
       <c r="AA8" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AK-74 w/ GP-25, vog-25 and grd-50 40mm nades
Added AK-74 w/ GP-25,
VOG-25 40mm frag grenade (missing sprite)
GRD-50 40mm Smoke grenade (missing sprite)
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBBAFDB-0DEE-4FDF-9716-7000B645EE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3C68CB-7752-4BFD-8F30-B621E8C6EE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="6" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="569">
   <si>
     <t>Name</t>
   </si>
@@ -1874,6 +1874,24 @@
   </si>
   <si>
     <t>Mk48/Negev/CBJ-MS (SAW)</t>
+  </si>
+  <si>
+    <t>Snap</t>
+  </si>
+  <si>
+    <t>[30,45,60][1]</t>
+  </si>
+  <si>
+    <t>AK-74 (GP-25)</t>
+  </si>
+  <si>
+    <t>Arcing</t>
+  </si>
+  <si>
+    <t>VOG-25 (Frag)</t>
+  </si>
+  <si>
+    <t>GRD-50 (Smoke)</t>
   </si>
 </sst>
 </file>
@@ -2805,13 +2823,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2841,7 +2859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3502,8 +3520,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{04AB2E62-598B-4666-8BAF-7BB7165BB6E6}" name="Table8" displayName="Table8" ref="B33:I44" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="B33:I44" xr:uid="{04AB2E62-598B-4666-8BAF-7BB7165BB6E6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{04AB2E62-598B-4666-8BAF-7BB7165BB6E6}" name="Table8" displayName="Table8" ref="B33:I46" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="B33:I46" xr:uid="{04AB2E62-598B-4666-8BAF-7BB7165BB6E6}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B4CC4C1E-3374-4B26-96BC-04C93FD2A144}" name="Name"/>
     <tableColumn id="2" xr3:uid="{C06185A8-6720-4F80-8AB3-39A31D26270F}" name="Power" dataDxfId="25"/>
@@ -3595,8 +3613,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8241084F-89A0-47CD-965A-F8C6F1FCBC05}" name="Table2" displayName="Table2" ref="A1:AA54" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A1:AA54" xr:uid="{8241084F-89A0-47CD-965A-F8C6F1FCBC05}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8241084F-89A0-47CD-965A-F8C6F1FCBC05}" name="Table2" displayName="Table2" ref="A1:AA55" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:AA55" xr:uid="{8241084F-89A0-47CD-965A-F8C6F1FCBC05}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA52">
     <sortCondition ref="A1:A52"/>
   </sortState>
@@ -4003,10 +4021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5446,54 +5464,108 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
+      <c r="B44" t="s">
+        <v>567</v>
+      </c>
+      <c r="C44">
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <v>0.4</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>3</v>
+      </c>
+      <c r="I44" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="53" t="s">
+      <c r="A45" s="9"/>
+      <c r="B45" t="s">
+        <v>568</v>
+      </c>
+      <c r="C45" s="113">
+        <v>40</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45" s="113">
+        <v>5</v>
+      </c>
+      <c r="F45" s="113">
+        <v>1</v>
+      </c>
+      <c r="G45" s="113">
+        <v>9</v>
+      </c>
+      <c r="H45" s="113"/>
+      <c r="I45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="C46" s="113"/>
+      <c r="E46" s="113"/>
+      <c r="F46" s="113"/>
+      <c r="G46" s="113"/>
+      <c r="H46" s="113"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="53" t="s">
         <v>451</v>
       </c>
-      <c r="B45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
         <v>2</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>4</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E47" t="s">
         <v>6</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F47" t="s">
         <v>7</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G47" t="s">
         <v>56</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H47" t="s">
         <v>57</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
-      <c r="B46" s="14" t="s">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="54"/>
+      <c r="B48" s="14" t="s">
         <v>442</v>
       </c>
-      <c r="C46">
+      <c r="C48">
         <v>40</v>
       </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
         <v>6</v>
       </c>
-      <c r="F46">
+      <c r="F48">
         <v>7</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I48" t="s">
         <v>443</v>
       </c>
     </row>
@@ -7857,8 +7929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C47" sqref="C47:C49"/>
     </sheetView>
   </sheetViews>
@@ -8008,8 +8080,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
@@ -8022,7 +8094,7 @@
       <c r="G7" s="59" t="s">
         <v>491</v>
       </c>
-      <c r="H7" s="101"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="100"/>
@@ -8068,8 +8140,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8082,7 +8154,7 @@
       <c r="G10" s="59" t="s">
         <v>497</v>
       </c>
-      <c r="H10" s="101"/>
+      <c r="H10" s="103"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="100"/>
@@ -8188,8 +8260,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
@@ -8202,7 +8274,7 @@
       <c r="G16" s="59" t="s">
         <v>468</v>
       </c>
-      <c r="H16" s="101"/>
+      <c r="H16" s="103"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="100"/>
@@ -8248,8 +8320,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8262,7 +8334,7 @@
       <c r="G19" s="59" t="s">
         <v>559</v>
       </c>
-      <c r="H19" s="101"/>
+      <c r="H19" s="103"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="100"/>
@@ -8322,7 +8394,7 @@
       <c r="G22" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="H22" s="103"/>
+      <c r="H22" s="101"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="100"/>
@@ -8367,9 +8439,9 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="103"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
@@ -8382,7 +8454,7 @@
       <c r="G25" s="47" t="s">
         <v>475</v>
       </c>
-      <c r="H25" s="103"/>
+      <c r="H25" s="101"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="102" t="s">
@@ -8470,8 +8542,8 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="100"/>
-      <c r="B31" s="101"/>
-      <c r="C31" s="101"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
@@ -8484,7 +8556,7 @@
       <c r="G31" s="78" t="s">
         <v>538</v>
       </c>
-      <c r="H31" s="101"/>
+      <c r="H31" s="103"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="100"/>
@@ -8829,9 +8901,9 @@
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="103"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="103"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
@@ -8844,22 +8916,35 @@
       <c r="G49" s="84" t="s">
         <v>518</v>
       </c>
-      <c r="H49" s="103"/>
+      <c r="H49" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="H35:H37"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8876,31 +8961,18 @@
     <mergeCell ref="H17:H19"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12076,11 +12148,11 @@
       <c r="V16" t="s">
         <v>14</v>
       </c>
-      <c r="W16" s="113">
+      <c r="W16" s="10">
         <f>INDEX(Caliber!B2:'Caliber'!C9,MATCH(V16,Caliber!B2:'Caliber'!B9,0),2)</f>
         <v>35</v>
       </c>
-      <c r="X16" s="113">
+      <c r="X16" s="10">
         <f>INDEX(Caliber!C2:'Caliber'!D9,MATCH(V16,Caliber!B2:'Caliber'!B9,0),2)</f>
         <v>0.1</v>
       </c>
@@ -12098,13 +12170,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E308052D-1B88-4699-843E-12AA607B59B8}">
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16570,12 +16642,94 @@
       </c>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="X55" t="e" cm="1">
+      <c r="A55" t="s">
+        <v>565</v>
+      </c>
+      <c r="B55">
+        <v>31</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E55" t="s">
+        <v>563</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>50</v>
+      </c>
+      <c r="H55">
+        <v>125</v>
+      </c>
+      <c r="I55">
+        <v>55</v>
+      </c>
+      <c r="J55">
+        <v>70</v>
+      </c>
+      <c r="K55">
+        <v>60</v>
+      </c>
+      <c r="L55">
+        <v>50</v>
+      </c>
+      <c r="M55">
+        <v>35</v>
+      </c>
+      <c r="N55">
+        <v>35</v>
+      </c>
+      <c r="O55">
+        <v>24</v>
+      </c>
+      <c r="P55">
+        <v>16</v>
+      </c>
+      <c r="Q55">
+        <v>10</v>
+      </c>
+      <c r="R55">
+        <v>200</v>
+      </c>
+      <c r="S55">
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <v>3</v>
+      </c>
+      <c r="U55">
+        <v>1</v>
+      </c>
+      <c r="V55">
+        <v>5</v>
+      </c>
+      <c r="W55" t="s">
+        <v>19</v>
+      </c>
+      <c r="X55" cm="1">
         <f t="array" aca="1" ref="X55" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>36</v>
+      </c>
+      <c r="Y55" cm="1">
+        <f t="array" aca="1" ref="Y55" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>0.3</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="X56" t="e" cm="1">
+        <f t="array" aca="1" ref="X56" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>#N/A</v>
       </c>
-      <c r="Y55" t="e" cm="1">
-        <f t="array" aca="1" ref="Y55" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y56" t="e" cm="1">
+        <f t="array" aca="1" ref="Y56" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
M1 Garand, Buffed Hunting rifle
Added .30-06 ammo
Added M1 Garand, M1D Garand
Buffed hunting rifle weight and accuracy
Nerfed M9
Updated enemy item sets to include M1 Garand
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076A50EB-FD2E-4D86-BD33-8BB2ACBEFD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3626016F-2BD1-4117-896D-4C00E4CDA116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="578">
   <si>
     <t>Name</t>
   </si>
@@ -1898,6 +1898,27 @@
   </si>
   <si>
     <t>M110 or M2010</t>
+  </si>
+  <si>
+    <t>M60E6</t>
+  </si>
+  <si>
+    <t>.30-06</t>
+  </si>
+  <si>
+    <t>Unscoped, Sling</t>
+  </si>
+  <si>
+    <t>M1D Garand</t>
+  </si>
+  <si>
+    <t>Sling</t>
+  </si>
+  <si>
+    <t>M1 Garand/M1D Garand/Hunting Rifle</t>
+  </si>
+  <si>
+    <t>Hunting Rifle/Hunting Rifle/M1 Garand</t>
   </si>
 </sst>
 </file>
@@ -2577,7 +2598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2865,6 +2886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3491,8 +3513,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4EBB74B-543A-4247-8D65-0E143A9BEBA4}" name="Table6" displayName="Table6" ref="B12:I23" totalsRowShown="0" dataDxfId="44" tableBorderDxfId="43">
-  <autoFilter ref="B12:I23" xr:uid="{A4EBB74B-543A-4247-8D65-0E143A9BEBA4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A4EBB74B-543A-4247-8D65-0E143A9BEBA4}" name="Table6" displayName="Table6" ref="B12:I24" totalsRowShown="0" dataDxfId="44" tableBorderDxfId="43">
+  <autoFilter ref="B12:I24" xr:uid="{A4EBB74B-543A-4247-8D65-0E143A9BEBA4}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A8C7ABBF-D256-4E65-A96F-CB8C79043F13}" name="Name"/>
     <tableColumn id="2" xr3:uid="{FF6CFE34-0508-4CB9-AB47-C96085BF18D3}" name="Power" dataDxfId="42"/>
@@ -3508,8 +3530,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{664A7A36-F4CD-41BE-9150-5714BC53B38A}" name="Table7" displayName="Table7" ref="B24:I32" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
-  <autoFilter ref="B24:I32" xr:uid="{664A7A36-F4CD-41BE-9150-5714BC53B38A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{664A7A36-F4CD-41BE-9150-5714BC53B38A}" name="Table7" displayName="Table7" ref="B25:I33" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+  <autoFilter ref="B25:I33" xr:uid="{664A7A36-F4CD-41BE-9150-5714BC53B38A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B572F9F5-F31A-42DA-93B6-64F0EE8AB069}" name="Name"/>
     <tableColumn id="2" xr3:uid="{7722C74B-D75C-4FB4-B0CE-8B2513EB63AB}" name="Power" dataDxfId="33"/>
@@ -3525,8 +3547,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{04AB2E62-598B-4666-8BAF-7BB7165BB6E6}" name="Table8" displayName="Table8" ref="B33:I46" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
-  <autoFilter ref="B33:I46" xr:uid="{04AB2E62-598B-4666-8BAF-7BB7165BB6E6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{04AB2E62-598B-4666-8BAF-7BB7165BB6E6}" name="Table8" displayName="Table8" ref="B34:I47" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="B34:I47" xr:uid="{04AB2E62-598B-4666-8BAF-7BB7165BB6E6}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B4CC4C1E-3374-4B26-96BC-04C93FD2A144}" name="Name"/>
     <tableColumn id="2" xr3:uid="{C06185A8-6720-4F80-8AB3-39A31D26270F}" name="Power" dataDxfId="25"/>
@@ -4026,10 +4048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4707,33 +4729,24 @@
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="11" t="s">
+      <c r="A24" s="5"/>
+      <c r="B24" t="s">
+        <v>572</v>
+      </c>
+      <c r="C24" s="113">
+        <v>40</v>
+      </c>
+      <c r="D24" s="113">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="113">
         <v>6</v>
       </c>
-      <c r="H24" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" t="s">
-        <v>21</v>
-      </c>
+      <c r="F24" s="113">
+        <v>1</v>
+      </c>
+      <c r="G24" s="113"/>
+      <c r="H24" s="113"/>
       <c r="M24" s="14" t="s">
         <v>34</v>
       </c>
@@ -4757,29 +4770,33 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="1">
-        <v>25</v>
-      </c>
-      <c r="D25" s="1">
-        <v>10</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1</v>
-      </c>
-      <c r="I25" s="1"/>
+      <c r="A25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" t="s">
+        <v>21</v>
+      </c>
       <c r="M25" s="15" t="s">
         <v>35</v>
       </c>
@@ -4803,28 +4820,29 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26">
-        <v>45</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26">
-        <v>0.7</v>
-      </c>
-      <c r="G26">
-        <v>6</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
+      <c r="A26" s="6"/>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1"/>
       <c r="M26" s="14" t="s">
         <v>37</v>
       </c>
@@ -4850,28 +4868,25 @@
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D27">
-        <v>10</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H27">
         <v>1</v>
-      </c>
-      <c r="I27" t="s">
-        <v>36</v>
       </c>
       <c r="M27" s="15" t="s">
         <v>38</v>
@@ -4898,10 +4913,10 @@
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
-        <v>448</v>
+        <v>35</v>
       </c>
       <c r="C28">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <v>10</v>
@@ -4919,7 +4934,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>449</v>
+        <v>36</v>
       </c>
       <c r="M28" s="16" t="s">
         <v>39</v>
@@ -4946,16 +4961,16 @@
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C29">
+        <v>25</v>
+      </c>
+      <c r="D29">
         <v>10</v>
       </c>
-      <c r="D29">
-        <v>4</v>
-      </c>
       <c r="E29">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -4967,23 +4982,23 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>451</v>
       </c>
       <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
         <v>25</v>
       </c>
-      <c r="D30">
-        <v>20</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
       <c r="F30">
         <v>0</v>
       </c>
@@ -4992,6 +5007,9 @@
       </c>
       <c r="H30">
         <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>452</v>
       </c>
       <c r="M30" s="12" t="s">
         <v>41</v>
@@ -5016,22 +5034,22 @@
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -5058,28 +5076,25 @@
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D32">
-        <v>20</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H32">
         <v>1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>36</v>
       </c>
       <c r="M32" s="15" t="s">
         <v>45</v>
@@ -5102,32 +5117,30 @@
       <c r="S32" s="10"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>56</v>
+      <c r="A33" s="7"/>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>20</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="M33" s="14" t="s">
         <v>47</v>
@@ -5149,28 +5162,32 @@
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="1">
-        <v>50</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="E34" s="1">
-        <v>3</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1</v>
-      </c>
-      <c r="G34" s="1">
-        <v>3</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1" t="s">
-        <v>42</v>
+      <c r="A34" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" t="s">
+        <v>21</v>
       </c>
       <c r="M34" s="15" t="s">
         <v>49</v>
@@ -5193,27 +5210,28 @@
       <c r="S34" s="10"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35">
-        <v>40</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>5</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>9</v>
-      </c>
-      <c r="I35" t="s">
-        <v>44</v>
+      <c r="A35" s="8"/>
+      <c r="B35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="1">
+        <v>50</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="M35" s="14" t="s">
         <v>50</v>
@@ -5237,7 +5255,7 @@
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C36">
         <v>40</v>
@@ -5246,16 +5264,16 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F36">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M36" s="15" t="s">
         <v>51</v>
@@ -5280,25 +5298,25 @@
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C37">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M37" s="14" t="s">
         <v>52</v>
@@ -5322,13 +5340,13 @@
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C38">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>3</v>
@@ -5337,7 +5355,10 @@
         <v>1</v>
       </c>
       <c r="G38">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>48</v>
       </c>
       <c r="M38" s="15" t="s">
         <v>53</v>
@@ -5362,16 +5383,16 @@
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D39">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -5383,16 +5404,16 @@
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -5404,10 +5425,10 @@
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -5425,16 +5446,16 @@
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="D42">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -5446,40 +5467,37 @@
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" t="s">
-        <v>545</v>
+        <v>53</v>
       </c>
       <c r="C43">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="D43">
-        <v>0.75</v>
+        <v>0.2</v>
       </c>
       <c r="E43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43">
         <v>3</v>
-      </c>
-      <c r="I43" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="C44">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="D44">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -5488,83 +5506,107 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C45">
         <v>40</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F45">
         <v>1</v>
       </c>
       <c r="G45">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>44</v>
+        <v>564</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
+      <c r="B46" t="s">
+        <v>566</v>
+      </c>
+      <c r="C46">
+        <v>40</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>9</v>
+      </c>
+      <c r="I46" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="9"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="53" t="s">
         <v>450</v>
       </c>
-      <c r="B47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
         <v>2</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>4</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E48" t="s">
         <v>6</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F48" t="s">
         <v>7</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G48" t="s">
         <v>56</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H48" t="s">
         <v>57</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I48" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
-      <c r="B48" s="14" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="54"/>
+      <c r="B49" s="14" t="s">
         <v>441</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>40</v>
       </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
         <v>6</v>
       </c>
-      <c r="F48">
+      <c r="F49">
         <v>7</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I49" t="s">
         <v>442</v>
       </c>
     </row>
@@ -7928,9 +7970,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8427,7 +8469,7 @@
         <v>348</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>148</v>
+        <v>577</v>
       </c>
       <c r="F24" s="46" t="s">
         <v>473</v>
@@ -8445,7 +8487,7 @@
         <v>349</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>148</v>
+        <v>576</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>471</v>
@@ -9459,7 +9501,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9573,6 +9615,9 @@
       <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>571</v>
+      </c>
       <c r="B21" s="14"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -9631,7 +9676,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A6" activeCellId="1" sqref="A7:XFD7 A6:XFD6"/>
+      <selection pane="topRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10797,10 +10842,10 @@
         <v>100</v>
       </c>
       <c r="H15">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I15">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J15" t="s">
         <v>76</v>
@@ -10865,9 +10910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X17" sqref="X17"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12172,10 +12217,10 @@
   <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A56" sqref="A56"/>
+      <selection pane="bottomRight" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16746,7 +16791,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A12" activeCellId="2" sqref="A4:XFD4 A10:XFD10 A12:XFD12"/>
+      <selection pane="topRight" activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16864,7 +16909,7 @@
         <v>148</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
@@ -16894,10 +16939,10 @@
         <v>76</v>
       </c>
       <c r="L2">
+        <v>105</v>
+      </c>
+      <c r="M2">
         <v>80</v>
-      </c>
-      <c r="M2">
-        <v>40</v>
       </c>
       <c r="N2" t="s">
         <v>76</v>
@@ -16915,7 +16960,7 @@
         <v>200</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T2">
         <v>1</v>
@@ -17844,23 +17889,173 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="X14" t="e">
-        <f>INDEX(Caliber!B13:'Caliber'!C23,MATCH(W14,Caliber!B13:'Caliber'!B23,0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y14" t="e">
-        <f>INDEX(Caliber!C13:'Caliber'!D23,MATCH(W14,Caliber!B13:'Caliber'!B23,0),2)</f>
-        <v>#N/A</v>
+      <c r="A14" t="s">
+        <v>547</v>
+      </c>
+      <c r="B14">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14">
+        <v>130</v>
+      </c>
+      <c r="I14">
+        <v>80</v>
+      </c>
+      <c r="J14">
+        <v>45</v>
+      </c>
+      <c r="K14" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14">
+        <v>80</v>
+      </c>
+      <c r="M14">
+        <v>60</v>
+      </c>
+      <c r="N14" t="s">
+        <v>76</v>
+      </c>
+      <c r="O14">
+        <v>30</v>
+      </c>
+      <c r="P14">
+        <v>20</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>76</v>
+      </c>
+      <c r="R14">
+        <v>200</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14" t="s">
+        <v>76</v>
+      </c>
+      <c r="W14" t="s">
+        <v>572</v>
+      </c>
+      <c r="X14">
+        <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W14,Caliber!B13:'Caliber'!B24,0),2)</f>
+        <v>40</v>
+      </c>
+      <c r="Y14">
+        <f>INDEX(Caliber!C13:'Caliber'!D24,MATCH(W14,Caliber!B13:'Caliber'!B24,0),2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="X15" t="e">
-        <f>INDEX(Caliber!B13:'Caliber'!C23,MATCH(W15,Caliber!B13:'Caliber'!B23,0),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y15" t="e">
-        <f>INDEX(Caliber!C13:'Caliber'!D23,MATCH(W15,Caliber!B13:'Caliber'!B23,0),2)</f>
-        <v>#N/A</v>
+      <c r="A15" t="s">
+        <v>574</v>
+      </c>
+      <c r="B15">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15">
+        <v>130</v>
+      </c>
+      <c r="I15">
+        <v>85</v>
+      </c>
+      <c r="J15">
+        <v>45</v>
+      </c>
+      <c r="K15" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15">
+        <v>100</v>
+      </c>
+      <c r="M15">
+        <v>55</v>
+      </c>
+      <c r="N15" t="s">
+        <v>76</v>
+      </c>
+      <c r="O15">
+        <v>200</v>
+      </c>
+      <c r="P15">
+        <v>25</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>76</v>
+      </c>
+      <c r="R15">
+        <v>200</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15" t="s">
+        <v>76</v>
+      </c>
+      <c r="W15" t="s">
+        <v>572</v>
+      </c>
+      <c r="X15">
+        <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W15,Caliber!B13:'Caliber'!B24,0),2)</f>
+        <v>40</v>
+      </c>
+      <c r="Y15">
+        <f>INDEX(Caliber!C13:'Caliber'!D24,MATCH(W15,Caliber!B13:'Caliber'!B24,0),2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -18026,7 +18221,7 @@
   <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
@@ -18214,15 +18409,15 @@
         <v>33</v>
       </c>
       <c r="X2">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W2,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W2,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y2">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W2,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W2,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z2">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W2,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W2,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA2" t="s">
@@ -18300,15 +18495,15 @@
         <v>33</v>
       </c>
       <c r="X3">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W3,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W3,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y3">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W3,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W3,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z3">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W3,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W3,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA3" t="s">
@@ -18389,15 +18584,15 @@
         <v>33</v>
       </c>
       <c r="X4">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W4,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W4,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y4">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W4,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W4,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z4">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W4,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W4,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA4" t="s">
@@ -18478,15 +18673,15 @@
         <v>33</v>
       </c>
       <c r="X5">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W5,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W5,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y5">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W5,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W5,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z5">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W5,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W5,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA5" t="s">
@@ -18567,15 +18762,15 @@
         <v>37</v>
       </c>
       <c r="X6">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W6,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W6,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y6">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W6,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W6,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>20</v>
       </c>
       <c r="Z6">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W6,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W6,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA6" t="s">
@@ -18656,15 +18851,15 @@
         <v>33</v>
       </c>
       <c r="X7">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W7,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W7,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y7">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W7,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W7,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z7">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W7,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W7,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA7" t="s">
@@ -18745,15 +18940,15 @@
         <v>33</v>
       </c>
       <c r="X8">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W8,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W8,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y8">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W8,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W8,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z8">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W8,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W8,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA8" t="s">
@@ -18834,15 +19029,15 @@
         <v>33</v>
       </c>
       <c r="X9">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W9,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W9,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y9">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W9,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W9,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z9">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W9,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W9,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA9" t="s">
@@ -18923,15 +19118,15 @@
         <v>33</v>
       </c>
       <c r="X10">
-        <f>INDEX(Caliber!B25:'Caliber'!C32,MATCH(W10,Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W10,Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y10">
-        <f>INDEX(Caliber!B25:'Caliber'!D32,MATCH(W10,Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W10,Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z10">
-        <f>INDEX(Caliber!B25:'Caliber'!F32,MATCH(W10,Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f>INDEX(Caliber!B26:'Caliber'!F33,MATCH(W10,Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA10" t="s">
@@ -19012,15 +19207,15 @@
         <v>33</v>
       </c>
       <c r="X11" cm="1">
-        <f t="array" aca="1" ref="X11" ca="1">INDEX(Caliber!B25:'Caliber'!C32,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B25:'Caliber'!B32,0),2)</f>
+        <f t="array" aca="1" ref="X11" ca="1">INDEX(Caliber!B26:'Caliber'!C33,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B26:'Caliber'!B33,0),2)</f>
         <v>25</v>
       </c>
       <c r="Y11" cm="1">
-        <f t="array" aca="1" ref="Y11" ca="1">INDEX(Caliber!B25:'Caliber'!D32,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B25:'Caliber'!B32,0),3)</f>
+        <f t="array" aca="1" ref="Y11" ca="1">INDEX(Caliber!B26:'Caliber'!D33,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B26:'Caliber'!B33,0),3)</f>
         <v>10</v>
       </c>
       <c r="Z11" cm="1">
-        <f t="array" aca="1" ref="Z11" ca="1">INDEX(Caliber!B25:'Caliber'!F32,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-3)),Caliber!B25:'Caliber'!B32,0),5)</f>
+        <f t="array" aca="1" ref="Z11" ca="1">INDEX(Caliber!B26:'Caliber'!F33,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-3)),Caliber!B26:'Caliber'!B33,0),5)</f>
         <v>0</v>
       </c>
       <c r="AA11" t="s">
@@ -19825,7 +20020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B2364D-F43A-47E4-8B6C-A03FB84E628E}">
   <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AA11" sqref="AA11"/>
     </sheetView>
@@ -20009,11 +20204,11 @@
         <v>41</v>
       </c>
       <c r="X2" cm="1">
-        <f t="array" aca="1" ref="X2" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X2" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>50</v>
       </c>
       <c r="Y2" cm="1">
-        <f t="array" aca="1" ref="Y2" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y2" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>0.2</v>
       </c>
       <c r="Z2" t="s">
@@ -20094,11 +20289,11 @@
         <v>41</v>
       </c>
       <c r="X3" cm="1">
-        <f t="array" aca="1" ref="X3" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X3" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>50</v>
       </c>
       <c r="Y3" cm="1">
-        <f t="array" aca="1" ref="Y3" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y3" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>0.2</v>
       </c>
       <c r="Z3" t="s">
@@ -20179,11 +20374,11 @@
         <v>41</v>
       </c>
       <c r="X4" cm="1">
-        <f t="array" aca="1" ref="X4" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X4" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>50</v>
       </c>
       <c r="Y4" cm="1">
-        <f t="array" aca="1" ref="Y4" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y4" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>0.2</v>
       </c>
       <c r="Z4" t="s">
@@ -20264,11 +20459,11 @@
         <v>49</v>
       </c>
       <c r="X5" cm="1">
-        <f t="array" aca="1" ref="X5" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X5" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>200</v>
       </c>
       <c r="Y5" cm="1">
-        <f t="array" aca="1" ref="Y5" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y5" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>1</v>
       </c>
       <c r="Z5" t="s">
@@ -20349,11 +20544,11 @@
         <v>51</v>
       </c>
       <c r="X6" cm="1">
-        <f t="array" aca="1" ref="X6" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X6" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>150</v>
       </c>
       <c r="Y6" cm="1">
-        <f t="array" aca="1" ref="Y6" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y6" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>1</v>
       </c>
       <c r="Z6" t="s">
@@ -20434,11 +20629,11 @@
         <v>52</v>
       </c>
       <c r="X7" cm="1">
-        <f t="array" aca="1" ref="X7" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X7" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>190</v>
       </c>
       <c r="Y7" cm="1">
-        <f t="array" aca="1" ref="Y7" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y7" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>1</v>
       </c>
       <c r="Z7" t="s">
@@ -20519,11 +20714,11 @@
         <v>545</v>
       </c>
       <c r="X8" cm="1">
-        <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B34:'Caliber'!C44,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B44,0),2)</f>
+        <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B35:'Caliber'!C45,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B45,0),2)</f>
         <v>95</v>
       </c>
       <c r="Y8" cm="1">
-        <f t="array" aca="1" ref="Y8" ca="1">INDEX(Caliber!C34:'Caliber'!D44,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B44,0),2)</f>
+        <f t="array" aca="1" ref="Y8" ca="1">INDEX(Caliber!C35:'Caliber'!D45,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B45,0),2)</f>
         <v>0.75</v>
       </c>
       <c r="Z8" t="s">
@@ -20535,81 +20730,81 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X9" t="e" cm="1">
-        <f t="array" aca="1" ref="X9" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X9" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
       <c r="Y9" t="e" cm="1">
-        <f t="array" aca="1" ref="Y9" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y9" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X10" t="e" cm="1">
-        <f t="array" aca="1" ref="X10" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X10" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
       <c r="Y10" t="e" cm="1">
-        <f t="array" aca="1" ref="Y10" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y10" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X11" t="e" cm="1">
-        <f t="array" aca="1" ref="X11" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X11" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
       <c r="Y11" t="e" cm="1">
-        <f t="array" aca="1" ref="Y11" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y11" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X12" t="e" cm="1">
-        <f t="array" aca="1" ref="X12" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X12" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
       <c r="Y12" t="e" cm="1">
-        <f t="array" aca="1" ref="Y12" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y12" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X13" t="e" cm="1">
-        <f t="array" aca="1" ref="X13" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X13" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
       <c r="Y13" t="e" cm="1">
-        <f t="array" aca="1" ref="Y13" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y13" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X14" t="e" cm="1">
-        <f t="array" aca="1" ref="X14" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X14" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
       <c r="Y14" t="e" cm="1">
-        <f t="array" aca="1" ref="Y14" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y14" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X15" t="e" cm="1">
-        <f t="array" aca="1" ref="X15" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X15" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
       <c r="Y15" t="e" cm="1">
-        <f t="array" aca="1" ref="Y15" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y15" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="X16" t="e" cm="1">
-        <f t="array" aca="1" ref="X16" ca="1">INDEX(Caliber!B34:'Caliber'!C42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="X16" ca="1">INDEX(Caliber!B35:'Caliber'!C43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
       <c r="Y16" t="e" cm="1">
-        <f t="array" aca="1" ref="Y16" ca="1">INDEX(Caliber!C34:'Caliber'!D42,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B34:'Caliber'!B42,0),2)</f>
+        <f t="array" aca="1" ref="Y16" ca="1">INDEX(Caliber!C35:'Caliber'!D43,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B35:'Caliber'!B43,0),2)</f>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flashbang fixes, updated item sets
Enemies partially flashed on your turn now glow blue instead of purple.
If you get flashed on the enemy turn, the flash has the proper duration.
PMC item sets updated, tier 3 grunts now have flashbangs.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3626016F-2BD1-4117-896D-4C00E4CDA116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E03F69A-89DE-42B9-835F-09D1D277D552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="580">
   <si>
     <t>Name</t>
   </si>
@@ -1699,9 +1699,6 @@
     <t>FN P90/G36C/Spas 12 (inc)</t>
   </si>
   <si>
-    <t>FN P90/FN P90 (Sopmod)/Spas 12 (inc)</t>
-  </si>
-  <si>
     <t>KS-23/Saiga 12/Sledgehammer</t>
   </si>
   <si>
@@ -1919,6 +1916,15 @@
   </si>
   <si>
     <t>Hunting Rifle/Hunting Rifle/M1 Garand</t>
+  </si>
+  <si>
+    <t>SIG MPX/MP7/Skorpion EVO + (flashbang)</t>
+  </si>
+  <si>
+    <t>FN P90/FN P90 (Sopmod)/Spas 12 (inc) + (flashbang)</t>
+  </si>
+  <si>
+    <t>Versek/AK-12/AKs-74u (Sopmod) + (flashbang)</t>
   </si>
 </sst>
 </file>
@@ -2598,7 +2604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2850,13 +2856,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2886,7 +2892,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4731,22 +4736,20 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>572</v>
-      </c>
-      <c r="C24" s="113">
+        <v>571</v>
+      </c>
+      <c r="C24">
         <v>40</v>
       </c>
-      <c r="D24" s="113">
+      <c r="D24">
         <v>0.5</v>
       </c>
-      <c r="E24" s="113">
+      <c r="E24">
         <v>6</v>
       </c>
-      <c r="F24" s="113">
-        <v>1</v>
-      </c>
-      <c r="G24" s="113"/>
-      <c r="H24" s="113"/>
+      <c r="F24">
+        <v>1</v>
+      </c>
       <c r="M24" s="14" t="s">
         <v>34</v>
       </c>
@@ -5488,7 +5491,7 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C44">
         <v>95</v>
@@ -5506,13 +5509,13 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C45">
         <v>40</v>
@@ -5530,13 +5533,13 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C46">
         <v>40</v>
@@ -7970,9 +7973,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27:G27"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8121,8 +8124,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
@@ -8135,7 +8138,7 @@
       <c r="G7" s="59" t="s">
         <v>490</v>
       </c>
-      <c r="H7" s="101"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="100"/>
@@ -8181,8 +8184,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8195,7 +8198,7 @@
       <c r="G10" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="H10" s="101"/>
+      <c r="H10" s="103"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="100"/>
@@ -8301,13 +8304,13 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F16" s="59" t="s">
         <v>464</v>
@@ -8315,7 +8318,7 @@
       <c r="G16" s="59" t="s">
         <v>467</v>
       </c>
-      <c r="H16" s="101"/>
+      <c r="H16" s="103"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="100"/>
@@ -8361,8 +8364,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8370,12 +8373,12 @@
         <v>463</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G19" s="59" t="s">
-        <v>557</v>
-      </c>
-      <c r="H19" s="101"/>
+        <v>556</v>
+      </c>
+      <c r="H19" s="103"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="100"/>
@@ -8392,7 +8395,7 @@
         <v>364</v>
       </c>
       <c r="F20" s="61" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G20" s="61" t="s">
         <v>365</v>
@@ -8409,10 +8412,10 @@
         <v>348</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G21" s="46" t="s">
         <v>365</v>
@@ -8435,7 +8438,7 @@
       <c r="G22" s="60" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="103"/>
+      <c r="H22" s="101"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="100"/>
@@ -8469,7 +8472,7 @@
         <v>348</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F24" s="46" t="s">
         <v>473</v>
@@ -8480,14 +8483,14 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="103"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>471</v>
@@ -8495,7 +8498,7 @@
       <c r="G25" s="47" t="s">
         <v>474</v>
       </c>
-      <c r="H25" s="103"/>
+      <c r="H25" s="101"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="102" t="s">
@@ -8551,10 +8554,10 @@
         <v>345</v>
       </c>
       <c r="E29" s="75" t="s">
+        <v>539</v>
+      </c>
+      <c r="F29" s="64" t="s">
         <v>540</v>
-      </c>
-      <c r="F29" s="64" t="s">
-        <v>541</v>
       </c>
       <c r="G29" s="76" t="s">
         <v>455</v>
@@ -8571,10 +8574,10 @@
         <v>348</v>
       </c>
       <c r="E30" s="79" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F30" s="71" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G30" s="77" t="s">
         <v>209</v>
@@ -8583,21 +8586,21 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="100"/>
-      <c r="B31" s="101"/>
-      <c r="C31" s="101"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E31" s="78" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>537</v>
-      </c>
-      <c r="H31" s="101"/>
+        <v>536</v>
+      </c>
+      <c r="H31" s="103"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="100"/>
@@ -8611,13 +8614,13 @@
         <v>345</v>
       </c>
       <c r="E32" s="73" t="s">
+        <v>531</v>
+      </c>
+      <c r="F32" s="80" t="s">
         <v>532</v>
       </c>
-      <c r="F32" s="80" t="s">
+      <c r="G32" s="73" t="s">
         <v>533</v>
-      </c>
-      <c r="G32" s="73" t="s">
-        <v>534</v>
       </c>
       <c r="H32" s="100" t="s">
         <v>347</v>
@@ -8631,13 +8634,13 @@
         <v>348</v>
       </c>
       <c r="E33" s="79" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F33" s="71" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G33" s="79" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H33" s="100"/>
     </row>
@@ -8649,13 +8652,13 @@
         <v>349</v>
       </c>
       <c r="E34" s="67" t="s">
+        <v>528</v>
+      </c>
+      <c r="F34" s="81" t="s">
         <v>529</v>
       </c>
-      <c r="F34" s="81" t="s">
-        <v>530</v>
-      </c>
       <c r="G34" s="67" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H34" s="100"/>
     </row>
@@ -8671,13 +8674,13 @@
         <v>345</v>
       </c>
       <c r="E35" s="75" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G35" s="75" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H35" s="99" t="s">
         <v>347</v>
@@ -8691,13 +8694,13 @@
         <v>348</v>
       </c>
       <c r="E36" s="79" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F36" s="79" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G36" s="79" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H36" s="100"/>
     </row>
@@ -8712,10 +8715,10 @@
         <v>481</v>
       </c>
       <c r="F37" s="90" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G37" s="90" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H37" s="100"/>
     </row>
@@ -8731,13 +8734,13 @@
         <v>345</v>
       </c>
       <c r="E38" s="63" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F38" s="85" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G38" s="63" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H38" s="99" t="s">
         <v>370</v>
@@ -8751,13 +8754,13 @@
         <v>348</v>
       </c>
       <c r="E39" s="79" t="s">
+        <v>506</v>
+      </c>
+      <c r="F39" s="71" t="s">
         <v>507</v>
       </c>
-      <c r="F39" s="71" t="s">
-        <v>508</v>
-      </c>
       <c r="G39" s="79" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="H39" s="100"/>
     </row>
@@ -8769,13 +8772,13 @@
         <v>349</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F40" s="81" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G40" s="67" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H40" s="100"/>
     </row>
@@ -8797,7 +8800,7 @@
         <v>502</v>
       </c>
       <c r="G41" s="86" t="s">
-        <v>502</v>
+        <v>579</v>
       </c>
       <c r="H41" s="99" t="s">
         <v>347</v>
@@ -8817,7 +8820,7 @@
         <v>503</v>
       </c>
       <c r="G42" s="87" t="s">
-        <v>504</v>
+        <v>578</v>
       </c>
       <c r="H42" s="100"/>
     </row>
@@ -8835,7 +8838,7 @@
         <v>501</v>
       </c>
       <c r="G43" s="67" t="s">
-        <v>501</v>
+        <v>577</v>
       </c>
       <c r="H43" s="100"/>
     </row>
@@ -8851,13 +8854,13 @@
         <v>345</v>
       </c>
       <c r="E44" s="68" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G44" s="68" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H44" s="99" t="s">
         <v>347</v>
@@ -8871,13 +8874,13 @@
         <v>348</v>
       </c>
       <c r="E45" s="69" t="s">
+        <v>558</v>
+      </c>
+      <c r="F45" s="69" t="s">
         <v>559</v>
       </c>
-      <c r="F45" s="69" t="s">
-        <v>560</v>
-      </c>
       <c r="G45" s="69" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H45" s="100"/>
     </row>
@@ -8889,13 +8892,13 @@
         <v>349</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F46" s="81" t="s">
+        <v>525</v>
+      </c>
+      <c r="G46" s="67" t="s">
         <v>526</v>
-      </c>
-      <c r="G46" s="67" t="s">
-        <v>527</v>
       </c>
       <c r="H46" s="100"/>
     </row>
@@ -8914,7 +8917,7 @@
         <v>158</v>
       </c>
       <c r="F47" s="80" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G47" s="63" t="s">
         <v>476</v>
@@ -8931,48 +8934,61 @@
         <v>348</v>
       </c>
       <c r="E48" s="70" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F48" s="83" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G48" s="70" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="103"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="103"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
       <c r="E49" s="84" t="s">
+        <v>518</v>
+      </c>
+      <c r="F49" s="72" t="s">
         <v>519</v>
       </c>
-      <c r="F49" s="72" t="s">
-        <v>520</v>
-      </c>
       <c r="G49" s="84" t="s">
-        <v>517</v>
-      </c>
-      <c r="H49" s="103"/>
+        <v>516</v>
+      </c>
+      <c r="H49" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="H35:H37"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8989,31 +9005,18 @@
     <mergeCell ref="H17:H19"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9500,7 +9503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -9565,7 +9568,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B12" s="14"/>
     </row>
@@ -9574,49 +9577,49 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B21" s="14"/>
     </row>
@@ -12127,7 +12130,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B16">
         <v>19</v>
@@ -16687,7 +16690,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B55">
         <v>31</v>
@@ -16699,7 +16702,7 @@
         <v>76</v>
       </c>
       <c r="E55" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -16764,7 +16767,7 @@
         <v>0.3</v>
       </c>
       <c r="Z55" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
@@ -17890,7 +17893,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -17956,7 +17959,7 @@
         <v>76</v>
       </c>
       <c r="W14" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="X14">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W14,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -17970,12 +17973,12 @@
         <v>178</v>
       </c>
       <c r="AA14" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B15">
         <v>37</v>
@@ -18041,7 +18044,7 @@
         <v>76</v>
       </c>
       <c r="W15" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="X15">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W15,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -18055,7 +18058,7 @@
         <v>178</v>
       </c>
       <c r="AA15" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -20645,7 +20648,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -20711,7 +20714,7 @@
         <v>76</v>
       </c>
       <c r="W8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="X8" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B35:'Caliber'!C45,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B45,0),2)</f>
@@ -20725,7 +20728,7 @@
         <v>82</v>
       </c>
       <c r="AA8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sorted listOrder IDs, more Ufopaedia descriptions
Sorted listOrder ID's for every item, now sorted by ammotype, system is commented at the top of WeaponsEquipment.rul.
Added ufopaedia entrys for the M9, AKs-74u, and Zevada rounds.
Tier 3 eastern EU PMC Heavys now can rarely spawn with flashbang rounds
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E03F69A-89DE-42B9-835F-09D1D277D552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F576F309-F3D5-41FC-8399-496F816B842F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -1714,9 +1714,6 @@
     <t>AA-12/Mk 18 Mod 0 MASS/AA-12 (Slug)</t>
   </si>
   <si>
-    <t>KS-23/Saiga 12/Saiga 12 (Slug)</t>
-  </si>
-  <si>
     <t>HK416 (SOPMOD)/Tavor 95x/HK416 (Mass)</t>
   </si>
   <si>
@@ -1925,6 +1922,9 @@
   </si>
   <si>
     <t>Versek/AK-12/AKs-74u (Sopmod) + (flashbang)</t>
+  </si>
+  <si>
+    <t>KS-23/Saiga 12/KS-23 (Flash)</t>
   </si>
 </sst>
 </file>
@@ -4055,7 +4055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -4736,7 +4736,7 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C24">
         <v>40</v>
@@ -5491,7 +5491,7 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C44">
         <v>95</v>
@@ -5509,13 +5509,13 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C45">
         <v>40</v>
@@ -5533,13 +5533,13 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C46">
         <v>40</v>
@@ -7973,9 +7973,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8310,7 +8310,7 @@
         <v>349</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F16" s="59" t="s">
         <v>464</v>
@@ -8373,10 +8373,10 @@
         <v>463</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G19" s="59" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="H19" s="103"/>
     </row>
@@ -8395,7 +8395,7 @@
         <v>364</v>
       </c>
       <c r="F20" s="61" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G20" s="61" t="s">
         <v>365</v>
@@ -8412,10 +8412,10 @@
         <v>348</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G21" s="46" t="s">
         <v>365</v>
@@ -8472,7 +8472,7 @@
         <v>348</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F24" s="46" t="s">
         <v>473</v>
@@ -8490,7 +8490,7 @@
         <v>349</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>471</v>
@@ -8554,10 +8554,10 @@
         <v>345</v>
       </c>
       <c r="E29" s="75" t="s">
+        <v>538</v>
+      </c>
+      <c r="F29" s="64" t="s">
         <v>539</v>
-      </c>
-      <c r="F29" s="64" t="s">
-        <v>540</v>
       </c>
       <c r="G29" s="76" t="s">
         <v>455</v>
@@ -8574,10 +8574,10 @@
         <v>348</v>
       </c>
       <c r="E30" s="79" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F30" s="71" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G30" s="77" t="s">
         <v>209</v>
@@ -8592,13 +8592,13 @@
         <v>349</v>
       </c>
       <c r="E31" s="78" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H31" s="103"/>
     </row>
@@ -8614,13 +8614,13 @@
         <v>345</v>
       </c>
       <c r="E32" s="73" t="s">
+        <v>530</v>
+      </c>
+      <c r="F32" s="80" t="s">
         <v>531</v>
       </c>
-      <c r="F32" s="80" t="s">
+      <c r="G32" s="73" t="s">
         <v>532</v>
-      </c>
-      <c r="G32" s="73" t="s">
-        <v>533</v>
       </c>
       <c r="H32" s="100" t="s">
         <v>347</v>
@@ -8634,13 +8634,13 @@
         <v>348</v>
       </c>
       <c r="E33" s="79" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F33" s="71" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="G33" s="79" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="H33" s="100"/>
     </row>
@@ -8652,13 +8652,13 @@
         <v>349</v>
       </c>
       <c r="E34" s="67" t="s">
+        <v>527</v>
+      </c>
+      <c r="F34" s="81" t="s">
         <v>528</v>
       </c>
-      <c r="F34" s="81" t="s">
-        <v>529</v>
-      </c>
       <c r="G34" s="67" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H34" s="100"/>
     </row>
@@ -8674,13 +8674,13 @@
         <v>345</v>
       </c>
       <c r="E35" s="75" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G35" s="75" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H35" s="99" t="s">
         <v>347</v>
@@ -8694,13 +8694,13 @@
         <v>348</v>
       </c>
       <c r="E36" s="79" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F36" s="79" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G36" s="79" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="H36" s="100"/>
     </row>
@@ -8715,10 +8715,10 @@
         <v>481</v>
       </c>
       <c r="F37" s="90" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G37" s="90" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H37" s="100"/>
     </row>
@@ -8740,7 +8740,7 @@
         <v>504</v>
       </c>
       <c r="G38" s="63" t="s">
-        <v>509</v>
+        <v>579</v>
       </c>
       <c r="H38" s="99" t="s">
         <v>370</v>
@@ -8772,7 +8772,7 @@
         <v>349</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F40" s="81" t="s">
         <v>508</v>
@@ -8800,7 +8800,7 @@
         <v>502</v>
       </c>
       <c r="G41" s="86" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H41" s="99" t="s">
         <v>347</v>
@@ -8820,7 +8820,7 @@
         <v>503</v>
       </c>
       <c r="G42" s="87" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H42" s="100"/>
     </row>
@@ -8838,7 +8838,7 @@
         <v>501</v>
       </c>
       <c r="G43" s="67" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H43" s="100"/>
     </row>
@@ -8854,13 +8854,13 @@
         <v>345</v>
       </c>
       <c r="E44" s="68" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G44" s="68" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H44" s="99" t="s">
         <v>347</v>
@@ -8874,13 +8874,13 @@
         <v>348</v>
       </c>
       <c r="E45" s="69" t="s">
+        <v>557</v>
+      </c>
+      <c r="F45" s="69" t="s">
         <v>558</v>
       </c>
-      <c r="F45" s="69" t="s">
-        <v>559</v>
-      </c>
       <c r="G45" s="69" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H45" s="100"/>
     </row>
@@ -8892,13 +8892,13 @@
         <v>349</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F46" s="81" t="s">
+        <v>524</v>
+      </c>
+      <c r="G46" s="67" t="s">
         <v>525</v>
-      </c>
-      <c r="G46" s="67" t="s">
-        <v>526</v>
       </c>
       <c r="H46" s="100"/>
     </row>
@@ -8917,7 +8917,7 @@
         <v>158</v>
       </c>
       <c r="F47" s="80" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G47" s="63" t="s">
         <v>476</v>
@@ -8934,13 +8934,13 @@
         <v>348</v>
       </c>
       <c r="E48" s="70" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F48" s="83" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G48" s="70" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H48" s="100"/>
     </row>
@@ -8952,13 +8952,13 @@
         <v>349</v>
       </c>
       <c r="E49" s="84" t="s">
+        <v>517</v>
+      </c>
+      <c r="F49" s="72" t="s">
         <v>518</v>
       </c>
-      <c r="F49" s="72" t="s">
-        <v>519</v>
-      </c>
       <c r="G49" s="84" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H49" s="101"/>
     </row>
@@ -9503,7 +9503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -9568,7 +9568,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B12" s="14"/>
     </row>
@@ -9577,49 +9577,49 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B21" s="14"/>
     </row>
@@ -9679,7 +9679,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M20" sqref="M20"/>
+      <selection pane="topRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12130,7 +12130,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B16">
         <v>19</v>
@@ -12220,10 +12220,10 @@
   <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L23" sqref="L23"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16690,7 +16690,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B55">
         <v>31</v>
@@ -16702,7 +16702,7 @@
         <v>76</v>
       </c>
       <c r="E55" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -16767,7 +16767,7 @@
         <v>0.3</v>
       </c>
       <c r="Z55" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
@@ -17893,7 +17893,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -17959,7 +17959,7 @@
         <v>76</v>
       </c>
       <c r="W14" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="X14">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W14,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -17973,12 +17973,12 @@
         <v>178</v>
       </c>
       <c r="AA14" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B15">
         <v>37</v>
@@ -18044,7 +18044,7 @@
         <v>76</v>
       </c>
       <c r="W15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="X15">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W15,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -18058,7 +18058,7 @@
         <v>178</v>
       </c>
       <c r="AA15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -20024,7 +20024,7 @@
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
@@ -20648,7 +20648,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -20714,7 +20714,7 @@
         <v>76</v>
       </c>
       <c r="W8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="X8" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B35:'Caliber'!C45,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B45,0),2)</f>
@@ -20728,7 +20728,7 @@
         <v>82</v>
       </c>
       <c r="AA8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Weapon sprites in ufopaedia articles appear loaded
-Weapon sprites in ufopaedia articles now appear loaded
-Added UfopaediaAmmoNo tag
-Added MSG90 10rnd sprite
-Fixed HK416 (M320) 30rnd sprite being set to no mag sprite
-Cleaned up categories.rul a bit
-Added prison facility sprite
-Fixed a couple of errors in ar18 ufopaedia article
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D985EE81-A887-4820-BD74-17986D18ABCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D43176-2B13-4924-9048-4A8E57B839E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
@@ -2859,13 +2859,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8127,8 +8127,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="100"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
@@ -8141,7 +8141,7 @@
       <c r="G7" s="59" t="s">
         <v>490</v>
       </c>
-      <c r="H7" s="103"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="100"/>
@@ -8187,8 +8187,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="100"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8201,7 +8201,7 @@
       <c r="G10" s="59" t="s">
         <v>496</v>
       </c>
-      <c r="H10" s="103"/>
+      <c r="H10" s="101"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="100"/>
@@ -8307,8 +8307,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="100"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="103"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="101"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
@@ -8321,7 +8321,7 @@
       <c r="G16" s="59" t="s">
         <v>467</v>
       </c>
-      <c r="H16" s="103"/>
+      <c r="H16" s="101"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="100"/>
@@ -8367,8 +8367,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="100"/>
-      <c r="B19" s="103"/>
-      <c r="C19" s="103"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="101"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8381,7 +8381,7 @@
       <c r="G19" s="59" t="s">
         <v>555</v>
       </c>
-      <c r="H19" s="103"/>
+      <c r="H19" s="101"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="100"/>
@@ -8441,7 +8441,7 @@
       <c r="G22" s="60" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="101"/>
+      <c r="H22" s="103"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="100"/>
@@ -8486,9 +8486,9 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="101"/>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
@@ -8501,7 +8501,7 @@
       <c r="G25" s="47" t="s">
         <v>474</v>
       </c>
-      <c r="H25" s="101"/>
+      <c r="H25" s="103"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="102" t="s">
@@ -8589,8 +8589,8 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="100"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
@@ -8603,7 +8603,7 @@
       <c r="G31" s="78" t="s">
         <v>535</v>
       </c>
-      <c r="H31" s="103"/>
+      <c r="H31" s="101"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="100"/>
@@ -8948,9 +8948,9 @@
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="101"/>
-      <c r="B49" s="101"/>
-      <c r="C49" s="101"/>
+      <c r="A49" s="103"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="103"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
@@ -8963,19 +8963,38 @@
       <c r="G49" s="84" t="s">
         <v>515</v>
       </c>
-      <c r="H49" s="101"/>
+      <c r="H49" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8992,34 +9011,15 @@
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="H35:H37"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Colored damage types in ufopaedia
Updated enemy item sets.
Added colors for every damage type.
Added less-lethal and breaching damage types (no stat changes).
Added extra ufopaedia pages for weapons with more than 3 ammo types.
Added Field dressing and Zevada(1x)/Shrapnel(2x) ufopaedia articles.
updated 12G Inc, knife, ballistic knife, and breaching hammer ufopaedia articles.
Zevada(1x)/Shrapnel(2x) is now 700$ and now has the proper listorder number.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94489C6-2641-4156-82FB-6EB7457E8B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8950FE0D-D53E-480B-A019-3F745F9E58B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -2856,13 +2856,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4055,8 +4055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4934,7 +4934,7 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I28" t="s">
         <v>36</v>
@@ -4982,7 +4982,7 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29" t="s">
         <v>449</v>
@@ -5009,7 +5009,7 @@
         <v>1</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I30" t="s">
         <v>452</v>
@@ -5140,7 +5140,7 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I33" t="s">
         <v>36</v>
@@ -5316,7 +5316,7 @@
         <v>6</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I37" t="s">
         <v>46</v>
@@ -8124,8 +8124,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="100"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
@@ -8138,7 +8138,7 @@
       <c r="G7" s="59" t="s">
         <v>489</v>
       </c>
-      <c r="H7" s="103"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="100"/>
@@ -8184,8 +8184,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="100"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8198,7 +8198,7 @@
       <c r="G10" s="59" t="s">
         <v>495</v>
       </c>
-      <c r="H10" s="103"/>
+      <c r="H10" s="101"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="100"/>
@@ -8304,8 +8304,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="100"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="103"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="101"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
@@ -8318,7 +8318,7 @@
       <c r="G16" s="59" t="s">
         <v>466</v>
       </c>
-      <c r="H16" s="103"/>
+      <c r="H16" s="101"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="100"/>
@@ -8364,8 +8364,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="100"/>
-      <c r="B19" s="103"/>
-      <c r="C19" s="103"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="101"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8378,7 +8378,7 @@
       <c r="G19" s="59" t="s">
         <v>554</v>
       </c>
-      <c r="H19" s="103"/>
+      <c r="H19" s="101"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="100"/>
@@ -8438,7 +8438,7 @@
       <c r="G22" s="60" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="101"/>
+      <c r="H22" s="103"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="100"/>
@@ -8483,9 +8483,9 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="101"/>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
@@ -8498,7 +8498,7 @@
       <c r="G25" s="47" t="s">
         <v>473</v>
       </c>
-      <c r="H25" s="101"/>
+      <c r="H25" s="103"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="102" t="s">
@@ -8586,8 +8586,8 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="100"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
@@ -8600,7 +8600,7 @@
       <c r="G31" s="78" t="s">
         <v>534</v>
       </c>
-      <c r="H31" s="103"/>
+      <c r="H31" s="101"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="100"/>
@@ -8945,9 +8945,9 @@
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="101"/>
-      <c r="B49" s="101"/>
-      <c r="C49" s="101"/>
+      <c r="A49" s="103"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="103"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
@@ -8960,19 +8960,38 @@
       <c r="G49" s="84" t="s">
         <v>514</v>
       </c>
-      <c r="H49" s="101"/>
+      <c r="H49" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8989,34 +9008,15 @@
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="H35:H37"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9503,7 +9503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FN MAG, more ufopaedia improvements
FN MAG
Flash ammo type
Zevada ammo now shows partial flash damage
New ufopaedia article that explains the flashbang system
Fixed armor ufopaedia article text
updated item sets
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8950FE0D-D53E-480B-A019-3F745F9E58B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7F723B-0EA0-4957-87B4-AD66A5D400C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="13" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <author>Ethan McLaughlin</author>
   </authors>
   <commentList>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{25CD22B6-3B72-484D-8ECD-F3C21230A65F}">
+    <comment ref="C44" authorId="0" shapeId="0" xr:uid="{F23E61E1-912C-44CC-AA1F-69DDAD9D6AD3}">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>to do</t>
+          <t>WIP</t>
         </r>
       </text>
     </comment>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="584">
   <si>
     <t>Name</t>
   </si>
@@ -1615,9 +1615,6 @@
     <t>VSS/OSV 96/OSV 96</t>
   </si>
   <si>
-    <t>(1 Grenade) + AK-74/?/AKs-74u</t>
-  </si>
-  <si>
     <t>AK-12/Aks-74u (Sopmod)/RK-62</t>
   </si>
   <si>
@@ -1675,9 +1672,6 @@
     <t>M249/M60/M60</t>
   </si>
   <si>
-    <t>Negev/M60/M60</t>
-  </si>
-  <si>
     <t>Vityaz/AKs-74u (Sopmod)/Vektor</t>
   </si>
   <si>
@@ -1750,9 +1744,6 @@
     <t>RPK</t>
   </si>
   <si>
-    <t>M249/M60/M249</t>
-  </si>
-  <si>
     <t>MK48/Negev/MK48</t>
   </si>
   <si>
@@ -1855,12 +1846,6 @@
     <t>AA-12(NL)/Serbu/Serbu (Breach)</t>
   </si>
   <si>
-    <t>Negev/M60/CBJ-MS (SAW)</t>
-  </si>
-  <si>
-    <t>Mk48/Negev/CBJ-MS (SAW)</t>
-  </si>
-  <si>
     <t>Snap</t>
   </si>
   <si>
@@ -1918,13 +1903,40 @@
     <t>Versek/AK-12/AKs-74u (Sopmod) + (flashbang)</t>
   </si>
   <si>
-    <t>KS-23/Saiga 12/KS-23 (Flash)</t>
-  </si>
-  <si>
     <t>Hi-Power (2 Molotovs)</t>
   </si>
   <si>
     <t xml:space="preserve">Hi-Power  </t>
+  </si>
+  <si>
+    <t>(1 Grenade) + (AK-74/?/AKs-74u)</t>
+  </si>
+  <si>
+    <t>KS-23/Saiga 12/KS-23 (1xFlash 2xbuck)</t>
+  </si>
+  <si>
+    <t>FN MAG</t>
+  </si>
+  <si>
+    <t>FN Minimi/FN Minimi/FN MAG</t>
+  </si>
+  <si>
+    <t>FN MAG/FN Minimi/FN Minimi</t>
+  </si>
+  <si>
+    <t>FN Minimi/FN Mag/CBJ-MS (SAW)</t>
+  </si>
+  <si>
+    <t>Mk48/FN Minimi/CBJ-MS (SAW)</t>
+  </si>
+  <si>
+    <t>M60/M60/M249</t>
+  </si>
+  <si>
+    <t>Bren</t>
+  </si>
+  <si>
+    <t>Aug HBAR</t>
   </si>
 </sst>
 </file>
@@ -2856,13 +2868,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4055,7 +4067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -4736,7 +4748,7 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="C24">
         <v>40</v>
@@ -5491,7 +5503,7 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C44">
         <v>95</v>
@@ -5509,13 +5521,13 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="9"/>
       <c r="B45" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="C45">
         <v>40</v>
@@ -5533,13 +5545,13 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="C46">
         <v>40</v>
@@ -7974,8 +7986,8 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8019,7 +8031,7 @@
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="102" t="s">
-        <v>337</v>
+        <v>388</v>
       </c>
       <c r="B2" s="102" t="s">
         <v>298</v>
@@ -8031,10 +8043,10 @@
         <v>345</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G2" s="45" t="s">
         <v>346</v>
@@ -8052,13 +8064,13 @@
         <v>348</v>
       </c>
       <c r="E3" s="46" t="s">
+        <v>477</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>477</v>
+      </c>
+      <c r="G3" s="46" t="s">
         <v>478</v>
-      </c>
-      <c r="F3" s="46" t="s">
-        <v>478</v>
-      </c>
-      <c r="G3" s="46" t="s">
-        <v>479</v>
       </c>
       <c r="H3" s="100"/>
     </row>
@@ -8070,13 +8082,13 @@
         <v>349</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G4" s="60" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H4" s="100"/>
     </row>
@@ -8092,13 +8104,13 @@
         <v>345</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="H5" s="99" t="s">
         <v>347</v>
@@ -8112,33 +8124,33 @@
         <v>348</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F6" s="46" t="s">
+        <v>489</v>
+      </c>
+      <c r="G6" s="46" t="s">
         <v>490</v>
-      </c>
-      <c r="G6" s="46" t="s">
-        <v>491</v>
       </c>
       <c r="H6" s="100"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F7" s="59" t="s">
+        <v>487</v>
+      </c>
+      <c r="G7" s="59" t="s">
         <v>488</v>
       </c>
-      <c r="G7" s="59" t="s">
-        <v>489</v>
-      </c>
-      <c r="H7" s="101"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="100"/>
@@ -8152,10 +8164,10 @@
         <v>345</v>
       </c>
       <c r="E8" s="61" t="s">
+        <v>491</v>
+      </c>
+      <c r="F8" s="61" t="s">
         <v>492</v>
-      </c>
-      <c r="F8" s="61" t="s">
-        <v>493</v>
       </c>
       <c r="G8" s="61" t="s">
         <v>220</v>
@@ -8175,17 +8187,17 @@
         <v>351</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>211</v>
+        <v>577</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>496</v>
+        <v>578</v>
       </c>
       <c r="H9" s="100"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="100"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8196,9 +8208,9 @@
         <v>211</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>495</v>
-      </c>
-      <c r="H10" s="101"/>
+        <v>494</v>
+      </c>
+      <c r="H10" s="103"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="100"/>
@@ -8218,7 +8230,7 @@
         <v>461</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>476</v>
+        <v>574</v>
       </c>
       <c r="H11" s="99" t="s">
         <v>357</v>
@@ -8235,10 +8247,10 @@
         <v>203</v>
       </c>
       <c r="F12" s="46" t="s">
+        <v>480</v>
+      </c>
+      <c r="G12" s="46" t="s">
         <v>481</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>482</v>
       </c>
       <c r="H12" s="100"/>
     </row>
@@ -8304,13 +8316,13 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="100"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F16" s="59" t="s">
         <v>463</v>
@@ -8318,7 +8330,7 @@
       <c r="G16" s="59" t="s">
         <v>466</v>
       </c>
-      <c r="H16" s="101"/>
+      <c r="H16" s="103"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="100"/>
@@ -8352,7 +8364,7 @@
         <v>348</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="F18" s="46" t="s">
         <v>352</v>
@@ -8364,8 +8376,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="100"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8373,12 +8385,12 @@
         <v>462</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="G19" s="59" t="s">
-        <v>554</v>
-      </c>
-      <c r="H19" s="101"/>
+        <v>551</v>
+      </c>
+      <c r="H19" s="103"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="100"/>
@@ -8395,7 +8407,7 @@
         <v>364</v>
       </c>
       <c r="F20" s="61" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="G20" s="61" t="s">
         <v>365</v>
@@ -8412,10 +8424,10 @@
         <v>348</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="G21" s="46" t="s">
         <v>365</v>
@@ -8438,7 +8450,7 @@
       <c r="G22" s="60" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="103"/>
+      <c r="H22" s="101"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="100"/>
@@ -8472,7 +8484,7 @@
         <v>348</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="F24" s="46" t="s">
         <v>472</v>
@@ -8483,14 +8495,14 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="103"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>470</v>
@@ -8498,7 +8510,7 @@
       <c r="G25" s="47" t="s">
         <v>473</v>
       </c>
-      <c r="H25" s="103"/>
+      <c r="H25" s="101"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="102" t="s">
@@ -8554,10 +8566,10 @@
         <v>345</v>
       </c>
       <c r="E29" s="75" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F29" s="64" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="G29" s="76" t="s">
         <v>455</v>
@@ -8574,10 +8586,10 @@
         <v>348</v>
       </c>
       <c r="E30" s="79" t="s">
+        <v>533</v>
+      </c>
+      <c r="F30" s="71" t="s">
         <v>536</v>
-      </c>
-      <c r="F30" s="71" t="s">
-        <v>539</v>
       </c>
       <c r="G30" s="77" t="s">
         <v>209</v>
@@ -8586,21 +8598,21 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="100"/>
-      <c r="B31" s="101"/>
-      <c r="C31" s="101"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E31" s="78" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>534</v>
-      </c>
-      <c r="H31" s="101"/>
+        <v>531</v>
+      </c>
+      <c r="H31" s="103"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="100"/>
@@ -8614,13 +8626,13 @@
         <v>345</v>
       </c>
       <c r="E32" s="73" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F32" s="80" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G32" s="73" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="H32" s="100" t="s">
         <v>347</v>
@@ -8634,13 +8646,13 @@
         <v>348</v>
       </c>
       <c r="E33" s="79" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F33" s="71" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="G33" s="79" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="H33" s="100"/>
     </row>
@@ -8652,13 +8664,13 @@
         <v>349</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="F34" s="81" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="G34" s="67" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H34" s="100"/>
     </row>
@@ -8674,13 +8686,13 @@
         <v>345</v>
       </c>
       <c r="E35" s="75" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="G35" s="75" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H35" s="99" t="s">
         <v>347</v>
@@ -8694,13 +8706,13 @@
         <v>348</v>
       </c>
       <c r="E36" s="79" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F36" s="79" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="G36" s="79" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H36" s="100"/>
     </row>
@@ -8712,13 +8724,13 @@
         <v>349</v>
       </c>
       <c r="E37" s="90" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F37" s="90" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="G37" s="90" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H37" s="100"/>
     </row>
@@ -8734,13 +8746,13 @@
         <v>345</v>
       </c>
       <c r="E38" s="63" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F38" s="85" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G38" s="63" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="H38" s="99" t="s">
         <v>370</v>
@@ -8754,13 +8766,13 @@
         <v>348</v>
       </c>
       <c r="E39" s="79" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F39" s="71" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G39" s="79" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H39" s="100"/>
     </row>
@@ -8772,13 +8784,13 @@
         <v>349</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F40" s="81" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="G40" s="67" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H40" s="100"/>
     </row>
@@ -8794,13 +8806,13 @@
         <v>345</v>
       </c>
       <c r="E41" s="86" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F41" s="80" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G41" s="86" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="H41" s="99" t="s">
         <v>347</v>
@@ -8814,13 +8826,13 @@
         <v>348</v>
       </c>
       <c r="E42" s="87" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F42" s="88" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="G42" s="87" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="H42" s="100"/>
     </row>
@@ -8832,13 +8844,13 @@
         <v>349</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F43" s="89" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G43" s="67" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="H43" s="100"/>
     </row>
@@ -8854,13 +8866,13 @@
         <v>345</v>
       </c>
       <c r="E44" s="68" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="G44" s="68" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="H44" s="99" t="s">
         <v>347</v>
@@ -8874,13 +8886,13 @@
         <v>348</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>556</v>
+        <v>579</v>
       </c>
       <c r="F45" s="69" t="s">
-        <v>557</v>
+        <v>580</v>
       </c>
       <c r="G45" s="69" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H45" s="100"/>
     </row>
@@ -8892,13 +8904,13 @@
         <v>349</v>
       </c>
       <c r="E46" s="67" t="s">
+        <v>581</v>
+      </c>
+      <c r="F46" s="81" t="s">
+        <v>520</v>
+      </c>
+      <c r="G46" s="67" t="s">
         <v>521</v>
-      </c>
-      <c r="F46" s="81" t="s">
-        <v>523</v>
-      </c>
-      <c r="G46" s="67" t="s">
-        <v>524</v>
       </c>
       <c r="H46" s="100"/>
     </row>
@@ -8917,7 +8929,7 @@
         <v>158</v>
       </c>
       <c r="F47" s="80" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="G47" s="63" t="s">
         <v>475</v>
@@ -8934,48 +8946,61 @@
         <v>348</v>
       </c>
       <c r="E48" s="70" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F48" s="83" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G48" s="70" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="103"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="103"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
       <c r="E49" s="84" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F49" s="72" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G49" s="84" t="s">
-        <v>514</v>
-      </c>
-      <c r="H49" s="103"/>
+        <v>512</v>
+      </c>
+      <c r="H49" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="H35:H37"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8992,31 +9017,18 @@
     <mergeCell ref="H17:H19"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -9503,8 +9515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6FEC12-ED84-4F38-9B1C-DC3BDC099D3A}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9568,50 +9580,56 @@
       <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>583</v>
+      </c>
       <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>582</v>
+      </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="B21" s="14"/>
     </row>
@@ -10895,7 +10913,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -12201,7 +12219,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B16">
         <v>19</v>
@@ -16761,7 +16779,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B55">
         <v>31</v>
@@ -16773,7 +16791,7 @@
         <v>76</v>
       </c>
       <c r="E55" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -16838,7 +16856,7 @@
         <v>0.3</v>
       </c>
       <c r="Z55" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.3">
@@ -17964,7 +17982,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -18030,7 +18048,7 @@
         <v>76</v>
       </c>
       <c r="W14" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="X14">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W14,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -18044,12 +18062,12 @@
         <v>178</v>
       </c>
       <c r="AA14" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="B15">
         <v>37</v>
@@ -18115,7 +18133,7 @@
         <v>76</v>
       </c>
       <c r="W15" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="X15">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W15,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -18129,7 +18147,7 @@
         <v>178</v>
       </c>
       <c r="AA15" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
@@ -19309,11 +19327,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0094531B-7BBB-4DD3-8835-99962592A6C6}">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="topRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19512,13 +19530,13 @@
         <v>215</v>
       </c>
       <c r="B3">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>212</v>
       </c>
-      <c r="D3">
-        <v>50000</v>
+      <c r="D3" t="s">
+        <v>76</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -19539,7 +19557,7 @@
         <v>40</v>
       </c>
       <c r="K3">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
         <v>76</v>
@@ -19548,7 +19566,7 @@
         <v>50</v>
       </c>
       <c r="N3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
         <v>76</v>
@@ -19845,8 +19863,8 @@
       <c r="C7" t="s">
         <v>212</v>
       </c>
-      <c r="D7">
-        <v>54000</v>
+      <c r="D7" t="s">
+        <v>76</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -20079,6 +20097,88 @@
       </c>
       <c r="Z9" t="s">
         <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>576</v>
+      </c>
+      <c r="B10">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10">
+        <v>145</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10">
+        <v>45</v>
+      </c>
+      <c r="K10">
+        <v>65</v>
+      </c>
+      <c r="L10" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10">
+        <v>45</v>
+      </c>
+      <c r="N10">
+        <v>25</v>
+      </c>
+      <c r="O10" t="s">
+        <v>76</v>
+      </c>
+      <c r="P10">
+        <v>35</v>
+      </c>
+      <c r="Q10">
+        <v>18</v>
+      </c>
+      <c r="R10">
+        <v>200</v>
+      </c>
+      <c r="S10">
+        <v>5</v>
+      </c>
+      <c r="T10" t="s">
+        <v>76</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>15</v>
+      </c>
+      <c r="W10" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10" cm="1">
+        <f t="array" aca="1" ref="X10" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>45</v>
+      </c>
+      <c r="Y10" cm="1">
+        <f t="array" aca="1" ref="Y10" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -20719,7 +20819,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -20785,7 +20885,7 @@
         <v>76</v>
       </c>
       <c r="W8" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="X8" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B35:'Caliber'!C45,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B45,0),2)</f>
@@ -20799,7 +20899,7 @@
         <v>82</v>
       </c>
       <c r="AA8" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Stats for new machine guns
Still need research to be set up, but they have stats and ufopaedia articles now.
Fixed bug with Vilban.mcd where the staircase would turn into a roof when broken
Renamed the breach test map to breaching sim, and improved its mission description.
Also updated enemy item sets to include new machine guns.
fixed item sets using glocks having 40x mags
Also removed unnecessary map viewer backup files.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F13B6FC-8E00-46D5-B27A-8D27E327D21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE496348-7910-43FB-9E24-D3C1F35B7E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -49,30 +49,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Ethan McLaughlin</author>
-  </authors>
-  <commentList>
-    <comment ref="C44" authorId="0" shapeId="0" xr:uid="{F23E61E1-912C-44CC-AA1F-69DDAD9D6AD3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>WIP</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ethan McLaughlin</author>
@@ -119,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="587">
   <si>
     <t>Name</t>
   </si>
@@ -1744,15 +1720,6 @@
     <t>RPK</t>
   </si>
   <si>
-    <t>MK48/Negev/MK48</t>
-  </si>
-  <si>
-    <t>FN Minimi/M60/M249</t>
-  </si>
-  <si>
-    <t>FN Minimi/M249/FN Minimi</t>
-  </si>
-  <si>
     <t>Pecheneg/?/RPK</t>
   </si>
   <si>
@@ -1915,26 +1882,53 @@
     <t>FN Minimi/FN Minimi/FN MAG</t>
   </si>
   <si>
-    <t>FN MAG/FN Minimi/FN Minimi</t>
-  </si>
-  <si>
     <t>FN Minimi/FN Mag/CBJ-MS (SAW)</t>
   </si>
   <si>
-    <t>Mk48/FN Minimi/CBJ-MS (SAW)</t>
-  </si>
-  <si>
-    <t>M60/M60/M249</t>
-  </si>
-  <si>
     <t>Bren</t>
+  </si>
+  <si>
+    <t>AUG HBAR</t>
+  </si>
+  <si>
+    <t>MG36</t>
+  </si>
+  <si>
+    <t>C7A1 LSW</t>
+  </si>
+  <si>
+    <t>Ultimax 100</t>
+  </si>
+  <si>
+    <t>M60E6</t>
+  </si>
+  <si>
+    <t>FN MAG/FN MAG/FN Minimi</t>
+  </si>
+  <si>
+    <t>M60/M60/C7A1 LSW</t>
+  </si>
+  <si>
+    <t>C7A1 LSW/M60/M249</t>
+  </si>
+  <si>
+    <t>M249/M249/M60E6</t>
+  </si>
+  <si>
+    <t>Mk48/AUG HBAR/MG36</t>
+  </si>
+  <si>
+    <t>MK48/Negev/MG36</t>
+  </si>
+  <si>
+    <t>M60E6/M249/Ultimax 100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1968,13 +1962,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="25">
@@ -2607,7 +2594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2859,13 +2846,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2895,6 +2882,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3446,8 +3434,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7B36A2CF-DAA4-4B61-B862-8F0D47D69557}" name="Table3" displayName="Table3" ref="A1:AA14" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:AA14" xr:uid="{7B36A2CF-DAA4-4B61-B862-8F0D47D69557}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7B36A2CF-DAA4-4B61-B862-8F0D47D69557}" name="Table3" displayName="Table3" ref="A1:AA15" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:AA15" xr:uid="{7B36A2CF-DAA4-4B61-B862-8F0D47D69557}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA8">
     <sortCondition ref="M1:M14"/>
   </sortState>
@@ -4058,8 +4046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4739,7 +4727,7 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C24">
         <v>40</v>
@@ -5494,7 +5482,7 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C44">
         <v>95</v>
@@ -5512,13 +5500,13 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C45">
         <v>40</v>
@@ -5536,13 +5524,13 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C46">
         <v>40</v>
@@ -7973,12 +7961,12 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8127,8 +8115,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
@@ -8141,7 +8129,7 @@
       <c r="G7" s="59" t="s">
         <v>488</v>
       </c>
-      <c r="H7" s="101"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="100"/>
@@ -8178,17 +8166,17 @@
         <v>351</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="H9" s="100"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8196,12 +8184,12 @@
         <v>353</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>211</v>
+        <v>581</v>
       </c>
       <c r="G10" s="59" t="s">
         <v>494</v>
       </c>
-      <c r="H10" s="101"/>
+      <c r="H10" s="103"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="100"/>
@@ -8221,7 +8209,7 @@
         <v>461</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="H11" s="99" t="s">
         <v>357</v>
@@ -8307,13 +8295,13 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F16" s="59" t="s">
         <v>463</v>
@@ -8321,7 +8309,7 @@
       <c r="G16" s="59" t="s">
         <v>466</v>
       </c>
-      <c r="H16" s="101"/>
+      <c r="H16" s="103"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="100"/>
@@ -8355,7 +8343,7 @@
         <v>348</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="F18" s="46" t="s">
         <v>352</v>
@@ -8367,8 +8355,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8376,12 +8364,12 @@
         <v>462</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="G19" s="59" t="s">
-        <v>550</v>
-      </c>
-      <c r="H19" s="101"/>
+        <v>547</v>
+      </c>
+      <c r="H19" s="103"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="100"/>
@@ -8398,7 +8386,7 @@
         <v>364</v>
       </c>
       <c r="F20" s="61" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="G20" s="61" t="s">
         <v>365</v>
@@ -8415,10 +8403,10 @@
         <v>348</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="G21" s="46" t="s">
         <v>365</v>
@@ -8441,7 +8429,7 @@
       <c r="G22" s="60" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="103"/>
+      <c r="H22" s="101"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="100"/>
@@ -8475,7 +8463,7 @@
         <v>348</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F24" s="46" t="s">
         <v>472</v>
@@ -8486,14 +8474,14 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="103"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>470</v>
@@ -8501,7 +8489,7 @@
       <c r="G25" s="47" t="s">
         <v>473</v>
       </c>
-      <c r="H25" s="103"/>
+      <c r="H25" s="101"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="102" t="s">
@@ -8557,10 +8545,10 @@
         <v>345</v>
       </c>
       <c r="E29" s="75" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F29" s="64" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G29" s="76" t="s">
         <v>455</v>
@@ -8577,10 +8565,10 @@
         <v>348</v>
       </c>
       <c r="E30" s="79" t="s">
+        <v>530</v>
+      </c>
+      <c r="F30" s="71" t="s">
         <v>533</v>
-      </c>
-      <c r="F30" s="71" t="s">
-        <v>536</v>
       </c>
       <c r="G30" s="77" t="s">
         <v>209</v>
@@ -8589,21 +8577,21 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="100"/>
-      <c r="B31" s="101"/>
-      <c r="C31" s="101"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E31" s="78" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>531</v>
-      </c>
-      <c r="H31" s="101"/>
+        <v>528</v>
+      </c>
+      <c r="H31" s="103"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="100"/>
@@ -8617,13 +8605,13 @@
         <v>345</v>
       </c>
       <c r="E32" s="73" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="F32" s="80" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="G32" s="73" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="H32" s="100" t="s">
         <v>347</v>
@@ -8637,13 +8625,13 @@
         <v>348</v>
       </c>
       <c r="E33" s="79" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F33" s="71" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="G33" s="79" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H33" s="100"/>
     </row>
@@ -8655,13 +8643,13 @@
         <v>349</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F34" s="81" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="G34" s="67" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H34" s="100"/>
     </row>
@@ -8743,7 +8731,7 @@
         <v>501</v>
       </c>
       <c r="G38" s="63" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="H38" s="99" t="s">
         <v>370</v>
@@ -8775,7 +8763,7 @@
         <v>349</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F40" s="81" t="s">
         <v>505</v>
@@ -8803,7 +8791,7 @@
         <v>499</v>
       </c>
       <c r="G41" s="86" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H41" s="99" t="s">
         <v>347</v>
@@ -8823,7 +8811,7 @@
         <v>500</v>
       </c>
       <c r="G42" s="87" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="H42" s="100"/>
     </row>
@@ -8841,7 +8829,7 @@
         <v>498</v>
       </c>
       <c r="G43" s="67" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="H43" s="100"/>
     </row>
@@ -8860,10 +8848,10 @@
         <v>518</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="G44" s="68" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H44" s="99" t="s">
         <v>347</v>
@@ -8877,13 +8865,13 @@
         <v>348</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="F45" s="69" t="s">
-        <v>578</v>
+        <v>584</v>
       </c>
       <c r="G45" s="69" t="s">
-        <v>519</v>
+        <v>585</v>
       </c>
       <c r="H45" s="100"/>
     </row>
@@ -8895,13 +8883,13 @@
         <v>349</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="F46" s="81" t="s">
-        <v>520</v>
+        <v>583</v>
       </c>
       <c r="G46" s="67" t="s">
-        <v>521</v>
+        <v>586</v>
       </c>
       <c r="H46" s="100"/>
     </row>
@@ -8948,9 +8936,9 @@
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="103"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="103"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
@@ -8963,22 +8951,35 @@
       <c r="G49" s="84" t="s">
         <v>512</v>
       </c>
-      <c r="H49" s="103"/>
+      <c r="H49" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="H35:H37"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8995,34 +8996,20 @@
     <mergeCell ref="H17:H19"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9575,19 +9562,19 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B16" s="14"/>
     </row>
@@ -9596,19 +9583,19 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B20" s="14"/>
     </row>
@@ -10895,7 +10882,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -12201,7 +12188,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B16">
         <v>19</v>
@@ -16761,7 +16748,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B55">
         <v>31</v>
@@ -16773,7 +16760,7 @@
         <v>76</v>
       </c>
       <c r="E55" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -16838,7 +16825,7 @@
         <v>0.3</v>
       </c>
       <c r="Z55" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
@@ -16864,7 +16851,7 @@
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
@@ -17964,7 +17951,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -18030,7 +18017,7 @@
         <v>76</v>
       </c>
       <c r="W14" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="X14">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W14,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -18044,12 +18031,12 @@
         <v>178</v>
       </c>
       <c r="AA14" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B15">
         <v>37</v>
@@ -18115,7 +18102,7 @@
         <v>76</v>
       </c>
       <c r="W15" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="X15">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W15,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -18129,7 +18116,7 @@
         <v>178</v>
       </c>
       <c r="AA15" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -19309,11 +19296,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0094531B-7BBB-4DD3-8835-99962592A6C6}">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M14" sqref="M14"/>
+      <selection pane="topRight" activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19536,19 +19523,19 @@
         <v>76</v>
       </c>
       <c r="J3">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="K3">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="L3" t="s">
         <v>76</v>
       </c>
       <c r="M3">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="N3">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="O3" t="s">
         <v>76</v>
@@ -19840,13 +19827,13 @@
         <v>222</v>
       </c>
       <c r="B7">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>212</v>
       </c>
-      <c r="D7" t="s">
-        <v>76</v>
+      <c r="D7">
+        <v>55000</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -19864,28 +19851,28 @@
         <v>76</v>
       </c>
       <c r="J7">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K7">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
         <v>76</v>
       </c>
       <c r="M7">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="N7">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="O7" t="s">
         <v>76</v>
       </c>
       <c r="P7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="Q7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="R7">
         <v>200</v>
@@ -20083,10 +20070,10 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B10">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
         <v>212</v>
@@ -20110,19 +20097,19 @@
         <v>76</v>
       </c>
       <c r="J10">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="K10">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="L10" t="s">
         <v>76</v>
       </c>
       <c r="M10">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="N10">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O10" t="s">
         <v>76</v>
@@ -20131,7 +20118,7 @@
         <v>35</v>
       </c>
       <c r="Q10">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="R10">
         <v>200</v>
@@ -20162,6 +20149,435 @@
       <c r="Z10" t="s">
         <v>213</v>
       </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>575</v>
+      </c>
+      <c r="B11">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11">
+        <v>63000</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11">
+        <v>145</v>
+      </c>
+      <c r="I11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11">
+        <v>60</v>
+      </c>
+      <c r="K11">
+        <v>70</v>
+      </c>
+      <c r="L11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11">
+        <v>65</v>
+      </c>
+      <c r="N11">
+        <v>40</v>
+      </c>
+      <c r="O11" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11">
+        <v>40</v>
+      </c>
+      <c r="Q11">
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <v>200</v>
+      </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
+      <c r="T11" t="s">
+        <v>76</v>
+      </c>
+      <c r="U11">
+        <v>5</v>
+      </c>
+      <c r="V11">
+        <v>15</v>
+      </c>
+      <c r="W11" t="s">
+        <v>120</v>
+      </c>
+      <c r="X11" cm="1">
+        <f t="array" aca="1" ref="X11" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>37</v>
+      </c>
+      <c r="Y11" cm="1">
+        <f t="array" aca="1" ref="Y11" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>576</v>
+      </c>
+      <c r="B12">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>80000</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12">
+        <v>145</v>
+      </c>
+      <c r="I12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12">
+        <v>35</v>
+      </c>
+      <c r="K12">
+        <v>60</v>
+      </c>
+      <c r="L12" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12">
+        <v>40</v>
+      </c>
+      <c r="N12">
+        <v>20</v>
+      </c>
+      <c r="O12" t="s">
+        <v>76</v>
+      </c>
+      <c r="P12">
+        <v>30</v>
+      </c>
+      <c r="Q12">
+        <v>15</v>
+      </c>
+      <c r="R12">
+        <v>200</v>
+      </c>
+      <c r="S12">
+        <v>5</v>
+      </c>
+      <c r="T12" t="s">
+        <v>76</v>
+      </c>
+      <c r="U12">
+        <v>5</v>
+      </c>
+      <c r="V12">
+        <v>15</v>
+      </c>
+      <c r="W12" t="s">
+        <v>120</v>
+      </c>
+      <c r="X12" cm="1">
+        <f t="array" aca="1" ref="X12" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>37</v>
+      </c>
+      <c r="Y12" cm="1">
+        <f t="array" aca="1" ref="Y12" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>577</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13">
+        <v>145</v>
+      </c>
+      <c r="I13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13">
+        <v>45</v>
+      </c>
+      <c r="K13">
+        <v>65</v>
+      </c>
+      <c r="L13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M13">
+        <v>45</v>
+      </c>
+      <c r="N13">
+        <v>25</v>
+      </c>
+      <c r="O13" t="s">
+        <v>76</v>
+      </c>
+      <c r="P13">
+        <v>25</v>
+      </c>
+      <c r="Q13">
+        <v>17</v>
+      </c>
+      <c r="R13">
+        <v>200</v>
+      </c>
+      <c r="S13">
+        <v>5</v>
+      </c>
+      <c r="T13" t="s">
+        <v>76</v>
+      </c>
+      <c r="U13">
+        <v>5</v>
+      </c>
+      <c r="V13">
+        <v>15</v>
+      </c>
+      <c r="W13" t="s">
+        <v>120</v>
+      </c>
+      <c r="X13" cm="1">
+        <f t="array" aca="1" ref="X13" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>37</v>
+      </c>
+      <c r="Y13" cm="1">
+        <f t="array" aca="1" ref="Y13" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>578</v>
+      </c>
+      <c r="B14" s="113">
+        <v>48</v>
+      </c>
+      <c r="C14" s="113" t="s">
+        <v>212</v>
+      </c>
+      <c r="D14" s="113">
+        <v>57000</v>
+      </c>
+      <c r="E14" s="113" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="113" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="113" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="113">
+        <v>145</v>
+      </c>
+      <c r="I14" s="113" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="113">
+        <v>55</v>
+      </c>
+      <c r="K14" s="113">
+        <v>60</v>
+      </c>
+      <c r="L14" s="113" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="113">
+        <v>63</v>
+      </c>
+      <c r="N14" s="113">
+        <v>35</v>
+      </c>
+      <c r="O14" s="113" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14" s="113">
+        <v>30</v>
+      </c>
+      <c r="Q14" s="113">
+        <v>20</v>
+      </c>
+      <c r="R14" s="113">
+        <v>200</v>
+      </c>
+      <c r="S14">
+        <v>5</v>
+      </c>
+      <c r="T14" t="s">
+        <v>76</v>
+      </c>
+      <c r="U14">
+        <v>5</v>
+      </c>
+      <c r="V14">
+        <v>15</v>
+      </c>
+      <c r="W14" t="s">
+        <v>120</v>
+      </c>
+      <c r="X14" cm="1">
+        <f t="array" aca="1" ref="X14" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>37</v>
+      </c>
+      <c r="Y14" cm="1">
+        <f t="array" aca="1" ref="Y14" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>579</v>
+      </c>
+      <c r="B15">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15">
+        <v>60000</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15">
+        <v>145</v>
+      </c>
+      <c r="I15" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15">
+        <v>50</v>
+      </c>
+      <c r="K15">
+        <v>75</v>
+      </c>
+      <c r="L15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15">
+        <v>50</v>
+      </c>
+      <c r="N15">
+        <v>23</v>
+      </c>
+      <c r="O15" t="s">
+        <v>76</v>
+      </c>
+      <c r="P15">
+        <v>30</v>
+      </c>
+      <c r="Q15">
+        <v>15</v>
+      </c>
+      <c r="R15">
+        <v>200</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="T15" t="s">
+        <v>76</v>
+      </c>
+      <c r="U15">
+        <v>5</v>
+      </c>
+      <c r="V15">
+        <v>15</v>
+      </c>
+      <c r="W15" t="s">
+        <v>26</v>
+      </c>
+      <c r="X15" cm="1">
+        <f t="array" aca="1" ref="X15" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+        <v>45</v>
+      </c>
+      <c r="Y15" cm="1">
+        <f t="array" aca="1" ref="Y15" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+        <v>0.6</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="113"/>
+      <c r="C20" s="113"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="113"/>
+      <c r="F20" s="113"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="113"/>
+      <c r="L20" s="113"/>
+      <c r="M20" s="113"/>
+      <c r="N20" s="113"/>
+      <c r="O20" s="113"/>
+      <c r="P20" s="113"/>
+      <c r="Q20" s="113"/>
+      <c r="R20" s="113"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20801,7 +21217,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -20867,7 +21283,7 @@
         <v>76</v>
       </c>
       <c r="W8" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="X8" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B35:'Caliber'!C45,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B45,0),2)</f>
@@ -20881,7 +21297,7 @@
         <v>82</v>
       </c>
       <c r="AA8" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
5.56 100x drum, LMG research, reorganized & swapped sounds
Swapped sounds on the fmg9, mp7, p90 (sopmod), P226, Sako and Ultimax to better fitting ones.
New sounds for double barrel.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE496348-7910-43FB-9E24-D3C1F35B7E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B16DD70-0ABC-48BF-9995-CA3F96B5D7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -2594,7 +2594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2846,13 +2846,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2882,7 +2882,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7965,7 +7964,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C44" sqref="C44:C46"/>
     </sheetView>
   </sheetViews>
@@ -8115,8 +8114,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100"/>
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
@@ -8129,7 +8128,7 @@
       <c r="G7" s="59" t="s">
         <v>488</v>
       </c>
-      <c r="H7" s="103"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="100"/>
@@ -8175,8 +8174,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8189,7 +8188,7 @@
       <c r="G10" s="59" t="s">
         <v>494</v>
       </c>
-      <c r="H10" s="103"/>
+      <c r="H10" s="101"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="100"/>
@@ -8295,8 +8294,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="103"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="101"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
@@ -8309,7 +8308,7 @@
       <c r="G16" s="59" t="s">
         <v>466</v>
       </c>
-      <c r="H16" s="103"/>
+      <c r="H16" s="101"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="100"/>
@@ -8355,8 +8354,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
-      <c r="B19" s="103"/>
-      <c r="C19" s="103"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="101"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8369,7 +8368,7 @@
       <c r="G19" s="59" t="s">
         <v>547</v>
       </c>
-      <c r="H19" s="103"/>
+      <c r="H19" s="101"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="100"/>
@@ -8429,7 +8428,7 @@
       <c r="G22" s="60" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="101"/>
+      <c r="H22" s="103"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="100"/>
@@ -8474,9 +8473,9 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="101"/>
-      <c r="B25" s="101"/>
-      <c r="C25" s="101"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
@@ -8489,7 +8488,7 @@
       <c r="G25" s="47" t="s">
         <v>473</v>
       </c>
-      <c r="H25" s="101"/>
+      <c r="H25" s="103"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="102" t="s">
@@ -8577,8 +8576,8 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="100"/>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
@@ -8591,7 +8590,7 @@
       <c r="G31" s="78" t="s">
         <v>528</v>
       </c>
-      <c r="H31" s="103"/>
+      <c r="H31" s="101"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="100"/>
@@ -8936,9 +8935,9 @@
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="101"/>
-      <c r="B49" s="101"/>
-      <c r="C49" s="101"/>
+      <c r="A49" s="103"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="103"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
@@ -8951,19 +8950,38 @@
       <c r="G49" s="84" t="s">
         <v>512</v>
       </c>
-      <c r="H49" s="101"/>
+      <c r="H49" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A26:A49"/>
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="C26:C28"/>
@@ -8980,34 +8998,15 @@
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="H35:H37"/>
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10971,7 +10970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="W16" sqref="W16"/>
     </sheetView>
@@ -19296,9 +19295,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0094531B-7BBB-4DD3-8835-99962592A6C6}">
-  <dimension ref="A1:AA20"/>
+  <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q26" sqref="Q26"/>
     </sheetView>
@@ -20400,55 +20399,55 @@
       <c r="A14" t="s">
         <v>578</v>
       </c>
-      <c r="B14" s="113">
+      <c r="B14">
         <v>48</v>
       </c>
-      <c r="C14" s="113" t="s">
+      <c r="C14" t="s">
         <v>212</v>
       </c>
-      <c r="D14" s="113">
+      <c r="D14">
         <v>57000</v>
       </c>
-      <c r="E14" s="113" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="113" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="113" t="s">
-        <v>76</v>
-      </c>
-      <c r="H14" s="113">
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14">
         <v>145</v>
       </c>
-      <c r="I14" s="113" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="113">
+      <c r="I14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14">
         <v>55</v>
       </c>
-      <c r="K14" s="113">
+      <c r="K14">
         <v>60</v>
       </c>
-      <c r="L14" s="113" t="s">
-        <v>76</v>
-      </c>
-      <c r="M14" s="113">
+      <c r="L14" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14">
         <v>63</v>
       </c>
-      <c r="N14" s="113">
+      <c r="N14">
         <v>35</v>
       </c>
-      <c r="O14" s="113" t="s">
-        <v>76</v>
-      </c>
-      <c r="P14" s="113">
+      <c r="O14" t="s">
+        <v>76</v>
+      </c>
+      <c r="P14">
         <v>30</v>
       </c>
-      <c r="Q14" s="113">
+      <c r="Q14">
         <v>20</v>
       </c>
-      <c r="R14" s="113">
+      <c r="R14">
         <v>200</v>
       </c>
       <c r="S14">
@@ -20559,25 +20558,6 @@
       <c r="Z15" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="113"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="113"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="113"/>
-      <c r="G20" s="113"/>
-      <c r="H20" s="113"/>
-      <c r="I20" s="113"/>
-      <c r="J20" s="113"/>
-      <c r="K20" s="113"/>
-      <c r="L20" s="113"/>
-      <c r="M20" s="113"/>
-      <c r="N20" s="113"/>
-      <c r="O20" s="113"/>
-      <c r="P20" s="113"/>
-      <c r="Q20" s="113"/>
-      <c r="R20" s="113"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bugfixes, itemset changes, Flashbanged color changes
fixed missing flor on CITY14.map
Fixed uniform NV having the wrong sprite on one of the models
Flashbanged units now flash blue
Partially flashed units now flash dark purple.
Updated todo list.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B16DD70-0ABC-48BF-9995-CA3F96B5D7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5949F3C4-8FE8-4A43-A15A-4D349D005628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="7" activeTab="7" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="589">
   <si>
     <t>Name</t>
   </si>
@@ -1558,12 +1558,6 @@
     <t>Spas12/Remington 870/Spas12(slug)</t>
   </si>
   <si>
-    <t>Spas12/Remington 870 (slug)/Spas12 (inc)</t>
-  </si>
-  <si>
-    <t>Remington 870/M3 (slug)/M3 (inc)</t>
-  </si>
-  <si>
     <t>KS-23/KS-23 (slug)/KS-23(NL)</t>
   </si>
   <si>
@@ -1922,6 +1916,18 @@
   </si>
   <si>
     <t>M60E6/M249/Ultimax 100</t>
+  </si>
+  <si>
+    <t>Spas12/Remington 870 (slug)/Spas12</t>
+  </si>
+  <si>
+    <t>Remington 870/M3 (slug)/M3</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Bushmaster ACR</t>
   </si>
 </sst>
 </file>
@@ -2846,13 +2852,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4726,7 +4732,7 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C24">
         <v>40</v>
@@ -5481,7 +5487,7 @@
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C44">
         <v>95</v>
@@ -5499,13 +5505,13 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C45">
         <v>40</v>
@@ -5523,13 +5529,13 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C46">
         <v>40</v>
@@ -7964,8 +7970,8 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44:C46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8021,10 +8027,10 @@
         <v>345</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G2" s="45" t="s">
         <v>346</v>
@@ -8042,13 +8048,13 @@
         <v>348</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H3" s="100"/>
     </row>
@@ -8060,13 +8066,13 @@
         <v>349</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F4" s="60" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G4" s="60" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H4" s="100"/>
     </row>
@@ -8082,13 +8088,13 @@
         <v>345</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H5" s="99" t="s">
         <v>347</v>
@@ -8102,33 +8108,33 @@
         <v>348</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G6" s="46" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H6" s="100"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>488</v>
-      </c>
-      <c r="H7" s="101"/>
+        <v>486</v>
+      </c>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="100"/>
@@ -8142,10 +8148,10 @@
         <v>345</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F8" s="61" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G8" s="61" t="s">
         <v>220</v>
@@ -8165,17 +8171,17 @@
         <v>351</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="H9" s="100"/>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8183,12 +8189,12 @@
         <v>353</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>494</v>
-      </c>
-      <c r="H10" s="101"/>
+        <v>492</v>
+      </c>
+      <c r="H10" s="103"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="100"/>
@@ -8208,7 +8214,7 @@
         <v>461</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="H11" s="99" t="s">
         <v>357</v>
@@ -8225,10 +8231,10 @@
         <v>203</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G12" s="46" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H12" s="100"/>
     </row>
@@ -8262,13 +8268,13 @@
         <v>345</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G14" s="61" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H14" s="99" t="s">
         <v>347</v>
@@ -8282,33 +8288,33 @@
         <v>348</v>
       </c>
       <c r="E15" s="46" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F15" s="46" t="s">
         <v>464</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>465</v>
+        <v>585</v>
       </c>
       <c r="H15" s="100"/>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F16" s="59" t="s">
         <v>463</v>
       </c>
       <c r="G16" s="59" t="s">
-        <v>466</v>
-      </c>
-      <c r="H16" s="101"/>
+        <v>586</v>
+      </c>
+      <c r="H16" s="103"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="100"/>
@@ -8342,7 +8348,7 @@
         <v>348</v>
       </c>
       <c r="E18" s="46" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F18" s="46" t="s">
         <v>352</v>
@@ -8354,8 +8360,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8363,12 +8369,12 @@
         <v>462</v>
       </c>
       <c r="F19" s="59" t="s">
+        <v>543</v>
+      </c>
+      <c r="G19" s="59" t="s">
         <v>545</v>
       </c>
-      <c r="G19" s="59" t="s">
-        <v>547</v>
-      </c>
-      <c r="H19" s="101"/>
+      <c r="H19" s="103"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="100"/>
@@ -8385,7 +8391,7 @@
         <v>364</v>
       </c>
       <c r="F20" s="61" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="G20" s="61" t="s">
         <v>365</v>
@@ -8402,10 +8408,10 @@
         <v>348</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="G21" s="46" t="s">
         <v>365</v>
@@ -8428,7 +8434,7 @@
       <c r="G22" s="60" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="103"/>
+      <c r="H22" s="101"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="100"/>
@@ -8445,10 +8451,10 @@
         <v>148</v>
       </c>
       <c r="F23" s="61" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G23" s="61" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H23" s="102" t="s">
         <v>355</v>
@@ -8462,33 +8468,33 @@
         <v>348</v>
       </c>
       <c r="E24" s="65" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F24" s="46" t="s">
+        <v>470</v>
+      </c>
+      <c r="G24" s="46" t="s">
         <v>472</v>
       </c>
-      <c r="G24" s="46" t="s">
-        <v>474</v>
-      </c>
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="103"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
       <c r="E25" s="47" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G25" s="47" t="s">
-        <v>473</v>
-      </c>
-      <c r="H25" s="103"/>
+        <v>471</v>
+      </c>
+      <c r="H25" s="101"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="102" t="s">
@@ -8544,10 +8550,10 @@
         <v>345</v>
       </c>
       <c r="E29" s="75" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F29" s="64" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="G29" s="76" t="s">
         <v>455</v>
@@ -8564,10 +8570,10 @@
         <v>348</v>
       </c>
       <c r="E30" s="79" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F30" s="71" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="G30" s="77" t="s">
         <v>209</v>
@@ -8576,21 +8582,21 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="100"/>
-      <c r="B31" s="101"/>
-      <c r="C31" s="101"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
       <c r="E31" s="78" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F31" s="74" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>528</v>
-      </c>
-      <c r="H31" s="101"/>
+        <v>526</v>
+      </c>
+      <c r="H31" s="103"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="100"/>
@@ -8604,13 +8610,13 @@
         <v>345</v>
       </c>
       <c r="E32" s="73" t="s">
+        <v>521</v>
+      </c>
+      <c r="F32" s="80" t="s">
+        <v>522</v>
+      </c>
+      <c r="G32" s="73" t="s">
         <v>523</v>
-      </c>
-      <c r="F32" s="80" t="s">
-        <v>524</v>
-      </c>
-      <c r="G32" s="73" t="s">
-        <v>525</v>
       </c>
       <c r="H32" s="100" t="s">
         <v>347</v>
@@ -8624,13 +8630,13 @@
         <v>348</v>
       </c>
       <c r="E33" s="79" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F33" s="71" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="G33" s="79" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H33" s="100"/>
     </row>
@@ -8642,13 +8648,13 @@
         <v>349</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F34" s="81" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="G34" s="67" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H34" s="100"/>
     </row>
@@ -8664,13 +8670,13 @@
         <v>345</v>
       </c>
       <c r="E35" s="75" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="G35" s="75" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H35" s="99" t="s">
         <v>347</v>
@@ -8684,13 +8690,13 @@
         <v>348</v>
       </c>
       <c r="E36" s="79" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F36" s="79" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G36" s="79" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H36" s="100"/>
     </row>
@@ -8702,13 +8708,13 @@
         <v>349</v>
       </c>
       <c r="E37" s="90" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F37" s="90" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="G37" s="90" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H37" s="100"/>
     </row>
@@ -8724,13 +8730,13 @@
         <v>345</v>
       </c>
       <c r="E38" s="63" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F38" s="85" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G38" s="63" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="H38" s="99" t="s">
         <v>370</v>
@@ -8744,13 +8750,13 @@
         <v>348</v>
       </c>
       <c r="E39" s="79" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F39" s="71" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="G39" s="79" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H39" s="100"/>
     </row>
@@ -8762,13 +8768,13 @@
         <v>349</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F40" s="81" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="G40" s="67" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H40" s="100"/>
     </row>
@@ -8784,13 +8790,13 @@
         <v>345</v>
       </c>
       <c r="E41" s="86" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F41" s="80" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="G41" s="86" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="H41" s="99" t="s">
         <v>347</v>
@@ -8804,13 +8810,13 @@
         <v>348</v>
       </c>
       <c r="E42" s="87" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F42" s="88" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G42" s="87" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="H42" s="100"/>
     </row>
@@ -8822,13 +8828,13 @@
         <v>349</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F43" s="89" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="G43" s="67" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="H43" s="100"/>
     </row>
@@ -8844,13 +8850,13 @@
         <v>345</v>
       </c>
       <c r="E44" s="68" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F44" s="82" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G44" s="68" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H44" s="99" t="s">
         <v>347</v>
@@ -8864,13 +8870,13 @@
         <v>348</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F45" s="69" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="G45" s="69" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="H45" s="100"/>
     </row>
@@ -8882,13 +8888,13 @@
         <v>349</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F46" s="81" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="G46" s="67" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="H46" s="100"/>
     </row>
@@ -8907,10 +8913,10 @@
         <v>158</v>
       </c>
       <c r="F47" s="80" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="G47" s="63" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H47" s="99" t="s">
         <v>347</v>
@@ -8924,48 +8930,61 @@
         <v>348</v>
       </c>
       <c r="E48" s="70" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F48" s="83" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="G48" s="70" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="103"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="103"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
       <c r="E49" s="84" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F49" s="72" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="G49" s="84" t="s">
-        <v>512</v>
-      </c>
-      <c r="H49" s="103"/>
+        <v>510</v>
+      </c>
+      <c r="H49" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="H35:H37"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -8982,31 +9001,18 @@
     <mergeCell ref="H17:H19"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9493,7 +9499,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9561,19 +9567,19 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B16" s="14"/>
     </row>
@@ -9582,26 +9588,32 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>587</v>
+      </c>
       <c r="B21" s="14"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>588</v>
+      </c>
       <c r="B22" s="14"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -10881,7 +10893,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -10970,7 +10982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941F1AF2-A8AA-477B-ABE7-7C87546ECF29}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="W16" sqref="W16"/>
     </sheetView>
@@ -12187,7 +12199,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B16">
         <v>19</v>
@@ -12277,7 +12289,7 @@
   <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
@@ -16747,7 +16759,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B55">
         <v>31</v>
@@ -16759,7 +16771,7 @@
         <v>76</v>
       </c>
       <c r="E55" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -16824,7 +16836,7 @@
         <v>0.3</v>
       </c>
       <c r="Z55" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
@@ -17950,7 +17962,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -18016,7 +18028,7 @@
         <v>76</v>
       </c>
       <c r="W14" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="X14">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W14,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -18030,12 +18042,12 @@
         <v>178</v>
       </c>
       <c r="AA14" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B15">
         <v>37</v>
@@ -18101,7 +18113,7 @@
         <v>76</v>
       </c>
       <c r="W15" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="X15">
         <f>INDEX(Caliber!B13:'Caliber'!C24,MATCH(W15,Caliber!B13:'Caliber'!B24,0),2)</f>
@@ -18115,7 +18127,7 @@
         <v>178</v>
       </c>
       <c r="AA15" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -20069,7 +20081,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B10">
         <v>78</v>
@@ -20151,7 +20163,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B11">
         <v>36</v>
@@ -20233,7 +20245,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="B12">
         <v>39</v>
@@ -20315,7 +20327,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B13">
         <v>30</v>
@@ -20397,7 +20409,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B14">
         <v>48</v>
@@ -20479,7 +20491,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B15">
         <v>47</v>
@@ -20572,7 +20584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B2364D-F43A-47E4-8B6C-A03FB84E628E}">
   <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AA11" sqref="AA11"/>
     </sheetView>
@@ -21197,7 +21209,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B8">
         <v>30</v>
@@ -21263,7 +21275,7 @@
         <v>76</v>
       </c>
       <c r="W8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="X8" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B35:'Caliber'!C45,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B35:'Caliber'!B45,0),2)</f>
@@ -21277,7 +21289,7 @@
         <v>82</v>
       </c>
       <c r="AA8" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bugfixes, balance changes, research changes
Balance:
M3 now has more aimed accuracy, and significantly increased range.
Buckshot damage 25->18.
Operators now cost 100k on veteran and below.
LMG Movement inaccuracy system added, Including ufopaedia article explaining system
Research:
GL acquisition no longer blocked by AT acquisition.
Separated breaching tool acquisitions, no longer mutually exclusive, Hammer at equipment acquisition, Serbu at military acquisition, C4 after High explosives.
Misc:
Changed Raider sprite to display armor.
Fixed OFFICE02 staircase being blocked.
Fixed spawn rates of office varients.
Updated draw.io file.
Updated changelog.
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30BB084-4856-4151-8D01-F058E065B84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF3C05C-572B-4B25-A2FB-BC96D923F020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="7" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -49,6 +49,31 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ethan McLaughlin</author>
+  </authors>
+  <commentList>
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{2BD37C75-D1E9-4229-BF01-F9B4377D63A0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>For every 1% of Missing TUs, accuracy multiplyer bonus is decreased by (1 * mvmt pen.) / 100.
+e.g 85 mvmnt pen = -0.85% acc multiplier per 1% TU missing</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Ethan McLaughlin</author>
@@ -95,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="592">
   <si>
     <t>Name</t>
   </si>
@@ -1934,13 +1959,16 @@
   </si>
   <si>
     <t>MASS standalone</t>
+  </si>
+  <si>
+    <t>Movement pen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1974,6 +2002,13 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="25">
@@ -3445,12 +3480,12 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7B36A2CF-DAA4-4B61-B862-8F0D47D69557}" name="Table3" displayName="Table3" ref="A1:AA15" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:AA15" xr:uid="{7B36A2CF-DAA4-4B61-B862-8F0D47D69557}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7B36A2CF-DAA4-4B61-B862-8F0D47D69557}" name="Table3" displayName="Table3" ref="A1:AB15" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:AB15" xr:uid="{7B36A2CF-DAA4-4B61-B862-8F0D47D69557}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AB8">
     <sortCondition ref="M1:M14"/>
   </sortState>
-  <tableColumns count="27">
+  <tableColumns count="28">
     <tableColumn id="1" xr3:uid="{A8BBADB3-0AE9-45E8-9C77-42482A2CF767}" name="Name"/>
     <tableColumn id="2" xr3:uid="{4BB894CD-D6CC-494C-8E57-A9C2E0592C4E}" name="weight"/>
     <tableColumn id="3" xr3:uid="{55D5DA56-1868-4260-8702-A77EACCF3E7D}" name="size"/>
@@ -3470,6 +3505,7 @@
     <tableColumn id="17" xr3:uid="{21DAF817-7B86-4F34-84CB-FAFBBC5FE476}" name="rangeAuto"/>
     <tableColumn id="18" xr3:uid="{0500C1D3-8E98-462B-8E61-4141DA94A55F}" name="maxRange"/>
     <tableColumn id="19" xr3:uid="{8090DF43-6704-4592-A789-709321B97EC1}" name="minRange"/>
+    <tableColumn id="28" xr3:uid="{C20A88B7-0836-4B21-BD6E-76E0A1B95104}" name="Movement pen."/>
     <tableColumn id="20" xr3:uid="{A262F3D1-6339-46F9-A86A-F76EC3AD31DF}" name="Aimed shots"/>
     <tableColumn id="21" xr3:uid="{6922DAA8-0EAD-4280-95AC-BA4DFDA1778A}" name="snap shots"/>
     <tableColumn id="22" xr3:uid="{5014F934-0FCB-42FF-BD38-D462B9CDFF7A}" name="auto shots"/>
@@ -4057,8 +4093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6695E0F0-C0B0-45B8-AA00-1AE0F467FE87}">
   <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4830,7 +4866,7 @@
         <v>33</v>
       </c>
       <c r="C26" s="1">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D26" s="1">
         <v>10</v>
@@ -4969,7 +5005,7 @@
         <v>448</v>
       </c>
       <c r="C29">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D29">
         <v>10</v>
@@ -5042,7 +5078,7 @@
         <v>37</v>
       </c>
       <c r="C31">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D31">
         <v>20</v>
@@ -7975,7 +8011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
@@ -18305,8 +18341,8 @@
   <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB14" sqref="AB14"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18494,7 +18530,7 @@
       </c>
       <c r="X2">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W2,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y2">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W2,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -18580,7 +18616,7 @@
       </c>
       <c r="X3">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W3,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y3">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W3,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -18669,7 +18705,7 @@
       </c>
       <c r="X4">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W4,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y4">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W4,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -18758,7 +18794,7 @@
       </c>
       <c r="X5">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W5,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y5">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W5,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -18847,7 +18883,7 @@
       </c>
       <c r="X6">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W6,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y6">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W6,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -18936,7 +18972,7 @@
       </c>
       <c r="X7">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W7,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y7">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W7,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -19025,7 +19061,7 @@
       </c>
       <c r="X8">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W8,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y8">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W8,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -19114,7 +19150,7 @@
       </c>
       <c r="X9">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W9,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y9">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W9,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -19203,7 +19239,7 @@
       </c>
       <c r="X10">
         <f>INDEX(Caliber!B26:'Caliber'!C33,MATCH(W10,Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y10">
         <f>INDEX(Caliber!B26:'Caliber'!D33,MATCH(W10,Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -19255,7 +19291,7 @@
         <v>76</v>
       </c>
       <c r="L11">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="M11">
         <v>80</v>
@@ -19264,10 +19300,10 @@
         <v>76</v>
       </c>
       <c r="O11">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="P11">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q11" t="s">
         <v>76</v>
@@ -19292,7 +19328,7 @@
       </c>
       <c r="X11" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">INDEX(Caliber!B26:'Caliber'!C33,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B26:'Caliber'!B33,0),2)</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Y11" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">INDEX(Caliber!B26:'Caliber'!D33,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B26:'Caliber'!B33,0),3)</f>
@@ -19318,12 +19354,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0094531B-7BBB-4DD3-8835-99962592A6C6}">
-  <dimension ref="A1:AA15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0094531B-7BBB-4DD3-8835-99962592A6C6}">
+  <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q26" sqref="Q26"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19344,7 +19380,7 @@
     <col min="16" max="17" width="12.42578125" customWidth="1"/>
     <col min="18" max="18" width="12.28515625" customWidth="1"/>
     <col min="19" max="19" width="12" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" customWidth="1"/>
     <col min="21" max="21" width="12.42578125" customWidth="1"/>
     <col min="22" max="22" width="12.28515625" customWidth="1"/>
     <col min="23" max="23" width="18.5703125" customWidth="1"/>
@@ -19352,7 +19388,7 @@
     <col min="26" max="26" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -19411,31 +19447,34 @@
         <v>73</v>
       </c>
       <c r="T1" s="19" t="s">
+        <v>591</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>211</v>
       </c>
@@ -19493,31 +19532,34 @@
       <c r="S2">
         <v>5</v>
       </c>
-      <c r="T2" t="s">
-        <v>76</v>
-      </c>
-      <c r="U2">
+      <c r="T2">
+        <v>85</v>
+      </c>
+      <c r="U2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V2">
         <v>5</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>15</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>26</v>
       </c>
-      <c r="X2" cm="1">
-        <f t="array" aca="1" ref="X2" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y2" cm="1">
+        <f t="array" aca="1" ref="Y2" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>45</v>
       </c>
-      <c r="Y2" cm="1">
-        <f t="array" aca="1" ref="Y2" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Z2" cm="1">
+        <f t="array" aca="1" ref="Z2" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>0.6</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -19575,31 +19617,34 @@
       <c r="S3">
         <v>5</v>
       </c>
-      <c r="T3" t="s">
-        <v>76</v>
-      </c>
-      <c r="U3">
+      <c r="T3">
+        <v>85</v>
+      </c>
+      <c r="U3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V3">
         <v>5</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>15</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>120</v>
       </c>
-      <c r="X3" cm="1">
-        <f t="array" aca="1" ref="X3" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y3" cm="1">
+        <f t="array" aca="1" ref="Y3" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>37</v>
       </c>
-      <c r="Y3" cm="1">
-        <f t="array" aca="1" ref="Y3" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Z3" cm="1">
+        <f t="array" aca="1" ref="Z3" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>0.4</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -19657,31 +19702,34 @@
       <c r="S4">
         <v>5</v>
       </c>
-      <c r="T4" t="s">
-        <v>76</v>
-      </c>
-      <c r="U4">
+      <c r="T4">
+        <v>85</v>
+      </c>
+      <c r="U4" t="s">
+        <v>76</v>
+      </c>
+      <c r="V4">
         <v>5</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>15</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>221</v>
       </c>
-      <c r="X4" cm="1">
-        <f t="array" aca="1" ref="X4" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y4" cm="1">
+        <f t="array" aca="1" ref="Y4" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>49</v>
       </c>
-      <c r="Y4" cm="1">
-        <f t="array" aca="1" ref="Y4" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Z4" cm="1">
+        <f t="array" aca="1" ref="Z4" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>0.7</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -19739,31 +19787,34 @@
       <c r="S5">
         <v>5</v>
       </c>
-      <c r="T5" t="s">
-        <v>76</v>
-      </c>
-      <c r="U5">
+      <c r="T5">
+        <v>85</v>
+      </c>
+      <c r="U5" t="s">
+        <v>76</v>
+      </c>
+      <c r="V5">
         <v>5</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>15</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>26</v>
       </c>
-      <c r="X5" cm="1">
-        <f t="array" aca="1" ref="X5" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y5" cm="1">
+        <f t="array" aca="1" ref="Y5" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>45</v>
       </c>
-      <c r="Y5" cm="1">
-        <f t="array" aca="1" ref="Y5" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Z5" cm="1">
+        <f t="array" aca="1" ref="Z5" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>0.6</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>216</v>
       </c>
@@ -19821,31 +19872,34 @@
       <c r="S6">
         <v>5</v>
       </c>
-      <c r="T6" t="s">
-        <v>76</v>
-      </c>
-      <c r="U6">
+      <c r="T6">
+        <v>85</v>
+      </c>
+      <c r="U6" t="s">
+        <v>76</v>
+      </c>
+      <c r="V6">
         <v>5</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>15</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>120</v>
       </c>
-      <c r="X6" cm="1">
-        <f t="array" aca="1" ref="X6" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y6" cm="1">
+        <f t="array" aca="1" ref="Y6" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>37</v>
       </c>
-      <c r="Y6" cm="1">
-        <f t="array" aca="1" ref="Y6" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Z6" cm="1">
+        <f t="array" aca="1" ref="Z6" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>0.4</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -19903,31 +19957,34 @@
       <c r="S7">
         <v>5</v>
       </c>
-      <c r="T7" t="s">
-        <v>76</v>
-      </c>
-      <c r="U7">
+      <c r="T7">
+        <v>85</v>
+      </c>
+      <c r="U7" t="s">
+        <v>76</v>
+      </c>
+      <c r="V7">
         <v>5</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>15</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>120</v>
       </c>
-      <c r="X7" cm="1">
-        <f t="array" aca="1" ref="X7" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y7" cm="1">
+        <f t="array" aca="1" ref="Y7" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>37</v>
       </c>
-      <c r="Y7" cm="1">
-        <f t="array" aca="1" ref="Y7" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Z7" cm="1">
+        <f t="array" aca="1" ref="Z7" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>0.4</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>218</v>
       </c>
@@ -19985,31 +20042,34 @@
       <c r="S8">
         <v>5</v>
       </c>
-      <c r="T8" t="s">
-        <v>76</v>
-      </c>
-      <c r="U8">
+      <c r="T8">
+        <v>85</v>
+      </c>
+      <c r="U8" t="s">
+        <v>76</v>
+      </c>
+      <c r="V8">
         <v>5</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>15</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>19</v>
       </c>
-      <c r="X8" cm="1">
-        <f t="array" aca="1" ref="X8" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y8" cm="1">
+        <f t="array" aca="1" ref="Y8" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>36</v>
       </c>
-      <c r="Y8" cm="1">
-        <f t="array" aca="1" ref="Y8" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Z8" cm="1">
+        <f t="array" aca="1" ref="Z8" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>0.3</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>445</v>
       </c>
@@ -20068,30 +20128,33 @@
         <v>4</v>
       </c>
       <c r="T9">
+        <v>85</v>
+      </c>
+      <c r="U9">
         <v>2</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>5</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>15</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>443</v>
       </c>
-      <c r="X9" cm="1">
-        <f t="array" aca="1" ref="X9" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
+      <c r="Y9" cm="1">
+        <f t="array" aca="1" ref="Y9" ca="1">INDEX(Caliber!B2:'Caliber'!C11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B2:'Caliber'!B11,0),2)</f>
         <v>30</v>
       </c>
-      <c r="Y9" cm="1">
-        <f t="array" aca="1" ref="Y9" ca="1">INDEX(Caliber!C2:'Caliber'!D11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B2:'Caliber'!B11,0),2)</f>
+      <c r="Z9" cm="1">
+        <f t="array" aca="1" ref="Z9" ca="1">INDEX(Caliber!C2:'Caliber'!D11,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B2:'Caliber'!B11,0),2)</f>
         <v>0.35</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>568</v>
       </c>
@@ -20149,31 +20212,34 @@
       <c r="S10">
         <v>5</v>
       </c>
-      <c r="T10" t="s">
-        <v>76</v>
-      </c>
-      <c r="U10">
+      <c r="T10">
+        <v>85</v>
+      </c>
+      <c r="U10" t="s">
+        <v>76</v>
+      </c>
+      <c r="V10">
         <v>5</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>15</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>26</v>
       </c>
-      <c r="X10" cm="1">
-        <f t="array" aca="1" ref="X10" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y10" cm="1">
+        <f t="array" aca="1" ref="Y10" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>45</v>
       </c>
-      <c r="Y10" cm="1">
-        <f t="array" aca="1" ref="Y10" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Z10" cm="1">
+        <f t="array" aca="1" ref="Z10" ca="1">INDEX(Caliber!C13:'Caliber'!D23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>0.6</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>572</v>
       </c>
@@ -20231,31 +20297,34 @@
       <c r="S11">
         <v>5</v>
       </c>
-      <c r="T11" t="s">
-        <v>76</v>
-      </c>
-      <c r="U11">
+      <c r="T11">
+        <v>50</v>
+      </c>
+      <c r="U11" t="s">
+        <v>76</v>
+      </c>
+      <c r="V11">
         <v>5</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>15</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
         <v>120</v>
       </c>
-      <c r="X11" cm="1">
-        <f t="array" aca="1" ref="X11" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y11" cm="1">
+        <f t="array" aca="1" ref="Y11" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>37</v>
       </c>
-      <c r="Y11" cm="1">
-        <f t="array" aca="1" ref="Y11" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+      <c r="Z11" cm="1">
+        <f t="array" aca="1" ref="Z11" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
         <v>0.4</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>573</v>
       </c>
@@ -20313,31 +20382,34 @@
       <c r="S12">
         <v>5</v>
       </c>
-      <c r="T12" t="s">
-        <v>76</v>
-      </c>
-      <c r="U12">
+      <c r="T12">
+        <v>85</v>
+      </c>
+      <c r="U12" t="s">
+        <v>76</v>
+      </c>
+      <c r="V12">
         <v>5</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>15</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>120</v>
       </c>
-      <c r="X12" cm="1">
-        <f t="array" aca="1" ref="X12" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y12" cm="1">
+        <f t="array" aca="1" ref="Y12" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>37</v>
       </c>
-      <c r="Y12" cm="1">
-        <f t="array" aca="1" ref="Y12" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+      <c r="Z12" cm="1">
+        <f t="array" aca="1" ref="Z12" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
         <v>0.4</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>574</v>
       </c>
@@ -20395,31 +20467,34 @@
       <c r="S13">
         <v>5</v>
       </c>
-      <c r="T13" t="s">
-        <v>76</v>
-      </c>
-      <c r="U13">
+      <c r="T13">
+        <v>85</v>
+      </c>
+      <c r="U13" t="s">
+        <v>76</v>
+      </c>
+      <c r="V13">
         <v>5</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>15</v>
       </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
         <v>120</v>
       </c>
-      <c r="X13" cm="1">
-        <f t="array" aca="1" ref="X13" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y13" cm="1">
+        <f t="array" aca="1" ref="Y13" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>37</v>
       </c>
-      <c r="Y13" cm="1">
-        <f t="array" aca="1" ref="Y13" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+      <c r="Z13" cm="1">
+        <f t="array" aca="1" ref="Z13" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
         <v>0.4</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AA13" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>575</v>
       </c>
@@ -20477,31 +20552,34 @@
       <c r="S14">
         <v>5</v>
       </c>
-      <c r="T14" t="s">
-        <v>76</v>
-      </c>
-      <c r="U14">
+      <c r="T14">
+        <v>85</v>
+      </c>
+      <c r="U14" t="s">
+        <v>76</v>
+      </c>
+      <c r="V14">
         <v>5</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>15</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>120</v>
       </c>
-      <c r="X14" cm="1">
-        <f t="array" aca="1" ref="X14" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y14" cm="1">
+        <f t="array" aca="1" ref="Y14" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>37</v>
       </c>
-      <c r="Y14" cm="1">
-        <f t="array" aca="1" ref="Y14" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+      <c r="Z14" cm="1">
+        <f t="array" aca="1" ref="Z14" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
         <v>0.4</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>576</v>
       </c>
@@ -20559,35 +20637,39 @@
       <c r="S15">
         <v>5</v>
       </c>
-      <c r="T15" t="s">
-        <v>76</v>
-      </c>
-      <c r="U15">
+      <c r="T15">
+        <v>85</v>
+      </c>
+      <c r="U15" t="s">
+        <v>76</v>
+      </c>
+      <c r="V15">
         <v>5</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>15</v>
       </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
         <v>26</v>
       </c>
-      <c r="X15" cm="1">
-        <f t="array" aca="1" ref="X15" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
+      <c r="Y15" cm="1">
+        <f t="array" aca="1" ref="Y15" ca="1">INDEX(Caliber!B13:'Caliber'!C23,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-1)),Caliber!B13:'Caliber'!B23,0),2)</f>
         <v>45</v>
       </c>
-      <c r="Y15" cm="1">
-        <f t="array" aca="1" ref="Y15" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
+      <c r="Z15" cm="1">
+        <f t="array" aca="1" ref="Z15" ca="1">INDEX(Caliber!C14:'Caliber'!D24,MATCH(INDIRECT(ADDRESS(ROW(),COLUMN()-2)),Caliber!B14:'Caliber'!B24,0),2)</f>
         <v>0.6</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
LMG inaccuracy now uses stamina instead of TUs
Changed LMG inaccuracy to now use stamina instead of TUs.
Adjusted APAV40 sprite position.
Updated translation
</commit_message>
<xml_diff>
--- a/CTO Wepon stat spreadsheet.xlsx
+++ b/CTO Wepon stat spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\OpenXcom\mods\IDT_Counter_Terrorist_Operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCC7667-06D5-46F1-A774-318AA0298414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD9858E-BB72-4436-972D-75B7692887F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" firstSheet="6" activeTab="11" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
+    <workbookView xWindow="28680" yWindow="735" windowWidth="19440" windowHeight="15000" activeTab="6" xr2:uid="{5CCF0F11-6EA0-4BA3-9FDA-51D6C50FE267}"/>
   </bookViews>
   <sheets>
     <sheet name="Caliber" sheetId="1" r:id="rId1"/>
@@ -64,8 +64,8 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>For every 1% of Missing TUs, accuracy multiplyer bonus is decreased by (1 * mvmt pen.) / 100.
-e.g 85 mvmnt pen = -0.85% acc multiplier per 1% TU missing</t>
+          <t>For every 1% of Missing stamina, accuracy multiplyer bonus is decreased by (1 * mvmt pen.) / 100.
+e.g 85 mvmnt pen = -0.85% acc multiplier per 1% stamina missing</t>
         </r>
       </text>
     </comment>
@@ -2893,13 +2893,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8011,7 +8011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21C18DE-CCD8-4ABA-9B3B-CCD73CA8C93E}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
@@ -8162,8 +8162,8 @@
     </row>
     <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="59" t="s">
         <v>349</v>
       </c>
@@ -8176,7 +8176,7 @@
       <c r="G7" s="59" t="s">
         <v>486</v>
       </c>
-      <c r="H7" s="101"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="100"/>
@@ -8222,8 +8222,8 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="59" t="s">
         <v>349</v>
       </c>
@@ -8236,7 +8236,7 @@
       <c r="G10" s="59" t="s">
         <v>491</v>
       </c>
-      <c r="H10" s="101"/>
+      <c r="H10" s="103"/>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="100"/>
@@ -8342,8 +8342,8 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="100"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="59" t="s">
         <v>349</v>
       </c>
@@ -8356,7 +8356,7 @@
       <c r="G16" s="59" t="s">
         <v>585</v>
       </c>
-      <c r="H16" s="101"/>
+      <c r="H16" s="103"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="100"/>
@@ -8402,8 +8402,8 @@
     </row>
     <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
-      <c r="B19" s="101"/>
-      <c r="C19" s="101"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="59" t="s">
         <v>349</v>
       </c>
@@ -8416,7 +8416,7 @@
       <c r="G19" s="59" t="s">
         <v>544</v>
       </c>
-      <c r="H19" s="101"/>
+      <c r="H19" s="103"/>
     </row>
     <row r="20" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="100"/>
@@ -8476,7 +8476,7 @@
       <c r="G22" s="60" t="s">
         <v>368</v>
       </c>
-      <c r="H22" s="103"/>
+      <c r="H22" s="101"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="100"/>
@@ -8521,9 +8521,9 @@
       <c r="H24" s="100"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="103"/>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="101"/>
       <c r="D25" s="47" t="s">
         <v>349</v>
       </c>
@@ -8536,7 +8536,7 @@
       <c r="G25" s="47" t="s">
         <v>471</v>
       </c>
-      <c r="H25" s="103"/>
+      <c r="H25" s="101"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="102" t="s">
@@ -8624,8 +8624,8 @@
     </row>
     <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="100"/>
-      <c r="B31" s="101"/>
-      <c r="C31" s="101"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="59" t="s">
         <v>349</v>
       </c>
@@ -8638,7 +8638,7 @@
       <c r="G31" s="78" t="s">
         <v>525</v>
       </c>
-      <c r="H31" s="101"/>
+      <c r="H31" s="103"/>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="100"/>
@@ -8983,9 +8983,9 @@
       <c r="H48" s="100"/>
     </row>
     <row r="49" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="103"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="103"/>
+      <c r="A49" s="101"/>
+      <c r="B49" s="101"/>
+      <c r="C49" s="101"/>
       <c r="D49" s="47" t="s">
         <v>349</v>
       </c>
@@ -8998,22 +8998,35 @@
       <c r="G49" s="84" t="s">
         <v>509</v>
       </c>
-      <c r="H49" s="103"/>
+      <c r="H49" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A26:A49"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="H29:H31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="H35:H37"/>
     <mergeCell ref="A2:A25"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -9030,31 +9043,18 @@
     <mergeCell ref="H17:H19"/>
     <mergeCell ref="H5:H7"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A26:A49"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="H29:H31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="H35:H37"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="H44:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12337,10 +12337,10 @@
   <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19357,9 +19357,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0094531B-7BBB-4DD3-8835-99962592A6C6}">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>